<commit_message>
Atualização base de dados 1
</commit_message>
<xml_diff>
--- a/1 - Acompanhamento Medições.xlsx
+++ b/1 - Acompanhamento Medições.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://brpucrs-my.sharepoint.com/personal/raphael_leitao_edu_pucrs_br/Documents/Python/Aplicativo de Acompanhamento de Medições/Acomp-de-Medicoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="13_ncr:1_{A1421A19-0108-4133-B863-EAC0C5A9202F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C26CD04-14F0-4D41-831F-0E4B25E2F75E}"/>
+  <xr:revisionPtr revIDLastSave="222" documentId="13_ncr:1_{A1421A19-0108-4133-B863-EAC0C5A9202F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{513AFEB8-35B1-4F5C-A22F-D140AA6CCEDE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="604" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="604" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RESUMO-2024" sheetId="11" r:id="rId1"/>
@@ -5538,7 +5538,7 @@
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="352">
+  <cellXfs count="355">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6403,16 +6403,46 @@
     <xf numFmtId="44" fontId="118" fillId="85" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="84" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="83" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="85" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="113" fillId="6" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="113" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="73" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="86" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="86" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="118" fillId="85" borderId="72" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="73" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="111" fillId="86" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="118" fillId="85" borderId="80" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6442,36 +6472,6 @@
     <xf numFmtId="0" fontId="22" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="83" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="84" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="85" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="113" fillId="6" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="113" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="111" fillId="86" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="111" fillId="86" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="111" fillId="86" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="113" fillId="5" borderId="84" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6546,6 +6546,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="127" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="127" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1536">
@@ -9690,55 +9699,55 @@
       <c r="C1" s="158"/>
       <c r="D1" s="158"/>
       <c r="E1" s="158"/>
-      <c r="F1" s="322"/>
-      <c r="G1" s="322"/>
-      <c r="H1" s="322"/>
-      <c r="I1" s="322"/>
-      <c r="J1" s="322"/>
-      <c r="K1" s="322"/>
-      <c r="L1" s="322"/>
-      <c r="M1" s="322"/>
-      <c r="N1" s="322"/>
-      <c r="O1" s="322"/>
-      <c r="P1" s="323"/>
-      <c r="Q1" s="322"/>
-      <c r="R1" s="322"/>
-      <c r="S1" s="322"/>
-      <c r="T1" s="322"/>
-      <c r="U1" s="322"/>
-      <c r="V1" s="322"/>
-      <c r="W1" s="322"/>
-      <c r="X1" s="322"/>
-      <c r="Y1" s="322"/>
-      <c r="Z1" s="322"/>
-      <c r="AA1" s="322"/>
-      <c r="AB1" s="322"/>
-      <c r="AC1" s="322"/>
-      <c r="AD1" s="322"/>
-      <c r="AE1" s="322"/>
-      <c r="AF1" s="322"/>
-      <c r="AG1" s="322"/>
-      <c r="AH1" s="322"/>
-      <c r="AI1" s="322"/>
-      <c r="AJ1" s="322"/>
-      <c r="AK1" s="322"/>
-      <c r="AL1" s="322"/>
-      <c r="AM1" s="322"/>
-      <c r="AN1" s="322"/>
-      <c r="AO1" s="322"/>
-      <c r="AP1" s="322"/>
-      <c r="AQ1" s="322"/>
-      <c r="AR1" s="322"/>
-      <c r="AS1" s="322"/>
-      <c r="AT1" s="322"/>
-      <c r="AU1" s="322"/>
-      <c r="AV1" s="322"/>
-      <c r="AW1" s="322"/>
-      <c r="AX1" s="322"/>
-      <c r="AY1" s="322"/>
-      <c r="AZ1" s="322"/>
-      <c r="BA1" s="322"/>
-      <c r="BB1" s="322"/>
+      <c r="F1" s="316"/>
+      <c r="G1" s="316"/>
+      <c r="H1" s="316"/>
+      <c r="I1" s="316"/>
+      <c r="J1" s="316"/>
+      <c r="K1" s="316"/>
+      <c r="L1" s="316"/>
+      <c r="M1" s="316"/>
+      <c r="N1" s="316"/>
+      <c r="O1" s="316"/>
+      <c r="P1" s="317"/>
+      <c r="Q1" s="316"/>
+      <c r="R1" s="316"/>
+      <c r="S1" s="316"/>
+      <c r="T1" s="316"/>
+      <c r="U1" s="316"/>
+      <c r="V1" s="316"/>
+      <c r="W1" s="316"/>
+      <c r="X1" s="316"/>
+      <c r="Y1" s="316"/>
+      <c r="Z1" s="316"/>
+      <c r="AA1" s="316"/>
+      <c r="AB1" s="316"/>
+      <c r="AC1" s="316"/>
+      <c r="AD1" s="316"/>
+      <c r="AE1" s="316"/>
+      <c r="AF1" s="316"/>
+      <c r="AG1" s="316"/>
+      <c r="AH1" s="316"/>
+      <c r="AI1" s="316"/>
+      <c r="AJ1" s="316"/>
+      <c r="AK1" s="316"/>
+      <c r="AL1" s="316"/>
+      <c r="AM1" s="316"/>
+      <c r="AN1" s="316"/>
+      <c r="AO1" s="316"/>
+      <c r="AP1" s="316"/>
+      <c r="AQ1" s="316"/>
+      <c r="AR1" s="316"/>
+      <c r="AS1" s="316"/>
+      <c r="AT1" s="316"/>
+      <c r="AU1" s="316"/>
+      <c r="AV1" s="316"/>
+      <c r="AW1" s="316"/>
+      <c r="AX1" s="316"/>
+      <c r="AY1" s="316"/>
+      <c r="AZ1" s="316"/>
+      <c r="BA1" s="316"/>
+      <c r="BB1" s="316"/>
     </row>
     <row r="2" spans="1:54" ht="18.600000000000001">
       <c r="A2" s="152"/>
@@ -9777,103 +9786,103 @@
       <c r="AD3" s="203"/>
     </row>
     <row r="4" spans="1:54" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A4" s="309" t="s">
+      <c r="A4" s="319" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="311" t="s">
+      <c r="B4" s="321" t="s">
         <v>234</v>
       </c>
-      <c r="C4" s="315" t="s">
+      <c r="C4" s="325" t="s">
         <v>244</v>
       </c>
-      <c r="D4" s="311" t="s">
+      <c r="D4" s="321" t="s">
         <v>235</v>
       </c>
-      <c r="E4" s="313" t="s">
+      <c r="E4" s="323" t="s">
         <v>236</v>
       </c>
-      <c r="F4" s="325" t="s">
+      <c r="F4" s="315" t="s">
         <v>251</v>
       </c>
-      <c r="G4" s="324"/>
-      <c r="H4" s="324"/>
-      <c r="I4" s="326"/>
-      <c r="J4" s="324" t="s">
+      <c r="G4" s="312"/>
+      <c r="H4" s="312"/>
+      <c r="I4" s="313"/>
+      <c r="J4" s="312" t="s">
         <v>250</v>
       </c>
-      <c r="K4" s="324"/>
-      <c r="L4" s="324"/>
-      <c r="M4" s="324"/>
-      <c r="N4" s="325" t="s">
+      <c r="K4" s="312"/>
+      <c r="L4" s="312"/>
+      <c r="M4" s="312"/>
+      <c r="N4" s="315" t="s">
         <v>252</v>
       </c>
-      <c r="O4" s="324"/>
-      <c r="P4" s="324"/>
-      <c r="Q4" s="326"/>
-      <c r="R4" s="325" t="s">
+      <c r="O4" s="312"/>
+      <c r="P4" s="312"/>
+      <c r="Q4" s="313"/>
+      <c r="R4" s="315" t="s">
         <v>257</v>
       </c>
-      <c r="S4" s="324"/>
-      <c r="T4" s="324"/>
-      <c r="U4" s="326"/>
-      <c r="V4" s="324" t="s">
+      <c r="S4" s="312"/>
+      <c r="T4" s="312"/>
+      <c r="U4" s="313"/>
+      <c r="V4" s="312" t="s">
         <v>258</v>
       </c>
-      <c r="W4" s="324"/>
-      <c r="X4" s="324"/>
-      <c r="Y4" s="324"/>
-      <c r="Z4" s="325" t="s">
+      <c r="W4" s="312"/>
+      <c r="X4" s="312"/>
+      <c r="Y4" s="312"/>
+      <c r="Z4" s="315" t="s">
         <v>259</v>
       </c>
-      <c r="AA4" s="324"/>
-      <c r="AB4" s="324"/>
-      <c r="AC4" s="326"/>
-      <c r="AD4" s="325" t="s">
+      <c r="AA4" s="312"/>
+      <c r="AB4" s="312"/>
+      <c r="AC4" s="313"/>
+      <c r="AD4" s="315" t="s">
         <v>261</v>
       </c>
-      <c r="AE4" s="324"/>
-      <c r="AF4" s="324"/>
-      <c r="AG4" s="326"/>
-      <c r="AH4" s="325" t="s">
+      <c r="AE4" s="312"/>
+      <c r="AF4" s="312"/>
+      <c r="AG4" s="313"/>
+      <c r="AH4" s="315" t="s">
         <v>262</v>
       </c>
-      <c r="AI4" s="324"/>
-      <c r="AJ4" s="324"/>
-      <c r="AK4" s="326"/>
-      <c r="AL4" s="325" t="s">
+      <c r="AI4" s="312"/>
+      <c r="AJ4" s="312"/>
+      <c r="AK4" s="313"/>
+      <c r="AL4" s="315" t="s">
         <v>237</v>
       </c>
-      <c r="AM4" s="324"/>
-      <c r="AN4" s="324"/>
-      <c r="AO4" s="326"/>
-      <c r="AP4" s="324" t="s">
+      <c r="AM4" s="312"/>
+      <c r="AN4" s="312"/>
+      <c r="AO4" s="313"/>
+      <c r="AP4" s="312" t="s">
         <v>238</v>
       </c>
-      <c r="AQ4" s="324"/>
-      <c r="AR4" s="324"/>
-      <c r="AS4" s="326"/>
-      <c r="AT4" s="325" t="s">
+      <c r="AQ4" s="312"/>
+      <c r="AR4" s="312"/>
+      <c r="AS4" s="313"/>
+      <c r="AT4" s="315" t="s">
         <v>239</v>
       </c>
-      <c r="AU4" s="324"/>
-      <c r="AV4" s="324"/>
-      <c r="AW4" s="326"/>
-      <c r="AX4" s="325" t="s">
+      <c r="AU4" s="312"/>
+      <c r="AV4" s="312"/>
+      <c r="AW4" s="313"/>
+      <c r="AX4" s="315" t="s">
         <v>240</v>
       </c>
-      <c r="AY4" s="324"/>
-      <c r="AZ4" s="324"/>
-      <c r="BA4" s="326"/>
+      <c r="AY4" s="312"/>
+      <c r="AZ4" s="312"/>
+      <c r="BA4" s="313"/>
       <c r="BB4" s="222" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:54" s="146" customFormat="1" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A5" s="310"/>
-      <c r="B5" s="312"/>
-      <c r="C5" s="316"/>
-      <c r="D5" s="312"/>
-      <c r="E5" s="314"/>
+      <c r="A5" s="320"/>
+      <c r="B5" s="322"/>
+      <c r="C5" s="326"/>
+      <c r="D5" s="322"/>
+      <c r="E5" s="324"/>
       <c r="F5" s="173" t="s">
         <v>247</v>
       </c>
@@ -10111,54 +10120,54 @@
       <c r="AC6" s="219">
         <v>0</v>
       </c>
-      <c r="AD6" s="304" t="s">
+      <c r="AD6" s="314" t="s">
         <v>233</v>
       </c>
-      <c r="AE6" s="305"/>
-      <c r="AF6" s="305" t="s">
+      <c r="AE6" s="310"/>
+      <c r="AF6" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="AG6" s="306"/>
-      <c r="AH6" s="304" t="s">
+      <c r="AG6" s="311"/>
+      <c r="AH6" s="314" t="s">
         <v>233</v>
       </c>
-      <c r="AI6" s="305"/>
-      <c r="AJ6" s="305" t="s">
+      <c r="AI6" s="310"/>
+      <c r="AJ6" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="AK6" s="306"/>
-      <c r="AL6" s="304" t="s">
+      <c r="AK6" s="311"/>
+      <c r="AL6" s="314" t="s">
         <v>233</v>
       </c>
-      <c r="AM6" s="305"/>
-      <c r="AN6" s="305" t="s">
+      <c r="AM6" s="310"/>
+      <c r="AN6" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="AO6" s="306"/>
-      <c r="AP6" s="304" t="s">
+      <c r="AO6" s="311"/>
+      <c r="AP6" s="314" t="s">
         <v>233</v>
       </c>
-      <c r="AQ6" s="305"/>
-      <c r="AR6" s="305" t="s">
+      <c r="AQ6" s="310"/>
+      <c r="AR6" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="AS6" s="306"/>
-      <c r="AT6" s="304" t="s">
+      <c r="AS6" s="311"/>
+      <c r="AT6" s="314" t="s">
         <v>233</v>
       </c>
-      <c r="AU6" s="305"/>
-      <c r="AV6" s="305" t="s">
+      <c r="AU6" s="310"/>
+      <c r="AV6" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="AW6" s="306"/>
-      <c r="AX6" s="304" t="s">
+      <c r="AW6" s="311"/>
+      <c r="AX6" s="314" t="s">
         <v>233</v>
       </c>
-      <c r="AY6" s="305"/>
-      <c r="AZ6" s="305" t="s">
+      <c r="AY6" s="310"/>
+      <c r="AZ6" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="BA6" s="306"/>
+      <c r="BA6" s="311"/>
       <c r="BB6" s="266">
         <f>AY6+AU6+AQ6+AM6+AI6+AE6+AA6+W6+S6+O6+K6+G6</f>
         <v>1928583.53</v>
@@ -10728,36 +10737,36 @@
       <c r="AK10" s="211">
         <v>0</v>
       </c>
-      <c r="AL10" s="320" t="s">
+      <c r="AL10" s="308" t="s">
         <v>267</v>
       </c>
-      <c r="AM10" s="321"/>
+      <c r="AM10" s="309"/>
       <c r="AN10" s="185"/>
       <c r="AO10" s="210"/>
-      <c r="AP10" s="320" t="s">
+      <c r="AP10" s="308" t="s">
         <v>267</v>
       </c>
-      <c r="AQ10" s="321"/>
+      <c r="AQ10" s="309"/>
       <c r="AR10" s="181">
         <v>0</v>
       </c>
       <c r="AS10" s="213">
         <v>0</v>
       </c>
-      <c r="AT10" s="320" t="s">
+      <c r="AT10" s="308" t="s">
         <v>267</v>
       </c>
-      <c r="AU10" s="321"/>
+      <c r="AU10" s="309"/>
       <c r="AV10" s="181">
         <v>0</v>
       </c>
       <c r="AW10" s="211">
         <v>0</v>
       </c>
-      <c r="AX10" s="320" t="s">
+      <c r="AX10" s="308" t="s">
         <v>267</v>
       </c>
-      <c r="AY10" s="321"/>
+      <c r="AY10" s="309"/>
       <c r="AZ10" s="181">
         <v>0</v>
       </c>
@@ -11857,22 +11866,22 @@
       <c r="M18" s="206">
         <v>0</v>
       </c>
-      <c r="N18" s="307" t="s">
+      <c r="N18" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="O18" s="317"/>
-      <c r="P18" s="307" t="s">
+      <c r="O18" s="305"/>
+      <c r="P18" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="Q18" s="317"/>
-      <c r="R18" s="307" t="s">
+      <c r="Q18" s="305"/>
+      <c r="R18" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="S18" s="317"/>
-      <c r="T18" s="307" t="s">
+      <c r="S18" s="305"/>
+      <c r="T18" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="U18" s="308"/>
+      <c r="U18" s="318"/>
       <c r="V18" s="303" t="s">
         <v>233</v>
       </c>
@@ -11976,22 +11985,22 @@
         <v>233</v>
       </c>
       <c r="M19" s="301"/>
-      <c r="N19" s="307" t="s">
+      <c r="N19" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="O19" s="317"/>
-      <c r="P19" s="307" t="s">
+      <c r="O19" s="305"/>
+      <c r="P19" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="Q19" s="317"/>
-      <c r="R19" s="307" t="s">
+      <c r="Q19" s="305"/>
+      <c r="R19" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="S19" s="317"/>
-      <c r="T19" s="307" t="s">
+      <c r="S19" s="305"/>
+      <c r="T19" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="U19" s="308"/>
+      <c r="U19" s="318"/>
       <c r="V19" s="303" t="s">
         <v>233</v>
       </c>
@@ -12579,94 +12588,94 @@
       <c r="I23" s="216">
         <v>0</v>
       </c>
-      <c r="J23" s="318" t="s">
+      <c r="J23" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="K23" s="317"/>
-      <c r="L23" s="307" t="s">
+      <c r="K23" s="305"/>
+      <c r="L23" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="M23" s="319"/>
-      <c r="N23" s="318" t="s">
+      <c r="M23" s="307"/>
+      <c r="N23" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="O23" s="317"/>
-      <c r="P23" s="307" t="s">
+      <c r="O23" s="305"/>
+      <c r="P23" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="Q23" s="319"/>
-      <c r="R23" s="318" t="s">
+      <c r="Q23" s="307"/>
+      <c r="R23" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="S23" s="317"/>
-      <c r="T23" s="307" t="s">
+      <c r="S23" s="305"/>
+      <c r="T23" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="U23" s="319"/>
-      <c r="V23" s="318" t="s">
+      <c r="U23" s="307"/>
+      <c r="V23" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="W23" s="317"/>
-      <c r="X23" s="307" t="s">
+      <c r="W23" s="305"/>
+      <c r="X23" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="Y23" s="319"/>
-      <c r="Z23" s="318" t="s">
+      <c r="Y23" s="307"/>
+      <c r="Z23" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="AA23" s="317"/>
-      <c r="AB23" s="307" t="s">
+      <c r="AA23" s="305"/>
+      <c r="AB23" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="AC23" s="319"/>
-      <c r="AD23" s="318" t="s">
+      <c r="AC23" s="307"/>
+      <c r="AD23" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="AE23" s="317"/>
-      <c r="AF23" s="307" t="s">
+      <c r="AE23" s="305"/>
+      <c r="AF23" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="AG23" s="319"/>
-      <c r="AH23" s="318" t="s">
+      <c r="AG23" s="307"/>
+      <c r="AH23" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="AI23" s="317"/>
-      <c r="AJ23" s="307" t="s">
+      <c r="AI23" s="305"/>
+      <c r="AJ23" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="AK23" s="319"/>
-      <c r="AL23" s="318" t="s">
+      <c r="AK23" s="307"/>
+      <c r="AL23" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="AM23" s="317"/>
-      <c r="AN23" s="307" t="s">
+      <c r="AM23" s="305"/>
+      <c r="AN23" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="AO23" s="319"/>
-      <c r="AP23" s="318" t="s">
+      <c r="AO23" s="307"/>
+      <c r="AP23" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="AQ23" s="317"/>
-      <c r="AR23" s="307" t="s">
+      <c r="AQ23" s="305"/>
+      <c r="AR23" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="AS23" s="319"/>
-      <c r="AT23" s="318" t="s">
+      <c r="AS23" s="307"/>
+      <c r="AT23" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="AU23" s="317"/>
-      <c r="AV23" s="307" t="s">
+      <c r="AU23" s="305"/>
+      <c r="AV23" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="AW23" s="319"/>
-      <c r="AX23" s="318" t="s">
+      <c r="AW23" s="307"/>
+      <c r="AX23" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="AY23" s="317"/>
-      <c r="AZ23" s="307" t="s">
+      <c r="AY23" s="305"/>
+      <c r="AZ23" s="306" t="s">
         <v>233</v>
       </c>
-      <c r="BA23" s="319"/>
+      <c r="BA23" s="307"/>
       <c r="BB23" s="267">
         <f t="shared" si="0"/>
         <v>163670.23000000001</v>
@@ -14303,59 +14312,121 @@
     <sortCondition ref="A6:A16"/>
   </sortState>
   <mergeCells count="192">
-    <mergeCell ref="AN15:AO15"/>
-    <mergeCell ref="AP13:AQ13"/>
-    <mergeCell ref="AR13:AS13"/>
-    <mergeCell ref="AP14:AQ14"/>
-    <mergeCell ref="AR14:AS14"/>
-    <mergeCell ref="AP15:AQ15"/>
-    <mergeCell ref="AR15:AS15"/>
-    <mergeCell ref="AV14:AW14"/>
-    <mergeCell ref="AT15:AU15"/>
-    <mergeCell ref="AV15:AW15"/>
-    <mergeCell ref="AX13:AY13"/>
-    <mergeCell ref="AZ13:BA13"/>
-    <mergeCell ref="AX14:AY14"/>
-    <mergeCell ref="AZ14:BA14"/>
-    <mergeCell ref="AT18:AU18"/>
-    <mergeCell ref="AT19:AU19"/>
-    <mergeCell ref="AV18:AW18"/>
-    <mergeCell ref="AV19:AW19"/>
-    <mergeCell ref="AX18:AY18"/>
-    <mergeCell ref="AX19:AY19"/>
-    <mergeCell ref="AZ18:BA18"/>
-    <mergeCell ref="AZ19:BA19"/>
-    <mergeCell ref="AX15:AY15"/>
-    <mergeCell ref="AZ15:BA15"/>
-    <mergeCell ref="AT13:AU13"/>
-    <mergeCell ref="AV13:AW13"/>
-    <mergeCell ref="AT14:AU14"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="Z23:AA23"/>
-    <mergeCell ref="AT23:AU23"/>
-    <mergeCell ref="AV23:AW23"/>
-    <mergeCell ref="AZ30:BA30"/>
-    <mergeCell ref="AT25:AU25"/>
-    <mergeCell ref="AV25:AW25"/>
-    <mergeCell ref="AT26:AU26"/>
-    <mergeCell ref="AV26:AW26"/>
-    <mergeCell ref="AX25:AY25"/>
-    <mergeCell ref="AZ25:BA25"/>
-    <mergeCell ref="AX26:AY26"/>
-    <mergeCell ref="AZ26:BA26"/>
-    <mergeCell ref="AT29:AU29"/>
-    <mergeCell ref="AV29:AW29"/>
-    <mergeCell ref="AX29:AY29"/>
-    <mergeCell ref="AZ29:BA29"/>
-    <mergeCell ref="AX23:AY23"/>
-    <mergeCell ref="AZ23:BA23"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="AD18:AE18"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="AD7:AE7"/>
+    <mergeCell ref="AH15:AI15"/>
+    <mergeCell ref="AJ13:AK13"/>
+    <mergeCell ref="AJ14:AK14"/>
+    <mergeCell ref="AJ15:AK15"/>
+    <mergeCell ref="AJ19:AK19"/>
+    <mergeCell ref="AF6:AG6"/>
+    <mergeCell ref="AF7:AG7"/>
+    <mergeCell ref="AH6:AI6"/>
+    <mergeCell ref="AH7:AI7"/>
+    <mergeCell ref="AH14:AI14"/>
+    <mergeCell ref="AJ6:AK6"/>
+    <mergeCell ref="AH13:AI13"/>
+    <mergeCell ref="AH18:AI18"/>
+    <mergeCell ref="T19:U19"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="X19:Y19"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="X18:Y18"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AL25:AM25"/>
+    <mergeCell ref="AL26:AM26"/>
+    <mergeCell ref="AP25:AQ25"/>
+    <mergeCell ref="AP26:AQ26"/>
+    <mergeCell ref="AD19:AE19"/>
+    <mergeCell ref="AH23:AI23"/>
+    <mergeCell ref="AH19:AI19"/>
+    <mergeCell ref="AJ23:AK23"/>
+    <mergeCell ref="AD25:AE25"/>
+    <mergeCell ref="AF25:AG25"/>
+    <mergeCell ref="AH25:AI25"/>
+    <mergeCell ref="AH26:AI26"/>
+    <mergeCell ref="AJ25:AK25"/>
+    <mergeCell ref="AJ26:AK26"/>
+    <mergeCell ref="AD23:AE23"/>
+    <mergeCell ref="AF19:AG19"/>
+    <mergeCell ref="AL6:AM6"/>
+    <mergeCell ref="AL7:AM7"/>
+    <mergeCell ref="AN6:AO6"/>
+    <mergeCell ref="AN7:AO7"/>
+    <mergeCell ref="AF23:AG23"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AD15:AE15"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AJ7:AK7"/>
+    <mergeCell ref="AJ18:AK18"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="AD14:AE14"/>
+    <mergeCell ref="AL10:AM10"/>
+    <mergeCell ref="AB23:AC23"/>
+    <mergeCell ref="AF13:AG13"/>
+    <mergeCell ref="AF14:AG14"/>
+    <mergeCell ref="AF15:AG15"/>
+    <mergeCell ref="AF18:AG18"/>
+    <mergeCell ref="AN13:AO13"/>
+    <mergeCell ref="AL14:AM14"/>
+    <mergeCell ref="AN14:AO14"/>
+    <mergeCell ref="AL15:AM15"/>
+    <mergeCell ref="F1:BB1"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="Z4:AC4"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="AH4:AK4"/>
+    <mergeCell ref="AL4:AO4"/>
+    <mergeCell ref="AP10:AQ10"/>
+    <mergeCell ref="AP9:AQ9"/>
+    <mergeCell ref="AR9:AS9"/>
+    <mergeCell ref="AR25:AS25"/>
+    <mergeCell ref="AN25:AO25"/>
+    <mergeCell ref="AP30:AQ30"/>
+    <mergeCell ref="AR30:AS30"/>
+    <mergeCell ref="AR26:AS26"/>
+    <mergeCell ref="AL9:AM9"/>
+    <mergeCell ref="AN9:AO9"/>
+    <mergeCell ref="AN26:AO26"/>
+    <mergeCell ref="AL18:AM18"/>
+    <mergeCell ref="AL19:AM19"/>
+    <mergeCell ref="AN18:AO18"/>
+    <mergeCell ref="AN19:AO19"/>
+    <mergeCell ref="AP18:AQ18"/>
+    <mergeCell ref="AP19:AQ19"/>
+    <mergeCell ref="AR18:AS18"/>
+    <mergeCell ref="AR19:AS19"/>
+    <mergeCell ref="AL23:AM23"/>
+    <mergeCell ref="AN23:AO23"/>
+    <mergeCell ref="AP23:AQ23"/>
+    <mergeCell ref="AR23:AS23"/>
+    <mergeCell ref="AL13:AM13"/>
     <mergeCell ref="AT10:AU10"/>
     <mergeCell ref="AX10:AY10"/>
     <mergeCell ref="AP7:AQ7"/>
@@ -14380,121 +14451,59 @@
     <mergeCell ref="AZ7:BA7"/>
     <mergeCell ref="AX9:AY9"/>
     <mergeCell ref="AZ9:BA9"/>
-    <mergeCell ref="AP10:AQ10"/>
-    <mergeCell ref="AP9:AQ9"/>
-    <mergeCell ref="AR9:AS9"/>
-    <mergeCell ref="AR25:AS25"/>
-    <mergeCell ref="AN25:AO25"/>
-    <mergeCell ref="AP30:AQ30"/>
-    <mergeCell ref="AR30:AS30"/>
-    <mergeCell ref="AR26:AS26"/>
-    <mergeCell ref="AL9:AM9"/>
-    <mergeCell ref="AN9:AO9"/>
-    <mergeCell ref="AN26:AO26"/>
-    <mergeCell ref="AL18:AM18"/>
-    <mergeCell ref="AL19:AM19"/>
-    <mergeCell ref="AN18:AO18"/>
-    <mergeCell ref="AN19:AO19"/>
-    <mergeCell ref="AP18:AQ18"/>
-    <mergeCell ref="AP19:AQ19"/>
-    <mergeCell ref="AR18:AS18"/>
-    <mergeCell ref="AR19:AS19"/>
-    <mergeCell ref="AL23:AM23"/>
-    <mergeCell ref="AN23:AO23"/>
-    <mergeCell ref="AP23:AQ23"/>
-    <mergeCell ref="AR23:AS23"/>
-    <mergeCell ref="AL13:AM13"/>
-    <mergeCell ref="F1:BB1"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="Z4:AC4"/>
-    <mergeCell ref="V4:Y4"/>
-    <mergeCell ref="AD4:AG4"/>
-    <mergeCell ref="AH4:AK4"/>
-    <mergeCell ref="AL4:AO4"/>
-    <mergeCell ref="AL6:AM6"/>
-    <mergeCell ref="AL7:AM7"/>
-    <mergeCell ref="AN6:AO6"/>
-    <mergeCell ref="AN7:AO7"/>
-    <mergeCell ref="AF23:AG23"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AD15:AE15"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AJ7:AK7"/>
-    <mergeCell ref="AJ18:AK18"/>
-    <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="AD14:AE14"/>
-    <mergeCell ref="AL10:AM10"/>
-    <mergeCell ref="AB23:AC23"/>
-    <mergeCell ref="AF13:AG13"/>
-    <mergeCell ref="AF14:AG14"/>
-    <mergeCell ref="AF15:AG15"/>
-    <mergeCell ref="AF18:AG18"/>
-    <mergeCell ref="AN13:AO13"/>
-    <mergeCell ref="AL14:AM14"/>
-    <mergeCell ref="AN14:AO14"/>
-    <mergeCell ref="AL15:AM15"/>
-    <mergeCell ref="AL25:AM25"/>
-    <mergeCell ref="AL26:AM26"/>
-    <mergeCell ref="AP25:AQ25"/>
-    <mergeCell ref="AP26:AQ26"/>
-    <mergeCell ref="AD19:AE19"/>
-    <mergeCell ref="AH23:AI23"/>
-    <mergeCell ref="AH19:AI19"/>
-    <mergeCell ref="AJ23:AK23"/>
-    <mergeCell ref="AD25:AE25"/>
-    <mergeCell ref="AF25:AG25"/>
-    <mergeCell ref="AH25:AI25"/>
-    <mergeCell ref="AH26:AI26"/>
-    <mergeCell ref="AJ25:AK25"/>
-    <mergeCell ref="AJ26:AK26"/>
-    <mergeCell ref="AD23:AE23"/>
-    <mergeCell ref="AF19:AG19"/>
-    <mergeCell ref="T19:U19"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="X19:Y19"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="X18:Y18"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="AD18:AE18"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="AD7:AE7"/>
-    <mergeCell ref="AH15:AI15"/>
-    <mergeCell ref="AJ13:AK13"/>
-    <mergeCell ref="AJ14:AK14"/>
-    <mergeCell ref="AJ15:AK15"/>
-    <mergeCell ref="AJ19:AK19"/>
-    <mergeCell ref="AF6:AG6"/>
-    <mergeCell ref="AF7:AG7"/>
-    <mergeCell ref="AH6:AI6"/>
-    <mergeCell ref="AH7:AI7"/>
-    <mergeCell ref="AH14:AI14"/>
-    <mergeCell ref="AJ6:AK6"/>
-    <mergeCell ref="AH13:AI13"/>
-    <mergeCell ref="AH18:AI18"/>
+    <mergeCell ref="AT23:AU23"/>
+    <mergeCell ref="AV23:AW23"/>
+    <mergeCell ref="AZ30:BA30"/>
+    <mergeCell ref="AT25:AU25"/>
+    <mergeCell ref="AV25:AW25"/>
+    <mergeCell ref="AT26:AU26"/>
+    <mergeCell ref="AV26:AW26"/>
+    <mergeCell ref="AX25:AY25"/>
+    <mergeCell ref="AZ25:BA25"/>
+    <mergeCell ref="AX26:AY26"/>
+    <mergeCell ref="AZ26:BA26"/>
+    <mergeCell ref="AT29:AU29"/>
+    <mergeCell ref="AV29:AW29"/>
+    <mergeCell ref="AX29:AY29"/>
+    <mergeCell ref="AZ29:BA29"/>
+    <mergeCell ref="AX23:AY23"/>
+    <mergeCell ref="AZ23:BA23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="AX13:AY13"/>
+    <mergeCell ref="AZ13:BA13"/>
+    <mergeCell ref="AX14:AY14"/>
+    <mergeCell ref="AZ14:BA14"/>
+    <mergeCell ref="AT18:AU18"/>
+    <mergeCell ref="AT19:AU19"/>
+    <mergeCell ref="AV18:AW18"/>
+    <mergeCell ref="AV19:AW19"/>
+    <mergeCell ref="AX18:AY18"/>
+    <mergeCell ref="AX19:AY19"/>
+    <mergeCell ref="AZ18:BA18"/>
+    <mergeCell ref="AZ19:BA19"/>
+    <mergeCell ref="AX15:AY15"/>
+    <mergeCell ref="AZ15:BA15"/>
+    <mergeCell ref="AT13:AU13"/>
+    <mergeCell ref="AV13:AW13"/>
+    <mergeCell ref="AT14:AU14"/>
+    <mergeCell ref="AN15:AO15"/>
+    <mergeCell ref="AP13:AQ13"/>
+    <mergeCell ref="AR13:AS13"/>
+    <mergeCell ref="AP14:AQ14"/>
+    <mergeCell ref="AR14:AS14"/>
+    <mergeCell ref="AP15:AQ15"/>
+    <mergeCell ref="AR15:AS15"/>
+    <mergeCell ref="AV14:AW14"/>
+    <mergeCell ref="AT15:AU15"/>
+    <mergeCell ref="AV15:AW15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -16444,17 +16453,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C49:G49"/>
     <mergeCell ref="C50:G50"/>
     <mergeCell ref="C52:G52"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="C21:G21"/>
     <mergeCell ref="C23:G23"/>
     <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="C49:G49"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -18037,93 +18046,93 @@
       <c r="AD3" s="203"/>
     </row>
     <row r="4" spans="1:56 16377:16378" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A4" s="309" t="s">
+      <c r="A4" s="319" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="311" t="s">
+      <c r="B4" s="321" t="s">
         <v>234</v>
       </c>
-      <c r="C4" s="311" t="s">
+      <c r="C4" s="321" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="313" t="s">
+      <c r="D4" s="323" t="s">
         <v>236</v>
       </c>
-      <c r="E4" s="311" t="s">
+      <c r="E4" s="321" t="s">
         <v>311</v>
       </c>
-      <c r="F4" s="325" t="s">
+      <c r="F4" s="315" t="s">
         <v>251</v>
       </c>
-      <c r="G4" s="324"/>
-      <c r="H4" s="324"/>
-      <c r="I4" s="326"/>
-      <c r="J4" s="324" t="s">
+      <c r="G4" s="312"/>
+      <c r="H4" s="312"/>
+      <c r="I4" s="313"/>
+      <c r="J4" s="312" t="s">
         <v>250</v>
       </c>
-      <c r="K4" s="324"/>
-      <c r="L4" s="324"/>
-      <c r="M4" s="324"/>
-      <c r="N4" s="325" t="s">
+      <c r="K4" s="312"/>
+      <c r="L4" s="312"/>
+      <c r="M4" s="312"/>
+      <c r="N4" s="315" t="s">
         <v>252</v>
       </c>
-      <c r="O4" s="324"/>
-      <c r="P4" s="324"/>
-      <c r="Q4" s="326"/>
-      <c r="R4" s="325" t="s">
+      <c r="O4" s="312"/>
+      <c r="P4" s="312"/>
+      <c r="Q4" s="313"/>
+      <c r="R4" s="315" t="s">
         <v>257</v>
       </c>
-      <c r="S4" s="324"/>
-      <c r="T4" s="324"/>
-      <c r="U4" s="326"/>
-      <c r="V4" s="324" t="s">
+      <c r="S4" s="312"/>
+      <c r="T4" s="312"/>
+      <c r="U4" s="313"/>
+      <c r="V4" s="312" t="s">
         <v>258</v>
       </c>
-      <c r="W4" s="324"/>
-      <c r="X4" s="324"/>
-      <c r="Y4" s="324"/>
-      <c r="Z4" s="325" t="s">
+      <c r="W4" s="312"/>
+      <c r="X4" s="312"/>
+      <c r="Y4" s="312"/>
+      <c r="Z4" s="315" t="s">
         <v>259</v>
       </c>
-      <c r="AA4" s="324"/>
-      <c r="AB4" s="324"/>
-      <c r="AC4" s="326"/>
-      <c r="AD4" s="325" t="s">
+      <c r="AA4" s="312"/>
+      <c r="AB4" s="312"/>
+      <c r="AC4" s="313"/>
+      <c r="AD4" s="315" t="s">
         <v>261</v>
       </c>
-      <c r="AE4" s="324"/>
-      <c r="AF4" s="324"/>
-      <c r="AG4" s="326"/>
-      <c r="AH4" s="325" t="s">
+      <c r="AE4" s="312"/>
+      <c r="AF4" s="312"/>
+      <c r="AG4" s="313"/>
+      <c r="AH4" s="315" t="s">
         <v>262</v>
       </c>
-      <c r="AI4" s="324"/>
-      <c r="AJ4" s="324"/>
-      <c r="AK4" s="326"/>
-      <c r="AL4" s="325" t="s">
+      <c r="AI4" s="312"/>
+      <c r="AJ4" s="312"/>
+      <c r="AK4" s="313"/>
+      <c r="AL4" s="315" t="s">
         <v>237</v>
       </c>
-      <c r="AM4" s="324"/>
-      <c r="AN4" s="324"/>
-      <c r="AO4" s="326"/>
-      <c r="AP4" s="324" t="s">
+      <c r="AM4" s="312"/>
+      <c r="AN4" s="312"/>
+      <c r="AO4" s="313"/>
+      <c r="AP4" s="312" t="s">
         <v>238</v>
       </c>
-      <c r="AQ4" s="324"/>
-      <c r="AR4" s="324"/>
-      <c r="AS4" s="326"/>
-      <c r="AT4" s="325" t="s">
+      <c r="AQ4" s="312"/>
+      <c r="AR4" s="312"/>
+      <c r="AS4" s="313"/>
+      <c r="AT4" s="315" t="s">
         <v>239</v>
       </c>
-      <c r="AU4" s="324"/>
-      <c r="AV4" s="324"/>
-      <c r="AW4" s="326"/>
-      <c r="AX4" s="325" t="s">
+      <c r="AU4" s="312"/>
+      <c r="AV4" s="312"/>
+      <c r="AW4" s="313"/>
+      <c r="AX4" s="315" t="s">
         <v>240</v>
       </c>
-      <c r="AY4" s="324"/>
-      <c r="AZ4" s="324"/>
-      <c r="BA4" s="326"/>
+      <c r="AY4" s="312"/>
+      <c r="AZ4" s="312"/>
+      <c r="BA4" s="313"/>
       <c r="BB4" s="222" t="s">
         <v>308</v>
       </c>
@@ -18135,11 +18144,11 @@
       </c>
     </row>
     <row r="5" spans="1:56 16377:16378" s="146" customFormat="1" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A5" s="310"/>
-      <c r="B5" s="312"/>
-      <c r="C5" s="312"/>
-      <c r="D5" s="314"/>
-      <c r="E5" s="312"/>
+      <c r="A5" s="320"/>
+      <c r="B5" s="322"/>
+      <c r="C5" s="322"/>
+      <c r="D5" s="324"/>
+      <c r="E5" s="322"/>
       <c r="F5" s="173" t="s">
         <v>247</v>
       </c>
@@ -20761,15 +20770,11 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="AD4:AG4"/>
-    <mergeCell ref="AT4:AW4"/>
-    <mergeCell ref="AX4:BA4"/>
-    <mergeCell ref="V4:Y4"/>
-    <mergeCell ref="Z4:AC4"/>
-    <mergeCell ref="AL4:AO4"/>
-    <mergeCell ref="AP4:AS4"/>
-    <mergeCell ref="AH4:AK4"/>
+    <mergeCell ref="AX9:BA9"/>
+    <mergeCell ref="AH9:AK9"/>
+    <mergeCell ref="AL9:AO9"/>
+    <mergeCell ref="AP9:AS9"/>
+    <mergeCell ref="AT9:AW9"/>
     <mergeCell ref="J9:M9"/>
     <mergeCell ref="N9:Q9"/>
     <mergeCell ref="A4:A5"/>
@@ -20780,11 +20785,15 @@
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="AX9:BA9"/>
-    <mergeCell ref="AH9:AK9"/>
-    <mergeCell ref="AL9:AO9"/>
-    <mergeCell ref="AP9:AS9"/>
-    <mergeCell ref="AT9:AW9"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="AT4:AW4"/>
+    <mergeCell ref="AX4:BA4"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="Z4:AC4"/>
+    <mergeCell ref="AL4:AO4"/>
+    <mergeCell ref="AP4:AS4"/>
+    <mergeCell ref="AH4:AK4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -20802,8 +20811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C60C3C0C-3E40-486A-9B59-1C5056167637}">
   <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -22063,8 +22072,8 @@
       <c r="A55" s="293">
         <v>225</v>
       </c>
-      <c r="B55" s="293" t="s">
-        <v>302</v>
+      <c r="B55" s="352" t="s">
+        <v>314</v>
       </c>
       <c r="C55" s="293" t="s">
         <v>219</v>
@@ -22446,8 +22455,8 @@
       <c r="A72" s="293">
         <v>225</v>
       </c>
-      <c r="B72" s="293" t="s">
-        <v>302</v>
+      <c r="B72" s="352" t="s">
+        <v>314</v>
       </c>
       <c r="C72" s="293" t="s">
         <v>219</v>
@@ -22489,393 +22498,393 @@
       </c>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="293">
+      <c r="A74" s="352">
         <v>106</v>
       </c>
-      <c r="B74" s="293" t="s">
+      <c r="B74" s="352" t="s">
         <v>210</v>
       </c>
-      <c r="C74" s="293" t="s">
+      <c r="C74" s="352" t="s">
         <v>214</v>
       </c>
-      <c r="D74" s="293" t="s">
+      <c r="D74" s="352" t="s">
         <v>202</v>
       </c>
-      <c r="E74" s="296">
+      <c r="E74" s="353">
         <v>45809</v>
       </c>
-      <c r="F74" s="295">
+      <c r="F74" s="354">
         <v>440000</v>
       </c>
-      <c r="G74" s="295">
+      <c r="G74" s="354">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="293">
+      <c r="A75" s="352">
         <v>154</v>
       </c>
-      <c r="B75" s="293" t="s">
+      <c r="B75" s="352" t="s">
         <v>206</v>
       </c>
-      <c r="C75" s="293" t="s">
+      <c r="C75" s="352" t="s">
         <v>219</v>
       </c>
-      <c r="D75" s="293" t="s">
+      <c r="D75" s="352" t="s">
         <v>307</v>
       </c>
-      <c r="E75" s="296">
+      <c r="E75" s="353">
         <v>45809</v>
       </c>
-      <c r="F75" s="295">
+      <c r="F75" s="354">
         <v>130000</v>
       </c>
-      <c r="G75" s="295">
+      <c r="G75" s="354">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="293">
+      <c r="A76" s="352">
         <v>159</v>
       </c>
-      <c r="B76" s="293" t="s">
+      <c r="B76" s="352" t="s">
         <v>310</v>
       </c>
-      <c r="C76" s="293" t="s">
+      <c r="C76" s="352" t="s">
         <v>215</v>
       </c>
-      <c r="D76" s="293" t="s">
+      <c r="D76" s="352" t="s">
         <v>204</v>
       </c>
-      <c r="E76" s="296">
+      <c r="E76" s="353">
         <v>45809</v>
       </c>
-      <c r="F76" s="295">
+      <c r="F76" s="354">
         <v>12000</v>
       </c>
-      <c r="G76" s="295">
+      <c r="G76" s="354">
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="293">
+      <c r="A77" s="352">
         <v>174</v>
       </c>
-      <c r="B77" s="293" t="s">
+      <c r="B77" s="352" t="s">
         <v>226</v>
       </c>
-      <c r="C77" s="293" t="s">
+      <c r="C77" s="352" t="s">
         <v>222</v>
       </c>
-      <c r="D77" s="293" t="s">
+      <c r="D77" s="352" t="s">
         <v>307</v>
       </c>
-      <c r="E77" s="296">
+      <c r="E77" s="353">
         <v>45809</v>
       </c>
-      <c r="F77" s="295">
+      <c r="F77" s="354">
         <v>200000</v>
       </c>
-      <c r="G77" s="295">
+      <c r="G77" s="354">
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="293">
+      <c r="A78" s="352">
         <v>175</v>
       </c>
-      <c r="B78" s="293" t="s">
+      <c r="B78" s="352" t="s">
         <v>224</v>
       </c>
-      <c r="C78" s="293" t="s">
+      <c r="C78" s="352" t="s">
         <v>217</v>
       </c>
-      <c r="D78" s="293" t="s">
+      <c r="D78" s="352" t="s">
         <v>225</v>
       </c>
-      <c r="E78" s="296">
+      <c r="E78" s="353">
         <v>45809</v>
       </c>
-      <c r="F78" s="295">
+      <c r="F78" s="354">
         <v>175000</v>
       </c>
-      <c r="G78" s="295">
-        <v>0</v>
+      <c r="G78" s="354">
+        <v>166911.03</v>
       </c>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="293">
+      <c r="A79" s="352">
         <v>183</v>
       </c>
-      <c r="B79" s="293" t="s">
+      <c r="B79" s="352" t="s">
         <v>232</v>
       </c>
-      <c r="C79" s="293" t="s">
+      <c r="C79" s="352" t="s">
         <v>217</v>
       </c>
-      <c r="D79" s="293" t="s">
+      <c r="D79" s="352" t="s">
         <v>225</v>
       </c>
-      <c r="E79" s="296">
+      <c r="E79" s="353">
         <v>45809</v>
       </c>
-      <c r="F79" s="295">
+      <c r="F79" s="354">
         <v>120000</v>
       </c>
-      <c r="G79" s="295">
+      <c r="G79" s="354">
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="293">
+      <c r="A80" s="352">
         <v>184</v>
       </c>
-      <c r="B80" s="293" t="s">
+      <c r="B80" s="352" t="s">
         <v>266</v>
       </c>
-      <c r="C80" s="293" t="s">
+      <c r="C80" s="352" t="s">
         <v>230</v>
       </c>
-      <c r="D80" s="293" t="s">
+      <c r="D80" s="352" t="s">
         <v>231</v>
       </c>
-      <c r="E80" s="296">
+      <c r="E80" s="353">
         <v>45809</v>
       </c>
-      <c r="F80" s="295">
+      <c r="F80" s="354">
         <v>250000</v>
       </c>
-      <c r="G80" s="295">
-        <v>0</v>
+      <c r="G80" s="354">
+        <v>286000</v>
       </c>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" s="293">
+      <c r="A81" s="352">
         <v>184</v>
       </c>
-      <c r="B81" s="293" t="s">
+      <c r="B81" s="352" t="s">
         <v>269</v>
       </c>
-      <c r="C81" s="293" t="s">
+      <c r="C81" s="352" t="s">
         <v>230</v>
       </c>
-      <c r="D81" s="293" t="s">
+      <c r="D81" s="352" t="s">
         <v>231</v>
       </c>
-      <c r="E81" s="296">
+      <c r="E81" s="353">
         <v>45809</v>
       </c>
-      <c r="F81" s="295">
+      <c r="F81" s="354">
         <v>150000</v>
       </c>
-      <c r="G81" s="295">
-        <v>0</v>
+      <c r="G81" s="354">
+        <v>124599.02</v>
       </c>
     </row>
     <row r="82" spans="1:7">
-      <c r="A82" s="293">
+      <c r="A82" s="352">
         <v>192</v>
       </c>
-      <c r="B82" s="293" t="s">
+      <c r="B82" s="352" t="s">
         <v>260</v>
       </c>
-      <c r="C82" s="293" t="s">
+      <c r="C82" s="352" t="s">
         <v>219</v>
       </c>
-      <c r="D82" s="293" t="s">
+      <c r="D82" s="352" t="s">
         <v>307</v>
       </c>
-      <c r="E82" s="296">
+      <c r="E82" s="353">
         <v>45809</v>
       </c>
-      <c r="F82" s="295">
+      <c r="F82" s="354">
         <v>50000</v>
       </c>
-      <c r="G82" s="295">
+      <c r="G82" s="354">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="293">
+      <c r="A83" s="352">
         <v>202</v>
       </c>
-      <c r="B83" s="293" t="s">
+      <c r="B83" s="352" t="s">
         <v>263</v>
       </c>
-      <c r="C83" s="293" t="s">
+      <c r="C83" s="352" t="s">
         <v>219</v>
       </c>
-      <c r="D83" s="293" t="s">
+      <c r="D83" s="352" t="s">
         <v>307</v>
       </c>
-      <c r="E83" s="296">
+      <c r="E83" s="353">
         <v>45809</v>
       </c>
-      <c r="F83" s="295">
+      <c r="F83" s="354">
         <v>25000</v>
       </c>
-      <c r="G83" s="295">
+      <c r="G83" s="354">
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="293">
+      <c r="A84" s="352">
         <v>208</v>
       </c>
-      <c r="B84" s="293" t="s">
+      <c r="B84" s="352" t="s">
         <v>284</v>
       </c>
-      <c r="C84" s="293" t="s">
+      <c r="C84" s="352" t="s">
         <v>215</v>
       </c>
-      <c r="D84" s="293" t="s">
+      <c r="D84" s="352" t="s">
         <v>231</v>
       </c>
-      <c r="E84" s="296">
+      <c r="E84" s="353">
         <v>45809</v>
       </c>
-      <c r="F84" s="295">
+      <c r="F84" s="354">
         <v>577754</v>
       </c>
-      <c r="G84" s="295">
+      <c r="G84" s="354">
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:7">
-      <c r="A85" s="293">
+      <c r="A85" s="352">
         <v>215</v>
       </c>
-      <c r="B85" s="293" t="s">
+      <c r="B85" s="352" t="s">
         <v>296</v>
       </c>
-      <c r="C85" s="293" t="s">
+      <c r="C85" s="352" t="s">
         <v>219</v>
       </c>
-      <c r="D85" s="293" t="s">
+      <c r="D85" s="352" t="s">
         <v>231</v>
       </c>
-      <c r="E85" s="296">
+      <c r="E85" s="353">
         <v>45809</v>
       </c>
-      <c r="F85" s="295">
+      <c r="F85" s="354">
         <v>5000</v>
       </c>
-      <c r="G85" s="295">
+      <c r="G85" s="354">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:7">
-      <c r="A86" s="293">
+      <c r="A86" s="352">
         <v>217</v>
       </c>
-      <c r="B86" s="293" t="s">
+      <c r="B86" s="352" t="s">
         <v>303</v>
       </c>
-      <c r="C86" s="293" t="s">
+      <c r="C86" s="352" t="s">
         <v>216</v>
       </c>
-      <c r="D86" s="293" t="s">
+      <c r="D86" s="352" t="s">
         <v>300</v>
       </c>
-      <c r="E86" s="296">
+      <c r="E86" s="353">
         <v>45809</v>
       </c>
-      <c r="F86" s="295">
-        <v>0</v>
-      </c>
-      <c r="G86" s="295">
+      <c r="F86" s="354">
+        <v>0</v>
+      </c>
+      <c r="G86" s="354">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:7">
-      <c r="A87" s="293">
+      <c r="A87" s="352">
         <v>218</v>
       </c>
-      <c r="B87" s="293" t="s">
+      <c r="B87" s="352" t="s">
         <v>298</v>
       </c>
-      <c r="C87" s="293" t="s">
+      <c r="C87" s="352" t="s">
         <v>299</v>
       </c>
-      <c r="D87" s="293" t="s">
+      <c r="D87" s="352" t="s">
         <v>301</v>
       </c>
-      <c r="E87" s="296">
+      <c r="E87" s="353">
         <v>45809</v>
       </c>
-      <c r="F87" s="295">
+      <c r="F87" s="354">
         <v>450000</v>
       </c>
-      <c r="G87" s="295">
-        <v>0</v>
+      <c r="G87" s="354">
+        <v>549344.87</v>
       </c>
     </row>
     <row r="88" spans="1:7">
-      <c r="A88" s="293">
+      <c r="A88" s="352">
         <v>220</v>
       </c>
-      <c r="B88" s="293" t="s">
+      <c r="B88" s="352" t="s">
         <v>306</v>
       </c>
-      <c r="C88" s="293" t="s">
+      <c r="C88" s="352" t="s">
         <v>222</v>
       </c>
-      <c r="D88" s="293" t="s">
+      <c r="D88" s="352" t="s">
         <v>307</v>
       </c>
-      <c r="E88" s="296">
+      <c r="E88" s="353">
         <v>45809</v>
       </c>
-      <c r="F88" s="295">
-        <v>0</v>
-      </c>
-      <c r="G88" s="295">
+      <c r="F88" s="354">
+        <v>0</v>
+      </c>
+      <c r="G88" s="354">
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:7">
-      <c r="A89" s="293">
+      <c r="A89" s="352">
         <v>225</v>
       </c>
-      <c r="B89" s="293" t="s">
-        <v>302</v>
-      </c>
-      <c r="C89" s="293" t="s">
+      <c r="B89" s="352" t="s">
+        <v>314</v>
+      </c>
+      <c r="C89" s="352" t="s">
         <v>219</v>
       </c>
-      <c r="D89" s="293" t="s">
+      <c r="D89" s="352" t="s">
         <v>307</v>
       </c>
-      <c r="E89" s="296">
+      <c r="E89" s="353">
         <v>45809</v>
       </c>
-      <c r="F89" s="295">
-        <v>106731.25</v>
-      </c>
-      <c r="G89" s="295">
-        <v>0</v>
+      <c r="F89" s="354">
+        <v>279614</v>
+      </c>
+      <c r="G89" s="354">
+        <v>223790.63</v>
       </c>
     </row>
     <row r="90" spans="1:7">
-      <c r="A90" s="293">
+      <c r="A90" s="352">
         <v>227</v>
       </c>
-      <c r="B90" s="293" t="s">
+      <c r="B90" s="352" t="s">
         <v>304</v>
       </c>
-      <c r="C90" s="293" t="s">
+      <c r="C90" s="352" t="s">
         <v>219</v>
       </c>
-      <c r="D90" s="293" t="s">
+      <c r="D90" s="352" t="s">
         <v>305</v>
       </c>
-      <c r="E90" s="296">
+      <c r="E90" s="353">
         <v>45809</v>
       </c>
-      <c r="F90" s="295">
+      <c r="F90" s="354">
         <v>80000</v>
       </c>
-      <c r="G90" s="295">
+      <c r="G90" s="354">
         <v>0</v>
       </c>
     </row>
@@ -22942,7 +22951,7 @@
         <v>45839</v>
       </c>
       <c r="F93" s="295">
-        <v>0</v>
+        <v>620000</v>
       </c>
       <c r="G93" s="295">
         <v>0</v>
@@ -22988,7 +22997,7 @@
         <v>45839</v>
       </c>
       <c r="F95" s="295">
-        <v>0</v>
+        <v>226000</v>
       </c>
       <c r="G95" s="295">
         <v>0</v>
@@ -23034,7 +23043,7 @@
         <v>45839</v>
       </c>
       <c r="F97" s="295">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="G97" s="295">
         <v>0</v>
@@ -23057,7 +23066,7 @@
         <v>45839</v>
       </c>
       <c r="F98" s="295">
-        <v>0</v>
+        <v>850000</v>
       </c>
       <c r="G98" s="295">
         <v>0</v>
@@ -23080,7 +23089,7 @@
         <v>45839</v>
       </c>
       <c r="F99" s="295">
-        <v>0</v>
+        <v>540000</v>
       </c>
       <c r="G99" s="295">
         <v>0</v>
@@ -23103,7 +23112,7 @@
         <v>45839</v>
       </c>
       <c r="F100" s="295">
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="G100" s="295">
         <v>0</v>
@@ -23126,7 +23135,7 @@
         <v>45839</v>
       </c>
       <c r="F101" s="295">
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="G101" s="295">
         <v>0</v>
@@ -23149,7 +23158,7 @@
         <v>45839</v>
       </c>
       <c r="F102" s="295">
-        <v>0</v>
+        <v>650000</v>
       </c>
       <c r="G102" s="295">
         <v>0</v>
@@ -23172,7 +23181,7 @@
         <v>45839</v>
       </c>
       <c r="F103" s="295">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="G103" s="295">
         <v>0</v>
@@ -23218,7 +23227,7 @@
         <v>45839</v>
       </c>
       <c r="F105" s="295">
-        <v>0</v>
+        <v>350000</v>
       </c>
       <c r="G105" s="295">
         <v>0</v>
@@ -23241,7 +23250,7 @@
         <v>45839</v>
       </c>
       <c r="F106" s="295">
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="G106" s="295">
         <v>0</v>
@@ -23251,8 +23260,8 @@
       <c r="A107" s="293">
         <v>225</v>
       </c>
-      <c r="B107" s="293" t="s">
-        <v>302</v>
+      <c r="B107" s="352" t="s">
+        <v>314</v>
       </c>
       <c r="C107" s="293" t="s">
         <v>219</v>
@@ -23305,7 +23314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF7C2BA-F766-47EF-8569-EB2756BF213B}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Atualização 07/08/25 - 2
</commit_message>
<xml_diff>
--- a/1 - Acompanhamento Medições.xlsx
+++ b/1 - Acompanhamento Medições.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://brpucrs-my.sharepoint.com/personal/raphael_leitao_edu_pucrs_br/Documents/Python/Aplicativo de Acompanhamento de Medições/Acomp-de-Medicoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="641" documentId="13_ncr:1_{A1421A19-0108-4133-B863-EAC0C5A9202F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5069A66-6713-48AB-B00E-8C0FFAFF0654}"/>
+  <xr:revisionPtr revIDLastSave="642" documentId="13_ncr:1_{A1421A19-0108-4133-B863-EAC0C5A9202F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{395A55F1-A280-4CEF-979A-59ED2FE107D0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="604" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="604" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RESUMO-2024" sheetId="11" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1945" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="315">
   <si>
     <t xml:space="preserve"> DNIT - Maranhão - CT Nº UT-15.00836.2020</t>
   </si>
@@ -6342,25 +6342,55 @@
     <xf numFmtId="44" fontId="127" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="75" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="118" fillId="85" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="84" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="83" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="85" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="113" fillId="6" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="113" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="73" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="86" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="86" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="118" fillId="85" borderId="72" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="73" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="111" fillId="86" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="75" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="118" fillId="85" borderId="80" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6382,36 +6412,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="7" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="83" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="84" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="85" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="113" fillId="6" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="113" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="111" fillId="86" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="111" fillId="86" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="111" fillId="86" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="113" fillId="5" borderId="84" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -9246,8 +9246,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C6985BB-829B-4487-B9C4-A57F3DBFCE52}" name="Tabela1" displayName="Tabela1" ref="A1:G289" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="A1:G289" xr:uid="{7C6985BB-829B-4487-B9C4-A57F3DBFCE52}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C6985BB-829B-4487-B9C4-A57F3DBFCE52}" name="Tabela1" displayName="Tabela1" ref="A1:G288" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="A1:G288" xr:uid="{7C6985BB-829B-4487-B9C4-A57F3DBFCE52}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E36FFB85-93AD-4CA4-8EE3-C83046716BD5}" name="CENTRO DE CUSTO" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{EE155F74-EE85-4003-8CC0-8828B59CB009}" name="OBRA" dataDxfId="12"/>
@@ -9630,55 +9630,55 @@
       </c>
       <c r="C1" s="157"/>
       <c r="D1" s="157"/>
-      <c r="E1" s="314"/>
-      <c r="F1" s="314"/>
-      <c r="G1" s="314"/>
-      <c r="H1" s="314"/>
-      <c r="I1" s="314"/>
-      <c r="J1" s="314"/>
-      <c r="K1" s="314"/>
-      <c r="L1" s="314"/>
-      <c r="M1" s="314"/>
-      <c r="N1" s="314"/>
-      <c r="O1" s="315"/>
-      <c r="P1" s="314"/>
-      <c r="Q1" s="314"/>
-      <c r="R1" s="314"/>
-      <c r="S1" s="314"/>
-      <c r="T1" s="314"/>
-      <c r="U1" s="314"/>
-      <c r="V1" s="314"/>
-      <c r="W1" s="314"/>
-      <c r="X1" s="314"/>
-      <c r="Y1" s="314"/>
-      <c r="Z1" s="314"/>
-      <c r="AA1" s="314"/>
-      <c r="AB1" s="314"/>
-      <c r="AC1" s="314"/>
-      <c r="AD1" s="314"/>
-      <c r="AE1" s="314"/>
-      <c r="AF1" s="314"/>
-      <c r="AG1" s="314"/>
-      <c r="AH1" s="314"/>
-      <c r="AI1" s="314"/>
-      <c r="AJ1" s="314"/>
-      <c r="AK1" s="314"/>
-      <c r="AL1" s="314"/>
-      <c r="AM1" s="314"/>
-      <c r="AN1" s="314"/>
-      <c r="AO1" s="314"/>
-      <c r="AP1" s="314"/>
-      <c r="AQ1" s="314"/>
-      <c r="AR1" s="314"/>
-      <c r="AS1" s="314"/>
-      <c r="AT1" s="314"/>
-      <c r="AU1" s="314"/>
-      <c r="AV1" s="314"/>
-      <c r="AW1" s="314"/>
-      <c r="AX1" s="314"/>
-      <c r="AY1" s="314"/>
-      <c r="AZ1" s="314"/>
-      <c r="BA1" s="314"/>
+      <c r="E1" s="310"/>
+      <c r="F1" s="310"/>
+      <c r="G1" s="310"/>
+      <c r="H1" s="310"/>
+      <c r="I1" s="310"/>
+      <c r="J1" s="310"/>
+      <c r="K1" s="310"/>
+      <c r="L1" s="310"/>
+      <c r="M1" s="310"/>
+      <c r="N1" s="310"/>
+      <c r="O1" s="311"/>
+      <c r="P1" s="310"/>
+      <c r="Q1" s="310"/>
+      <c r="R1" s="310"/>
+      <c r="S1" s="310"/>
+      <c r="T1" s="310"/>
+      <c r="U1" s="310"/>
+      <c r="V1" s="310"/>
+      <c r="W1" s="310"/>
+      <c r="X1" s="310"/>
+      <c r="Y1" s="310"/>
+      <c r="Z1" s="310"/>
+      <c r="AA1" s="310"/>
+      <c r="AB1" s="310"/>
+      <c r="AC1" s="310"/>
+      <c r="AD1" s="310"/>
+      <c r="AE1" s="310"/>
+      <c r="AF1" s="310"/>
+      <c r="AG1" s="310"/>
+      <c r="AH1" s="310"/>
+      <c r="AI1" s="310"/>
+      <c r="AJ1" s="310"/>
+      <c r="AK1" s="310"/>
+      <c r="AL1" s="310"/>
+      <c r="AM1" s="310"/>
+      <c r="AN1" s="310"/>
+      <c r="AO1" s="310"/>
+      <c r="AP1" s="310"/>
+      <c r="AQ1" s="310"/>
+      <c r="AR1" s="310"/>
+      <c r="AS1" s="310"/>
+      <c r="AT1" s="310"/>
+      <c r="AU1" s="310"/>
+      <c r="AV1" s="310"/>
+      <c r="AW1" s="310"/>
+      <c r="AX1" s="310"/>
+      <c r="AY1" s="310"/>
+      <c r="AZ1" s="310"/>
+      <c r="BA1" s="310"/>
     </row>
     <row r="2" spans="1:53" ht="18.600000000000001">
       <c r="A2" s="151"/>
@@ -9717,99 +9717,99 @@
       <c r="AC3" s="201"/>
     </row>
     <row r="4" spans="1:53" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A4" s="303" t="s">
+      <c r="A4" s="313" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="305" t="s">
+      <c r="B4" s="315" t="s">
         <v>234</v>
       </c>
-      <c r="C4" s="305" t="s">
+      <c r="C4" s="315" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="307" t="s">
+      <c r="D4" s="317" t="s">
         <v>236</v>
       </c>
-      <c r="E4" s="317" t="s">
+      <c r="E4" s="309" t="s">
         <v>250</v>
       </c>
-      <c r="F4" s="316"/>
-      <c r="G4" s="316"/>
-      <c r="H4" s="318"/>
-      <c r="I4" s="316" t="s">
+      <c r="F4" s="306"/>
+      <c r="G4" s="306"/>
+      <c r="H4" s="307"/>
+      <c r="I4" s="306" t="s">
         <v>249</v>
       </c>
-      <c r="J4" s="316"/>
-      <c r="K4" s="316"/>
-      <c r="L4" s="316"/>
-      <c r="M4" s="317" t="s">
+      <c r="J4" s="306"/>
+      <c r="K4" s="306"/>
+      <c r="L4" s="306"/>
+      <c r="M4" s="309" t="s">
         <v>251</v>
       </c>
-      <c r="N4" s="316"/>
-      <c r="O4" s="316"/>
-      <c r="P4" s="318"/>
-      <c r="Q4" s="317" t="s">
+      <c r="N4" s="306"/>
+      <c r="O4" s="306"/>
+      <c r="P4" s="307"/>
+      <c r="Q4" s="309" t="s">
         <v>256</v>
       </c>
-      <c r="R4" s="316"/>
-      <c r="S4" s="316"/>
-      <c r="T4" s="318"/>
-      <c r="U4" s="316" t="s">
+      <c r="R4" s="306"/>
+      <c r="S4" s="306"/>
+      <c r="T4" s="307"/>
+      <c r="U4" s="306" t="s">
         <v>257</v>
       </c>
-      <c r="V4" s="316"/>
-      <c r="W4" s="316"/>
-      <c r="X4" s="316"/>
-      <c r="Y4" s="317" t="s">
+      <c r="V4" s="306"/>
+      <c r="W4" s="306"/>
+      <c r="X4" s="306"/>
+      <c r="Y4" s="309" t="s">
         <v>258</v>
       </c>
-      <c r="Z4" s="316"/>
-      <c r="AA4" s="316"/>
-      <c r="AB4" s="318"/>
-      <c r="AC4" s="317" t="s">
+      <c r="Z4" s="306"/>
+      <c r="AA4" s="306"/>
+      <c r="AB4" s="307"/>
+      <c r="AC4" s="309" t="s">
         <v>260</v>
       </c>
-      <c r="AD4" s="316"/>
-      <c r="AE4" s="316"/>
-      <c r="AF4" s="318"/>
-      <c r="AG4" s="317" t="s">
+      <c r="AD4" s="306"/>
+      <c r="AE4" s="306"/>
+      <c r="AF4" s="307"/>
+      <c r="AG4" s="309" t="s">
         <v>261</v>
       </c>
-      <c r="AH4" s="316"/>
-      <c r="AI4" s="316"/>
-      <c r="AJ4" s="318"/>
-      <c r="AK4" s="317" t="s">
+      <c r="AH4" s="306"/>
+      <c r="AI4" s="306"/>
+      <c r="AJ4" s="307"/>
+      <c r="AK4" s="309" t="s">
         <v>237</v>
       </c>
-      <c r="AL4" s="316"/>
-      <c r="AM4" s="316"/>
-      <c r="AN4" s="318"/>
-      <c r="AO4" s="316" t="s">
+      <c r="AL4" s="306"/>
+      <c r="AM4" s="306"/>
+      <c r="AN4" s="307"/>
+      <c r="AO4" s="306" t="s">
         <v>238</v>
       </c>
-      <c r="AP4" s="316"/>
-      <c r="AQ4" s="316"/>
-      <c r="AR4" s="318"/>
-      <c r="AS4" s="317" t="s">
+      <c r="AP4" s="306"/>
+      <c r="AQ4" s="306"/>
+      <c r="AR4" s="307"/>
+      <c r="AS4" s="309" t="s">
         <v>239</v>
       </c>
-      <c r="AT4" s="316"/>
-      <c r="AU4" s="316"/>
-      <c r="AV4" s="318"/>
-      <c r="AW4" s="317" t="s">
+      <c r="AT4" s="306"/>
+      <c r="AU4" s="306"/>
+      <c r="AV4" s="307"/>
+      <c r="AW4" s="309" t="s">
         <v>240</v>
       </c>
-      <c r="AX4" s="316"/>
-      <c r="AY4" s="316"/>
-      <c r="AZ4" s="318"/>
+      <c r="AX4" s="306"/>
+      <c r="AY4" s="306"/>
+      <c r="AZ4" s="307"/>
       <c r="BA4" s="220" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:53" s="145" customFormat="1" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A5" s="304"/>
-      <c r="B5" s="306"/>
-      <c r="C5" s="306"/>
-      <c r="D5" s="308"/>
+      <c r="A5" s="314"/>
+      <c r="B5" s="316"/>
+      <c r="C5" s="316"/>
+      <c r="D5" s="318"/>
       <c r="E5" s="172" t="s">
         <v>246</v>
       </c>
@@ -10046,54 +10046,54 @@
       <c r="AB6" s="217">
         <v>0</v>
       </c>
-      <c r="AC6" s="297" t="s">
+      <c r="AC6" s="308" t="s">
         <v>233</v>
       </c>
-      <c r="AD6" s="298"/>
-      <c r="AE6" s="298" t="s">
+      <c r="AD6" s="304"/>
+      <c r="AE6" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="AF6" s="300"/>
-      <c r="AG6" s="297" t="s">
+      <c r="AF6" s="305"/>
+      <c r="AG6" s="308" t="s">
         <v>233</v>
       </c>
-      <c r="AH6" s="298"/>
-      <c r="AI6" s="298" t="s">
+      <c r="AH6" s="304"/>
+      <c r="AI6" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="AJ6" s="300"/>
-      <c r="AK6" s="297" t="s">
+      <c r="AJ6" s="305"/>
+      <c r="AK6" s="308" t="s">
         <v>233</v>
       </c>
-      <c r="AL6" s="298"/>
-      <c r="AM6" s="298" t="s">
+      <c r="AL6" s="304"/>
+      <c r="AM6" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="AN6" s="300"/>
-      <c r="AO6" s="297" t="s">
+      <c r="AN6" s="305"/>
+      <c r="AO6" s="308" t="s">
         <v>233</v>
       </c>
-      <c r="AP6" s="298"/>
-      <c r="AQ6" s="298" t="s">
+      <c r="AP6" s="304"/>
+      <c r="AQ6" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="AR6" s="300"/>
-      <c r="AS6" s="297" t="s">
+      <c r="AR6" s="305"/>
+      <c r="AS6" s="308" t="s">
         <v>233</v>
       </c>
-      <c r="AT6" s="298"/>
-      <c r="AU6" s="298" t="s">
+      <c r="AT6" s="304"/>
+      <c r="AU6" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="AV6" s="300"/>
-      <c r="AW6" s="297" t="s">
+      <c r="AV6" s="305"/>
+      <c r="AW6" s="308" t="s">
         <v>233</v>
       </c>
-      <c r="AX6" s="298"/>
-      <c r="AY6" s="298" t="s">
+      <c r="AX6" s="304"/>
+      <c r="AY6" s="304" t="s">
         <v>233</v>
       </c>
-      <c r="AZ6" s="300"/>
+      <c r="AZ6" s="305"/>
       <c r="BA6" s="256">
         <f>AX6+AT6+AP6+AL6+AH6+AD6+Z6+V6+R6+N6+J6+F6</f>
         <v>1928583.53</v>
@@ -10186,54 +10186,54 @@
       <c r="AB7" s="209">
         <v>0</v>
       </c>
-      <c r="AC7" s="295" t="s">
+      <c r="AC7" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AD7" s="296"/>
-      <c r="AE7" s="296" t="s">
+      <c r="AD7" s="295"/>
+      <c r="AE7" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AF7" s="299"/>
-      <c r="AG7" s="295" t="s">
+      <c r="AF7" s="296"/>
+      <c r="AG7" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AH7" s="296"/>
-      <c r="AI7" s="296" t="s">
+      <c r="AH7" s="295"/>
+      <c r="AI7" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AJ7" s="299"/>
-      <c r="AK7" s="295" t="s">
+      <c r="AJ7" s="296"/>
+      <c r="AK7" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AL7" s="296"/>
-      <c r="AM7" s="296" t="s">
+      <c r="AL7" s="295"/>
+      <c r="AM7" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AN7" s="299"/>
-      <c r="AO7" s="295" t="s">
+      <c r="AN7" s="296"/>
+      <c r="AO7" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AP7" s="296"/>
-      <c r="AQ7" s="296" t="s">
+      <c r="AP7" s="295"/>
+      <c r="AQ7" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AR7" s="299"/>
-      <c r="AS7" s="295" t="s">
+      <c r="AR7" s="296"/>
+      <c r="AS7" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AT7" s="296"/>
-      <c r="AU7" s="296" t="s">
+      <c r="AT7" s="295"/>
+      <c r="AU7" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AV7" s="299"/>
-      <c r="AW7" s="295" t="s">
+      <c r="AV7" s="296"/>
+      <c r="AW7" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AX7" s="296"/>
-      <c r="AY7" s="296" t="s">
+      <c r="AX7" s="295"/>
+      <c r="AY7" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AZ7" s="299"/>
+      <c r="AZ7" s="296"/>
       <c r="BA7" s="257">
         <f t="shared" ref="BA7:BA31" si="0">AX7+AT7+AP7+AL7+AH7+AD7+Z7+V7+R7+N7+J7+F7</f>
         <v>1513239.29</v>
@@ -10514,38 +10514,38 @@
       <c r="AJ9" s="209">
         <v>0</v>
       </c>
-      <c r="AK9" s="295" t="s">
+      <c r="AK9" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AL9" s="296"/>
-      <c r="AM9" s="296" t="s">
+      <c r="AL9" s="295"/>
+      <c r="AM9" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AN9" s="299"/>
-      <c r="AO9" s="295" t="s">
+      <c r="AN9" s="296"/>
+      <c r="AO9" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AP9" s="296"/>
-      <c r="AQ9" s="296" t="s">
+      <c r="AP9" s="295"/>
+      <c r="AQ9" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AR9" s="299"/>
-      <c r="AS9" s="295" t="s">
+      <c r="AR9" s="296"/>
+      <c r="AS9" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AT9" s="296"/>
-      <c r="AU9" s="296" t="s">
+      <c r="AT9" s="295"/>
+      <c r="AU9" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AV9" s="299"/>
-      <c r="AW9" s="295" t="s">
+      <c r="AV9" s="296"/>
+      <c r="AW9" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AX9" s="296"/>
-      <c r="AY9" s="296" t="s">
+      <c r="AX9" s="295"/>
+      <c r="AY9" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AZ9" s="299"/>
+      <c r="AZ9" s="296"/>
       <c r="BA9" s="257">
         <f t="shared" si="0"/>
         <v>137879.14000000001</v>
@@ -10659,36 +10659,36 @@
       <c r="AJ10" s="209">
         <v>0</v>
       </c>
-      <c r="AK10" s="312" t="s">
+      <c r="AK10" s="302" t="s">
         <v>266</v>
       </c>
-      <c r="AL10" s="313"/>
+      <c r="AL10" s="303"/>
       <c r="AM10" s="184"/>
       <c r="AN10" s="208"/>
-      <c r="AO10" s="312" t="s">
+      <c r="AO10" s="302" t="s">
         <v>266</v>
       </c>
-      <c r="AP10" s="313"/>
+      <c r="AP10" s="303"/>
       <c r="AQ10" s="180">
         <v>0</v>
       </c>
       <c r="AR10" s="211">
         <v>0</v>
       </c>
-      <c r="AS10" s="312" t="s">
+      <c r="AS10" s="302" t="s">
         <v>266</v>
       </c>
-      <c r="AT10" s="313"/>
+      <c r="AT10" s="303"/>
       <c r="AU10" s="180">
         <v>0</v>
       </c>
       <c r="AV10" s="209">
         <v>0</v>
       </c>
-      <c r="AW10" s="312" t="s">
+      <c r="AW10" s="302" t="s">
         <v>266</v>
       </c>
-      <c r="AX10" s="313"/>
+      <c r="AX10" s="303"/>
       <c r="AY10" s="180">
         <v>0</v>
       </c>
@@ -11095,62 +11095,62 @@
       <c r="X13" s="209">
         <v>0</v>
       </c>
-      <c r="Y13" s="295" t="s">
+      <c r="Y13" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="Z13" s="296"/>
-      <c r="AA13" s="296" t="s">
+      <c r="Z13" s="295"/>
+      <c r="AA13" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AB13" s="299"/>
-      <c r="AC13" s="295" t="s">
+      <c r="AB13" s="296"/>
+      <c r="AC13" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AD13" s="296"/>
-      <c r="AE13" s="296" t="s">
+      <c r="AD13" s="295"/>
+      <c r="AE13" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AF13" s="299"/>
-      <c r="AG13" s="295" t="s">
+      <c r="AF13" s="296"/>
+      <c r="AG13" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AH13" s="296"/>
-      <c r="AI13" s="296" t="s">
+      <c r="AH13" s="295"/>
+      <c r="AI13" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AJ13" s="299"/>
-      <c r="AK13" s="295" t="s">
+      <c r="AJ13" s="296"/>
+      <c r="AK13" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AL13" s="296"/>
-      <c r="AM13" s="296" t="s">
+      <c r="AL13" s="295"/>
+      <c r="AM13" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AN13" s="299"/>
-      <c r="AO13" s="295" t="s">
+      <c r="AN13" s="296"/>
+      <c r="AO13" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AP13" s="296"/>
-      <c r="AQ13" s="296" t="s">
+      <c r="AP13" s="295"/>
+      <c r="AQ13" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AR13" s="299"/>
-      <c r="AS13" s="295" t="s">
+      <c r="AR13" s="296"/>
+      <c r="AS13" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AT13" s="296"/>
-      <c r="AU13" s="296" t="s">
+      <c r="AT13" s="295"/>
+      <c r="AU13" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AV13" s="299"/>
-      <c r="AW13" s="295" t="s">
+      <c r="AV13" s="296"/>
+      <c r="AW13" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AX13" s="296"/>
-      <c r="AY13" s="296" t="s">
+      <c r="AX13" s="295"/>
+      <c r="AY13" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AZ13" s="299"/>
+      <c r="AZ13" s="296"/>
       <c r="BA13" s="257">
         <f t="shared" si="0"/>
         <v>3541.48</v>
@@ -11227,62 +11227,62 @@
       <c r="X14" s="209">
         <v>0</v>
       </c>
-      <c r="Y14" s="295" t="s">
+      <c r="Y14" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="Z14" s="296"/>
-      <c r="AA14" s="296" t="s">
+      <c r="Z14" s="295"/>
+      <c r="AA14" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AB14" s="299"/>
-      <c r="AC14" s="295" t="s">
+      <c r="AB14" s="296"/>
+      <c r="AC14" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AD14" s="296"/>
-      <c r="AE14" s="296" t="s">
+      <c r="AD14" s="295"/>
+      <c r="AE14" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AF14" s="299"/>
-      <c r="AG14" s="295" t="s">
+      <c r="AF14" s="296"/>
+      <c r="AG14" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AH14" s="296"/>
-      <c r="AI14" s="296" t="s">
+      <c r="AH14" s="295"/>
+      <c r="AI14" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AJ14" s="299"/>
-      <c r="AK14" s="295" t="s">
+      <c r="AJ14" s="296"/>
+      <c r="AK14" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AL14" s="296"/>
-      <c r="AM14" s="296" t="s">
+      <c r="AL14" s="295"/>
+      <c r="AM14" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AN14" s="299"/>
-      <c r="AO14" s="295" t="s">
+      <c r="AN14" s="296"/>
+      <c r="AO14" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AP14" s="296"/>
-      <c r="AQ14" s="296" t="s">
+      <c r="AP14" s="295"/>
+      <c r="AQ14" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AR14" s="299"/>
-      <c r="AS14" s="295" t="s">
+      <c r="AR14" s="296"/>
+      <c r="AS14" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AT14" s="296"/>
-      <c r="AU14" s="296" t="s">
+      <c r="AT14" s="295"/>
+      <c r="AU14" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AV14" s="299"/>
-      <c r="AW14" s="295" t="s">
+      <c r="AV14" s="296"/>
+      <c r="AW14" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AX14" s="296"/>
-      <c r="AY14" s="296" t="s">
+      <c r="AX14" s="295"/>
+      <c r="AY14" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AZ14" s="299"/>
+      <c r="AZ14" s="296"/>
       <c r="BA14" s="257">
         <f t="shared" si="0"/>
         <v>58229.89</v>
@@ -11361,62 +11361,62 @@
       <c r="X15" s="209">
         <v>0</v>
       </c>
-      <c r="Y15" s="295" t="s">
+      <c r="Y15" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="Z15" s="296"/>
-      <c r="AA15" s="296" t="s">
+      <c r="Z15" s="295"/>
+      <c r="AA15" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AB15" s="299"/>
-      <c r="AC15" s="295" t="s">
+      <c r="AB15" s="296"/>
+      <c r="AC15" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AD15" s="296"/>
-      <c r="AE15" s="296" t="s">
+      <c r="AD15" s="295"/>
+      <c r="AE15" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AF15" s="299"/>
-      <c r="AG15" s="295" t="s">
+      <c r="AF15" s="296"/>
+      <c r="AG15" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AH15" s="296"/>
-      <c r="AI15" s="296" t="s">
+      <c r="AH15" s="295"/>
+      <c r="AI15" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AJ15" s="299"/>
-      <c r="AK15" s="295" t="s">
+      <c r="AJ15" s="296"/>
+      <c r="AK15" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AL15" s="296"/>
-      <c r="AM15" s="296" t="s">
+      <c r="AL15" s="295"/>
+      <c r="AM15" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AN15" s="299"/>
-      <c r="AO15" s="295" t="s">
+      <c r="AN15" s="296"/>
+      <c r="AO15" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AP15" s="296"/>
-      <c r="AQ15" s="296" t="s">
+      <c r="AP15" s="295"/>
+      <c r="AQ15" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AR15" s="299"/>
-      <c r="AS15" s="295" t="s">
+      <c r="AR15" s="296"/>
+      <c r="AS15" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AT15" s="296"/>
-      <c r="AU15" s="296" t="s">
+      <c r="AT15" s="295"/>
+      <c r="AU15" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AV15" s="299"/>
-      <c r="AW15" s="295" t="s">
+      <c r="AV15" s="296"/>
+      <c r="AW15" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AX15" s="296"/>
-      <c r="AY15" s="296" t="s">
+      <c r="AX15" s="295"/>
+      <c r="AY15" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AZ15" s="299"/>
+      <c r="AZ15" s="296"/>
       <c r="BA15" s="257">
         <f t="shared" si="0"/>
         <v>130564.39</v>
@@ -11780,86 +11780,86 @@
       <c r="L18" s="204">
         <v>0</v>
       </c>
-      <c r="M18" s="301" t="s">
+      <c r="M18" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="N18" s="309"/>
-      <c r="O18" s="301" t="s">
+      <c r="N18" s="299"/>
+      <c r="O18" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="P18" s="309"/>
-      <c r="Q18" s="301" t="s">
+      <c r="P18" s="299"/>
+      <c r="Q18" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="R18" s="309"/>
-      <c r="S18" s="301" t="s">
+      <c r="R18" s="299"/>
+      <c r="S18" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="T18" s="302"/>
-      <c r="U18" s="295" t="s">
+      <c r="T18" s="312"/>
+      <c r="U18" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="V18" s="296"/>
-      <c r="W18" s="296" t="s">
+      <c r="V18" s="295"/>
+      <c r="W18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="X18" s="299"/>
-      <c r="Y18" s="295" t="s">
+      <c r="X18" s="296"/>
+      <c r="Y18" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="Z18" s="296"/>
-      <c r="AA18" s="296" t="s">
+      <c r="Z18" s="295"/>
+      <c r="AA18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AB18" s="299"/>
-      <c r="AC18" s="295" t="s">
+      <c r="AB18" s="296"/>
+      <c r="AC18" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AD18" s="296"/>
-      <c r="AE18" s="296" t="s">
+      <c r="AD18" s="295"/>
+      <c r="AE18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AF18" s="299"/>
-      <c r="AG18" s="295" t="s">
+      <c r="AF18" s="296"/>
+      <c r="AG18" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AH18" s="296"/>
-      <c r="AI18" s="296" t="s">
+      <c r="AH18" s="295"/>
+      <c r="AI18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AJ18" s="299"/>
-      <c r="AK18" s="295" t="s">
+      <c r="AJ18" s="296"/>
+      <c r="AK18" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AL18" s="296"/>
-      <c r="AM18" s="296" t="s">
+      <c r="AL18" s="295"/>
+      <c r="AM18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AN18" s="299"/>
-      <c r="AO18" s="295" t="s">
+      <c r="AN18" s="296"/>
+      <c r="AO18" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AP18" s="296"/>
-      <c r="AQ18" s="296" t="s">
+      <c r="AP18" s="295"/>
+      <c r="AQ18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AR18" s="299"/>
-      <c r="AS18" s="295" t="s">
+      <c r="AR18" s="296"/>
+      <c r="AS18" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AT18" s="296"/>
-      <c r="AU18" s="296" t="s">
+      <c r="AT18" s="295"/>
+      <c r="AU18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AV18" s="299"/>
-      <c r="AW18" s="295" t="s">
+      <c r="AV18" s="296"/>
+      <c r="AW18" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AX18" s="296"/>
-      <c r="AY18" s="296" t="s">
+      <c r="AX18" s="295"/>
+      <c r="AY18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AZ18" s="299"/>
+      <c r="AZ18" s="296"/>
       <c r="BA18" s="257">
         <f t="shared" si="0"/>
         <v>141707.61000000002</v>
@@ -11890,94 +11890,94 @@
       <c r="H19" s="214">
         <v>0</v>
       </c>
-      <c r="I19" s="295" t="s">
+      <c r="I19" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="J19" s="296"/>
-      <c r="K19" s="296" t="s">
+      <c r="J19" s="295"/>
+      <c r="K19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="L19" s="296"/>
-      <c r="M19" s="301" t="s">
+      <c r="L19" s="295"/>
+      <c r="M19" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="N19" s="309"/>
-      <c r="O19" s="301" t="s">
+      <c r="N19" s="299"/>
+      <c r="O19" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="P19" s="309"/>
-      <c r="Q19" s="301" t="s">
+      <c r="P19" s="299"/>
+      <c r="Q19" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="R19" s="309"/>
-      <c r="S19" s="301" t="s">
+      <c r="R19" s="299"/>
+      <c r="S19" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="T19" s="302"/>
-      <c r="U19" s="295" t="s">
+      <c r="T19" s="312"/>
+      <c r="U19" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="V19" s="296"/>
-      <c r="W19" s="296" t="s">
+      <c r="V19" s="295"/>
+      <c r="W19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="X19" s="299"/>
-      <c r="Y19" s="295" t="s">
+      <c r="X19" s="296"/>
+      <c r="Y19" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="Z19" s="296"/>
-      <c r="AA19" s="296" t="s">
+      <c r="Z19" s="295"/>
+      <c r="AA19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AB19" s="299"/>
-      <c r="AC19" s="295" t="s">
+      <c r="AB19" s="296"/>
+      <c r="AC19" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AD19" s="296"/>
-      <c r="AE19" s="296" t="s">
+      <c r="AD19" s="295"/>
+      <c r="AE19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AF19" s="299"/>
-      <c r="AG19" s="295" t="s">
+      <c r="AF19" s="296"/>
+      <c r="AG19" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AH19" s="296"/>
-      <c r="AI19" s="296" t="s">
+      <c r="AH19" s="295"/>
+      <c r="AI19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AJ19" s="299"/>
-      <c r="AK19" s="295" t="s">
+      <c r="AJ19" s="296"/>
+      <c r="AK19" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AL19" s="296"/>
-      <c r="AM19" s="296" t="s">
+      <c r="AL19" s="295"/>
+      <c r="AM19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AN19" s="299"/>
-      <c r="AO19" s="295" t="s">
+      <c r="AN19" s="296"/>
+      <c r="AO19" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AP19" s="296"/>
-      <c r="AQ19" s="296" t="s">
+      <c r="AP19" s="295"/>
+      <c r="AQ19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AR19" s="299"/>
-      <c r="AS19" s="295" t="s">
+      <c r="AR19" s="296"/>
+      <c r="AS19" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AT19" s="296"/>
-      <c r="AU19" s="296" t="s">
+      <c r="AT19" s="295"/>
+      <c r="AU19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AV19" s="299"/>
-      <c r="AW19" s="295" t="s">
+      <c r="AV19" s="296"/>
+      <c r="AW19" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AX19" s="296"/>
-      <c r="AY19" s="296" t="s">
+      <c r="AX19" s="295"/>
+      <c r="AY19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AZ19" s="299"/>
+      <c r="AZ19" s="296"/>
       <c r="BA19" s="257">
         <f t="shared" si="0"/>
         <v>99385</v>
@@ -12497,94 +12497,94 @@
       <c r="H23" s="214">
         <v>0</v>
       </c>
-      <c r="I23" s="310" t="s">
+      <c r="I23" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="J23" s="309"/>
-      <c r="K23" s="301" t="s">
+      <c r="J23" s="299"/>
+      <c r="K23" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="L23" s="311"/>
-      <c r="M23" s="310" t="s">
+      <c r="L23" s="301"/>
+      <c r="M23" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="N23" s="309"/>
-      <c r="O23" s="301" t="s">
+      <c r="N23" s="299"/>
+      <c r="O23" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="P23" s="311"/>
-      <c r="Q23" s="310" t="s">
+      <c r="P23" s="301"/>
+      <c r="Q23" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="R23" s="309"/>
-      <c r="S23" s="301" t="s">
+      <c r="R23" s="299"/>
+      <c r="S23" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="T23" s="311"/>
-      <c r="U23" s="310" t="s">
+      <c r="T23" s="301"/>
+      <c r="U23" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="V23" s="309"/>
-      <c r="W23" s="301" t="s">
+      <c r="V23" s="299"/>
+      <c r="W23" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="X23" s="311"/>
-      <c r="Y23" s="310" t="s">
+      <c r="X23" s="301"/>
+      <c r="Y23" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="Z23" s="309"/>
-      <c r="AA23" s="301" t="s">
+      <c r="Z23" s="299"/>
+      <c r="AA23" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="AB23" s="311"/>
-      <c r="AC23" s="310" t="s">
+      <c r="AB23" s="301"/>
+      <c r="AC23" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="AD23" s="309"/>
-      <c r="AE23" s="301" t="s">
+      <c r="AD23" s="299"/>
+      <c r="AE23" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="AF23" s="311"/>
-      <c r="AG23" s="310" t="s">
+      <c r="AF23" s="301"/>
+      <c r="AG23" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="AH23" s="309"/>
-      <c r="AI23" s="301" t="s">
+      <c r="AH23" s="299"/>
+      <c r="AI23" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="AJ23" s="311"/>
-      <c r="AK23" s="310" t="s">
+      <c r="AJ23" s="301"/>
+      <c r="AK23" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="AL23" s="309"/>
-      <c r="AM23" s="301" t="s">
+      <c r="AL23" s="299"/>
+      <c r="AM23" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="AN23" s="311"/>
-      <c r="AO23" s="310" t="s">
+      <c r="AN23" s="301"/>
+      <c r="AO23" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="AP23" s="309"/>
-      <c r="AQ23" s="301" t="s">
+      <c r="AP23" s="299"/>
+      <c r="AQ23" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="AR23" s="311"/>
-      <c r="AS23" s="310" t="s">
+      <c r="AR23" s="301"/>
+      <c r="AS23" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="AT23" s="309"/>
-      <c r="AU23" s="301" t="s">
+      <c r="AT23" s="299"/>
+      <c r="AU23" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="AV23" s="311"/>
-      <c r="AW23" s="310" t="s">
+      <c r="AV23" s="301"/>
+      <c r="AW23" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="AX23" s="309"/>
-      <c r="AY23" s="301" t="s">
+      <c r="AX23" s="299"/>
+      <c r="AY23" s="300" t="s">
         <v>233</v>
       </c>
-      <c r="AZ23" s="311"/>
+      <c r="AZ23" s="301"/>
       <c r="BA23" s="257">
         <f t="shared" si="0"/>
         <v>163670.23000000001</v>
@@ -12841,54 +12841,54 @@
       <c r="AB25" s="209">
         <v>0</v>
       </c>
-      <c r="AC25" s="295" t="s">
+      <c r="AC25" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AD25" s="296"/>
-      <c r="AE25" s="296" t="s">
+      <c r="AD25" s="295"/>
+      <c r="AE25" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AF25" s="299"/>
-      <c r="AG25" s="295" t="s">
+      <c r="AF25" s="296"/>
+      <c r="AG25" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AH25" s="296"/>
-      <c r="AI25" s="296" t="s">
+      <c r="AH25" s="295"/>
+      <c r="AI25" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AJ25" s="299"/>
-      <c r="AK25" s="295" t="s">
+      <c r="AJ25" s="296"/>
+      <c r="AK25" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AL25" s="296"/>
-      <c r="AM25" s="296" t="s">
+      <c r="AL25" s="295"/>
+      <c r="AM25" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AN25" s="299"/>
-      <c r="AO25" s="295" t="s">
+      <c r="AN25" s="296"/>
+      <c r="AO25" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AP25" s="296"/>
-      <c r="AQ25" s="296" t="s">
+      <c r="AP25" s="295"/>
+      <c r="AQ25" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AR25" s="299"/>
-      <c r="AS25" s="295" t="s">
+      <c r="AR25" s="296"/>
+      <c r="AS25" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AT25" s="296"/>
-      <c r="AU25" s="296" t="s">
+      <c r="AT25" s="295"/>
+      <c r="AU25" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AV25" s="299"/>
-      <c r="AW25" s="295" t="s">
+      <c r="AV25" s="296"/>
+      <c r="AW25" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AX25" s="296"/>
-      <c r="AY25" s="296" t="s">
+      <c r="AX25" s="295"/>
+      <c r="AY25" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AZ25" s="299"/>
+      <c r="AZ25" s="296"/>
       <c r="BA25" s="257">
         <f t="shared" si="0"/>
         <v>90477.23</v>
@@ -12992,46 +12992,46 @@
       <c r="AF26" s="211">
         <v>0</v>
       </c>
-      <c r="AG26" s="295" t="s">
+      <c r="AG26" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AH26" s="296"/>
-      <c r="AI26" s="296" t="s">
+      <c r="AH26" s="295"/>
+      <c r="AI26" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AJ26" s="299"/>
-      <c r="AK26" s="295" t="s">
+      <c r="AJ26" s="296"/>
+      <c r="AK26" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AL26" s="296"/>
-      <c r="AM26" s="296" t="s">
+      <c r="AL26" s="295"/>
+      <c r="AM26" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AN26" s="299"/>
-      <c r="AO26" s="295" t="s">
+      <c r="AN26" s="296"/>
+      <c r="AO26" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AP26" s="296"/>
-      <c r="AQ26" s="296" t="s">
+      <c r="AP26" s="295"/>
+      <c r="AQ26" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AR26" s="299"/>
-      <c r="AS26" s="295" t="s">
+      <c r="AR26" s="296"/>
+      <c r="AS26" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AT26" s="296"/>
-      <c r="AU26" s="296" t="s">
+      <c r="AT26" s="295"/>
+      <c r="AU26" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AV26" s="299"/>
-      <c r="AW26" s="295" t="s">
+      <c r="AV26" s="296"/>
+      <c r="AW26" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AX26" s="296"/>
-      <c r="AY26" s="296" t="s">
+      <c r="AX26" s="295"/>
+      <c r="AY26" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AZ26" s="299"/>
+      <c r="AZ26" s="296"/>
       <c r="BA26" s="257">
         <f t="shared" si="0"/>
         <v>65199.1</v>
@@ -13500,22 +13500,22 @@
       <c r="AR29" s="209">
         <v>0</v>
       </c>
-      <c r="AS29" s="295" t="s">
+      <c r="AS29" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AT29" s="296"/>
-      <c r="AU29" s="296" t="s">
+      <c r="AT29" s="295"/>
+      <c r="AU29" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AV29" s="299"/>
-      <c r="AW29" s="295" t="s">
+      <c r="AV29" s="296"/>
+      <c r="AW29" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AX29" s="296"/>
-      <c r="AY29" s="296" t="s">
+      <c r="AX29" s="295"/>
+      <c r="AY29" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AZ29" s="299"/>
+      <c r="AZ29" s="296"/>
       <c r="BA29" s="257">
         <f t="shared" si="0"/>
         <v>518414.18</v>
@@ -13641,30 +13641,30 @@
         <v>44788.195919999998</v>
       </c>
       <c r="AN30" s="209"/>
-      <c r="AO30" s="295" t="s">
+      <c r="AO30" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AP30" s="296"/>
-      <c r="AQ30" s="296" t="s">
+      <c r="AP30" s="295"/>
+      <c r="AQ30" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AR30" s="299"/>
-      <c r="AS30" s="295" t="s">
+      <c r="AR30" s="296"/>
+      <c r="AS30" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AT30" s="296"/>
-      <c r="AU30" s="296" t="s">
+      <c r="AT30" s="295"/>
+      <c r="AU30" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AV30" s="299"/>
-      <c r="AW30" s="295" t="s">
+      <c r="AV30" s="296"/>
+      <c r="AW30" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AX30" s="296"/>
-      <c r="AY30" s="296" t="s">
+      <c r="AX30" s="295"/>
+      <c r="AY30" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AZ30" s="299"/>
+      <c r="AZ30" s="296"/>
       <c r="BA30" s="257">
         <f t="shared" si="0"/>
         <v>48341.279999999999</v>
@@ -14204,59 +14204,120 @@
     <sortCondition ref="A6:A16"/>
   </sortState>
   <mergeCells count="191">
-    <mergeCell ref="AM15:AN15"/>
-    <mergeCell ref="AO13:AP13"/>
-    <mergeCell ref="AQ13:AR13"/>
-    <mergeCell ref="AO14:AP14"/>
-    <mergeCell ref="AQ14:AR14"/>
-    <mergeCell ref="AO15:AP15"/>
-    <mergeCell ref="AQ15:AR15"/>
-    <mergeCell ref="AU14:AV14"/>
-    <mergeCell ref="AS15:AT15"/>
-    <mergeCell ref="AU15:AV15"/>
-    <mergeCell ref="AW13:AX13"/>
-    <mergeCell ref="AY13:AZ13"/>
-    <mergeCell ref="AW14:AX14"/>
-    <mergeCell ref="AY14:AZ14"/>
-    <mergeCell ref="AS18:AT18"/>
-    <mergeCell ref="AS19:AT19"/>
-    <mergeCell ref="AU18:AV18"/>
-    <mergeCell ref="AU19:AV19"/>
-    <mergeCell ref="AW18:AX18"/>
-    <mergeCell ref="AW19:AX19"/>
-    <mergeCell ref="AY18:AZ18"/>
-    <mergeCell ref="AY19:AZ19"/>
-    <mergeCell ref="AW15:AX15"/>
-    <mergeCell ref="AY15:AZ15"/>
-    <mergeCell ref="AS13:AT13"/>
-    <mergeCell ref="AU13:AV13"/>
-    <mergeCell ref="AS14:AT14"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="Y23:Z23"/>
-    <mergeCell ref="AS23:AT23"/>
-    <mergeCell ref="AU23:AV23"/>
-    <mergeCell ref="AY30:AZ30"/>
-    <mergeCell ref="AS25:AT25"/>
-    <mergeCell ref="AU25:AV25"/>
-    <mergeCell ref="AS26:AT26"/>
-    <mergeCell ref="AU26:AV26"/>
-    <mergeCell ref="AW25:AX25"/>
-    <mergeCell ref="AY25:AZ25"/>
-    <mergeCell ref="AW26:AX26"/>
-    <mergeCell ref="AY26:AZ26"/>
-    <mergeCell ref="AS29:AT29"/>
-    <mergeCell ref="AU29:AV29"/>
-    <mergeCell ref="AW29:AX29"/>
-    <mergeCell ref="AY29:AZ29"/>
-    <mergeCell ref="AW23:AX23"/>
-    <mergeCell ref="AY23:AZ23"/>
+    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="AG15:AH15"/>
+    <mergeCell ref="AI13:AJ13"/>
+    <mergeCell ref="AI14:AJ14"/>
+    <mergeCell ref="AI15:AJ15"/>
+    <mergeCell ref="AI19:AJ19"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="AG7:AH7"/>
+    <mergeCell ref="AG14:AH14"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="AG13:AH13"/>
+    <mergeCell ref="AG18:AH18"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="W19:X19"/>
+    <mergeCell ref="Y19:Z19"/>
+    <mergeCell ref="AA19:AB19"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="W18:X18"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="AA18:AB18"/>
+    <mergeCell ref="AK25:AL25"/>
+    <mergeCell ref="AK26:AL26"/>
+    <mergeCell ref="AO25:AP25"/>
+    <mergeCell ref="AO26:AP26"/>
+    <mergeCell ref="AC19:AD19"/>
+    <mergeCell ref="AG23:AH23"/>
+    <mergeCell ref="AG19:AH19"/>
+    <mergeCell ref="AI23:AJ23"/>
+    <mergeCell ref="AC25:AD25"/>
+    <mergeCell ref="AE25:AF25"/>
+    <mergeCell ref="AG25:AH25"/>
+    <mergeCell ref="AG26:AH26"/>
+    <mergeCell ref="AI25:AJ25"/>
+    <mergeCell ref="AI26:AJ26"/>
+    <mergeCell ref="AC23:AD23"/>
+    <mergeCell ref="AE19:AF19"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="AK7:AL7"/>
+    <mergeCell ref="AM6:AN6"/>
+    <mergeCell ref="AM7:AN7"/>
+    <mergeCell ref="AE23:AF23"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="AA13:AB13"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="AI7:AJ7"/>
+    <mergeCell ref="AI18:AJ18"/>
+    <mergeCell ref="AC13:AD13"/>
+    <mergeCell ref="AC14:AD14"/>
+    <mergeCell ref="AK10:AL10"/>
+    <mergeCell ref="AA23:AB23"/>
+    <mergeCell ref="AE13:AF13"/>
+    <mergeCell ref="AE14:AF14"/>
+    <mergeCell ref="AE15:AF15"/>
+    <mergeCell ref="AE18:AF18"/>
+    <mergeCell ref="AM13:AN13"/>
+    <mergeCell ref="AK14:AL14"/>
+    <mergeCell ref="AM14:AN14"/>
+    <mergeCell ref="AK15:AL15"/>
+    <mergeCell ref="E1:BA1"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="Y4:AB4"/>
+    <mergeCell ref="U4:X4"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="AG4:AJ4"/>
+    <mergeCell ref="AK4:AN4"/>
+    <mergeCell ref="AO10:AP10"/>
+    <mergeCell ref="AO9:AP9"/>
+    <mergeCell ref="AQ9:AR9"/>
+    <mergeCell ref="AQ25:AR25"/>
+    <mergeCell ref="AM25:AN25"/>
+    <mergeCell ref="AO30:AP30"/>
+    <mergeCell ref="AQ30:AR30"/>
+    <mergeCell ref="AQ26:AR26"/>
+    <mergeCell ref="AK9:AL9"/>
+    <mergeCell ref="AM9:AN9"/>
+    <mergeCell ref="AM26:AN26"/>
+    <mergeCell ref="AK18:AL18"/>
+    <mergeCell ref="AK19:AL19"/>
+    <mergeCell ref="AM18:AN18"/>
+    <mergeCell ref="AM19:AN19"/>
+    <mergeCell ref="AO18:AP18"/>
+    <mergeCell ref="AO19:AP19"/>
+    <mergeCell ref="AQ18:AR18"/>
+    <mergeCell ref="AQ19:AR19"/>
+    <mergeCell ref="AK23:AL23"/>
+    <mergeCell ref="AM23:AN23"/>
+    <mergeCell ref="AO23:AP23"/>
+    <mergeCell ref="AQ23:AR23"/>
+    <mergeCell ref="AK13:AL13"/>
     <mergeCell ref="AS10:AT10"/>
     <mergeCell ref="AW10:AX10"/>
     <mergeCell ref="AO7:AP7"/>
@@ -14281,120 +14342,59 @@
     <mergeCell ref="AY7:AZ7"/>
     <mergeCell ref="AW9:AX9"/>
     <mergeCell ref="AY9:AZ9"/>
-    <mergeCell ref="AO10:AP10"/>
-    <mergeCell ref="AO9:AP9"/>
-    <mergeCell ref="AQ9:AR9"/>
-    <mergeCell ref="AQ25:AR25"/>
-    <mergeCell ref="AM25:AN25"/>
-    <mergeCell ref="AO30:AP30"/>
-    <mergeCell ref="AQ30:AR30"/>
-    <mergeCell ref="AQ26:AR26"/>
-    <mergeCell ref="AK9:AL9"/>
-    <mergeCell ref="AM9:AN9"/>
-    <mergeCell ref="AM26:AN26"/>
-    <mergeCell ref="AK18:AL18"/>
-    <mergeCell ref="AK19:AL19"/>
-    <mergeCell ref="AM18:AN18"/>
-    <mergeCell ref="AM19:AN19"/>
-    <mergeCell ref="AO18:AP18"/>
-    <mergeCell ref="AO19:AP19"/>
-    <mergeCell ref="AQ18:AR18"/>
-    <mergeCell ref="AQ19:AR19"/>
-    <mergeCell ref="AK23:AL23"/>
-    <mergeCell ref="AM23:AN23"/>
-    <mergeCell ref="AO23:AP23"/>
-    <mergeCell ref="AQ23:AR23"/>
-    <mergeCell ref="AK13:AL13"/>
-    <mergeCell ref="E1:BA1"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="Y4:AB4"/>
-    <mergeCell ref="U4:X4"/>
-    <mergeCell ref="AC4:AF4"/>
-    <mergeCell ref="AG4:AJ4"/>
-    <mergeCell ref="AK4:AN4"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="AK7:AL7"/>
-    <mergeCell ref="AM6:AN6"/>
-    <mergeCell ref="AM7:AN7"/>
-    <mergeCell ref="AE23:AF23"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="AA13:AB13"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="AC15:AD15"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="AI7:AJ7"/>
-    <mergeCell ref="AI18:AJ18"/>
-    <mergeCell ref="AC13:AD13"/>
-    <mergeCell ref="AC14:AD14"/>
-    <mergeCell ref="AK10:AL10"/>
-    <mergeCell ref="AA23:AB23"/>
-    <mergeCell ref="AE13:AF13"/>
-    <mergeCell ref="AE14:AF14"/>
-    <mergeCell ref="AE15:AF15"/>
-    <mergeCell ref="AE18:AF18"/>
-    <mergeCell ref="AM13:AN13"/>
-    <mergeCell ref="AK14:AL14"/>
-    <mergeCell ref="AM14:AN14"/>
-    <mergeCell ref="AK15:AL15"/>
-    <mergeCell ref="AK25:AL25"/>
-    <mergeCell ref="AK26:AL26"/>
-    <mergeCell ref="AO25:AP25"/>
-    <mergeCell ref="AO26:AP26"/>
-    <mergeCell ref="AC19:AD19"/>
-    <mergeCell ref="AG23:AH23"/>
-    <mergeCell ref="AG19:AH19"/>
-    <mergeCell ref="AI23:AJ23"/>
-    <mergeCell ref="AC25:AD25"/>
-    <mergeCell ref="AE25:AF25"/>
-    <mergeCell ref="AG25:AH25"/>
-    <mergeCell ref="AG26:AH26"/>
-    <mergeCell ref="AI25:AJ25"/>
-    <mergeCell ref="AI26:AJ26"/>
-    <mergeCell ref="AC23:AD23"/>
-    <mergeCell ref="AE19:AF19"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="W19:X19"/>
-    <mergeCell ref="Y19:Z19"/>
-    <mergeCell ref="AA19:AB19"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="Y13:Z13"/>
-    <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="W18:X18"/>
-    <mergeCell ref="Y18:Z18"/>
-    <mergeCell ref="AA18:AB18"/>
-    <mergeCell ref="AC18:AD18"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="AG15:AH15"/>
-    <mergeCell ref="AI13:AJ13"/>
-    <mergeCell ref="AI14:AJ14"/>
-    <mergeCell ref="AI15:AJ15"/>
-    <mergeCell ref="AI19:AJ19"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="AG7:AH7"/>
-    <mergeCell ref="AG14:AH14"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="AG13:AH13"/>
-    <mergeCell ref="AG18:AH18"/>
+    <mergeCell ref="AS23:AT23"/>
+    <mergeCell ref="AU23:AV23"/>
+    <mergeCell ref="AY30:AZ30"/>
+    <mergeCell ref="AS25:AT25"/>
+    <mergeCell ref="AU25:AV25"/>
+    <mergeCell ref="AS26:AT26"/>
+    <mergeCell ref="AU26:AV26"/>
+    <mergeCell ref="AW25:AX25"/>
+    <mergeCell ref="AY25:AZ25"/>
+    <mergeCell ref="AW26:AX26"/>
+    <mergeCell ref="AY26:AZ26"/>
+    <mergeCell ref="AS29:AT29"/>
+    <mergeCell ref="AU29:AV29"/>
+    <mergeCell ref="AW29:AX29"/>
+    <mergeCell ref="AY29:AZ29"/>
+    <mergeCell ref="AW23:AX23"/>
+    <mergeCell ref="AY23:AZ23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="Y23:Z23"/>
+    <mergeCell ref="AW13:AX13"/>
+    <mergeCell ref="AY13:AZ13"/>
+    <mergeCell ref="AW14:AX14"/>
+    <mergeCell ref="AY14:AZ14"/>
+    <mergeCell ref="AS18:AT18"/>
+    <mergeCell ref="AS19:AT19"/>
+    <mergeCell ref="AU18:AV18"/>
+    <mergeCell ref="AU19:AV19"/>
+    <mergeCell ref="AW18:AX18"/>
+    <mergeCell ref="AW19:AX19"/>
+    <mergeCell ref="AY18:AZ18"/>
+    <mergeCell ref="AY19:AZ19"/>
+    <mergeCell ref="AW15:AX15"/>
+    <mergeCell ref="AY15:AZ15"/>
+    <mergeCell ref="AS13:AT13"/>
+    <mergeCell ref="AU13:AV13"/>
+    <mergeCell ref="AS14:AT14"/>
+    <mergeCell ref="AM15:AN15"/>
+    <mergeCell ref="AO13:AP13"/>
+    <mergeCell ref="AQ13:AR13"/>
+    <mergeCell ref="AO14:AP14"/>
+    <mergeCell ref="AQ14:AR14"/>
+    <mergeCell ref="AO15:AP15"/>
+    <mergeCell ref="AQ15:AR15"/>
+    <mergeCell ref="AU14:AV14"/>
+    <mergeCell ref="AS15:AT15"/>
+    <mergeCell ref="AU15:AV15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -16344,17 +16344,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C49:G49"/>
     <mergeCell ref="C50:G50"/>
     <mergeCell ref="C52:G52"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="C21:G21"/>
     <mergeCell ref="C23:G23"/>
     <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="C49:G49"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -17788,10 +17788,10 @@
   <dimension ref="A1:XEX31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="X6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="M15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="Z6" sqref="Z6:AA24"/>
+      <selection pane="bottomRight" activeCell="N22" sqref="N22:Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -17937,93 +17937,93 @@
       <c r="AD3" s="201"/>
     </row>
     <row r="4" spans="1:56 16377:16378" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A4" s="303" t="s">
+      <c r="A4" s="313" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="305" t="s">
+      <c r="B4" s="315" t="s">
         <v>234</v>
       </c>
-      <c r="C4" s="305" t="s">
+      <c r="C4" s="315" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="307" t="s">
+      <c r="D4" s="317" t="s">
         <v>236</v>
       </c>
-      <c r="E4" s="305" t="s">
+      <c r="E4" s="315" t="s">
         <v>310</v>
       </c>
-      <c r="F4" s="317" t="s">
+      <c r="F4" s="309" t="s">
         <v>250</v>
       </c>
-      <c r="G4" s="316"/>
-      <c r="H4" s="316"/>
-      <c r="I4" s="318"/>
-      <c r="J4" s="316" t="s">
+      <c r="G4" s="306"/>
+      <c r="H4" s="306"/>
+      <c r="I4" s="307"/>
+      <c r="J4" s="306" t="s">
         <v>249</v>
       </c>
-      <c r="K4" s="316"/>
-      <c r="L4" s="316"/>
-      <c r="M4" s="316"/>
-      <c r="N4" s="317" t="s">
+      <c r="K4" s="306"/>
+      <c r="L4" s="306"/>
+      <c r="M4" s="306"/>
+      <c r="N4" s="309" t="s">
         <v>251</v>
       </c>
-      <c r="O4" s="316"/>
-      <c r="P4" s="316"/>
-      <c r="Q4" s="318"/>
-      <c r="R4" s="317" t="s">
+      <c r="O4" s="306"/>
+      <c r="P4" s="306"/>
+      <c r="Q4" s="307"/>
+      <c r="R4" s="309" t="s">
         <v>256</v>
       </c>
-      <c r="S4" s="316"/>
-      <c r="T4" s="316"/>
-      <c r="U4" s="318"/>
-      <c r="V4" s="316" t="s">
+      <c r="S4" s="306"/>
+      <c r="T4" s="306"/>
+      <c r="U4" s="307"/>
+      <c r="V4" s="306" t="s">
         <v>257</v>
       </c>
-      <c r="W4" s="316"/>
-      <c r="X4" s="316"/>
-      <c r="Y4" s="316"/>
-      <c r="Z4" s="317" t="s">
+      <c r="W4" s="306"/>
+      <c r="X4" s="306"/>
+      <c r="Y4" s="306"/>
+      <c r="Z4" s="309" t="s">
         <v>258</v>
       </c>
-      <c r="AA4" s="316"/>
-      <c r="AB4" s="316"/>
-      <c r="AC4" s="318"/>
-      <c r="AD4" s="317" t="s">
+      <c r="AA4" s="306"/>
+      <c r="AB4" s="306"/>
+      <c r="AC4" s="307"/>
+      <c r="AD4" s="309" t="s">
         <v>260</v>
       </c>
-      <c r="AE4" s="316"/>
-      <c r="AF4" s="316"/>
-      <c r="AG4" s="318"/>
-      <c r="AH4" s="317" t="s">
+      <c r="AE4" s="306"/>
+      <c r="AF4" s="306"/>
+      <c r="AG4" s="307"/>
+      <c r="AH4" s="309" t="s">
         <v>261</v>
       </c>
-      <c r="AI4" s="316"/>
-      <c r="AJ4" s="316"/>
-      <c r="AK4" s="318"/>
-      <c r="AL4" s="317" t="s">
+      <c r="AI4" s="306"/>
+      <c r="AJ4" s="306"/>
+      <c r="AK4" s="307"/>
+      <c r="AL4" s="309" t="s">
         <v>237</v>
       </c>
-      <c r="AM4" s="316"/>
-      <c r="AN4" s="316"/>
-      <c r="AO4" s="318"/>
-      <c r="AP4" s="316" t="s">
+      <c r="AM4" s="306"/>
+      <c r="AN4" s="306"/>
+      <c r="AO4" s="307"/>
+      <c r="AP4" s="306" t="s">
         <v>238</v>
       </c>
-      <c r="AQ4" s="316"/>
-      <c r="AR4" s="316"/>
-      <c r="AS4" s="318"/>
-      <c r="AT4" s="317" t="s">
+      <c r="AQ4" s="306"/>
+      <c r="AR4" s="306"/>
+      <c r="AS4" s="307"/>
+      <c r="AT4" s="309" t="s">
         <v>239</v>
       </c>
-      <c r="AU4" s="316"/>
-      <c r="AV4" s="316"/>
-      <c r="AW4" s="318"/>
-      <c r="AX4" s="317" t="s">
+      <c r="AU4" s="306"/>
+      <c r="AV4" s="306"/>
+      <c r="AW4" s="307"/>
+      <c r="AX4" s="309" t="s">
         <v>240</v>
       </c>
-      <c r="AY4" s="316"/>
-      <c r="AZ4" s="316"/>
-      <c r="BA4" s="318"/>
+      <c r="AY4" s="306"/>
+      <c r="AZ4" s="306"/>
+      <c r="BA4" s="307"/>
       <c r="BB4" s="220" t="s">
         <v>307</v>
       </c>
@@ -18035,11 +18035,11 @@
       </c>
     </row>
     <row r="5" spans="1:56 16377:16378" s="145" customFormat="1" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A5" s="304"/>
-      <c r="B5" s="306"/>
-      <c r="C5" s="306"/>
-      <c r="D5" s="308"/>
-      <c r="E5" s="306"/>
+      <c r="A5" s="314"/>
+      <c r="B5" s="316"/>
+      <c r="C5" s="316"/>
+      <c r="D5" s="318"/>
+      <c r="E5" s="316"/>
       <c r="F5" s="172" t="s">
         <v>246</v>
       </c>
@@ -20661,15 +20661,11 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="AD4:AG4"/>
-    <mergeCell ref="AT4:AW4"/>
-    <mergeCell ref="AX4:BA4"/>
-    <mergeCell ref="V4:Y4"/>
-    <mergeCell ref="Z4:AC4"/>
-    <mergeCell ref="AL4:AO4"/>
-    <mergeCell ref="AP4:AS4"/>
-    <mergeCell ref="AH4:AK4"/>
+    <mergeCell ref="AX9:BA9"/>
+    <mergeCell ref="AH9:AK9"/>
+    <mergeCell ref="AL9:AO9"/>
+    <mergeCell ref="AP9:AS9"/>
+    <mergeCell ref="AT9:AW9"/>
     <mergeCell ref="J9:M9"/>
     <mergeCell ref="N9:Q9"/>
     <mergeCell ref="A4:A5"/>
@@ -20680,11 +20676,15 @@
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="AX9:BA9"/>
-    <mergeCell ref="AH9:AK9"/>
-    <mergeCell ref="AL9:AO9"/>
-    <mergeCell ref="AP9:AS9"/>
-    <mergeCell ref="AT9:AW9"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="AT4:AW4"/>
+    <mergeCell ref="AX4:BA4"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="Z4:AC4"/>
+    <mergeCell ref="AL4:AO4"/>
+    <mergeCell ref="AP4:AS4"/>
+    <mergeCell ref="AH4:AK4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -20700,10 +20700,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C60C3C0C-3E40-486A-9B59-1C5056167637}">
-  <dimension ref="A1:G289"/>
+  <dimension ref="A1:G288"/>
   <sheetViews>
-    <sheetView topLeftCell="A266" workbookViewId="0">
-      <selection activeCell="F290" sqref="F290"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="I220" sqref="I220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -25799,126 +25799,126 @@
       </c>
     </row>
     <row r="222" spans="1:7">
-      <c r="A222" s="283">
-        <v>220</v>
-      </c>
-      <c r="B222" s="283" t="s">
-        <v>305</v>
-      </c>
-      <c r="C222" s="283" t="s">
-        <v>222</v>
-      </c>
-      <c r="D222" s="283" t="s">
+      <c r="A222" s="292">
+        <v>106</v>
+      </c>
+      <c r="B222" s="292" t="s">
+        <v>210</v>
+      </c>
+      <c r="C222" s="292" t="s">
+        <v>214</v>
+      </c>
+      <c r="D222" s="292" t="s">
+        <v>202</v>
+      </c>
+      <c r="E222" s="293">
+        <v>45748</v>
+      </c>
+      <c r="F222" s="294">
+        <v>245000</v>
+      </c>
+      <c r="G222" s="294">
+        <v>252573.51</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7">
+      <c r="A223" s="283">
+        <v>154</v>
+      </c>
+      <c r="B223" s="283" t="s">
+        <v>206</v>
+      </c>
+      <c r="C223" s="283" t="s">
+        <v>219</v>
+      </c>
+      <c r="D223" s="283" t="s">
         <v>306</v>
       </c>
-      <c r="E222" s="286">
-        <v>45717</v>
-      </c>
-      <c r="F222" s="285">
-        <v>290064.15999999997</v>
-      </c>
-      <c r="G222" s="285">
-        <v>290064.15999999997</v>
-      </c>
-    </row>
-    <row r="223" spans="1:7">
-      <c r="A223" s="292">
-        <v>106</v>
-      </c>
-      <c r="B223" s="292" t="s">
-        <v>210</v>
-      </c>
-      <c r="C223" s="292" t="s">
-        <v>214</v>
-      </c>
-      <c r="D223" s="292" t="s">
-        <v>202</v>
-      </c>
-      <c r="E223" s="293">
+      <c r="E223" s="286">
         <v>45748</v>
       </c>
-      <c r="F223" s="294">
-        <v>245000</v>
-      </c>
-      <c r="G223" s="294">
-        <v>252573.51</v>
+      <c r="F223" s="285">
+        <v>125000</v>
+      </c>
+      <c r="G223" s="285">
+        <v>127017.52</v>
       </c>
     </row>
     <row r="224" spans="1:7">
       <c r="A224" s="283">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B224" s="283" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C224" s="283" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D224" s="283" t="s">
-        <v>306</v>
+        <v>204</v>
       </c>
       <c r="E224" s="286">
         <v>45748</v>
       </c>
       <c r="F224" s="285">
-        <v>125000</v>
+        <v>72000</v>
       </c>
       <c r="G224" s="285">
-        <v>127017.52</v>
+        <v>110093.142589</v>
       </c>
     </row>
     <row r="225" spans="1:7">
       <c r="A225" s="283">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="B225" s="283" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="C225" s="283" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="D225" s="283" t="s">
-        <v>204</v>
+        <v>306</v>
       </c>
       <c r="E225" s="286">
         <v>45748</v>
       </c>
       <c r="F225" s="285">
-        <v>72000</v>
+        <v>239000</v>
       </c>
       <c r="G225" s="285">
-        <v>110093.142589</v>
+        <v>354792.61</v>
       </c>
     </row>
     <row r="226" spans="1:7">
       <c r="A226" s="283">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B226" s="283" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C226" s="283" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D226" s="283" t="s">
-        <v>306</v>
+        <v>225</v>
       </c>
       <c r="E226" s="286">
         <v>45748</v>
       </c>
       <c r="F226" s="285">
-        <v>239000</v>
+        <v>445485.93</v>
       </c>
       <c r="G226" s="285">
-        <v>354792.61</v>
+        <v>445485.93</v>
       </c>
     </row>
     <row r="227" spans="1:7">
       <c r="A227" s="283">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B227" s="283" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C227" s="283" t="s">
         <v>217</v>
@@ -25930,33 +25930,33 @@
         <v>45748</v>
       </c>
       <c r="F227" s="285">
-        <v>445485.93</v>
+        <v>120000</v>
       </c>
       <c r="G227" s="285">
-        <v>445485.93</v>
+        <v>210261.44</v>
       </c>
     </row>
     <row r="228" spans="1:7">
       <c r="A228" s="283">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B228" s="283" t="s">
-        <v>232</v>
+        <v>265</v>
       </c>
       <c r="C228" s="283" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="D228" s="283" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="E228" s="286">
         <v>45748</v>
       </c>
       <c r="F228" s="285">
-        <v>120000</v>
+        <v>500000</v>
       </c>
       <c r="G228" s="285">
-        <v>210261.44</v>
+        <v>523177.87407679996</v>
       </c>
     </row>
     <row r="229" spans="1:7">
@@ -25964,7 +25964,7 @@
         <v>184</v>
       </c>
       <c r="B229" s="283" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C229" s="283" t="s">
         <v>230</v>
@@ -25976,41 +25976,41 @@
         <v>45748</v>
       </c>
       <c r="F229" s="285">
-        <v>500000</v>
+        <v>265000</v>
       </c>
       <c r="G229" s="285">
-        <v>523177.87407679996</v>
+        <v>274123.785965905</v>
       </c>
     </row>
     <row r="230" spans="1:7">
       <c r="A230" s="283">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B230" s="283" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C230" s="283" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D230" s="283" t="s">
-        <v>231</v>
+        <v>306</v>
       </c>
       <c r="E230" s="286">
         <v>45748</v>
       </c>
       <c r="F230" s="285">
-        <v>265000</v>
+        <v>175000</v>
       </c>
       <c r="G230" s="285">
-        <v>274123.785965905</v>
+        <v>339470.45999999996</v>
       </c>
     </row>
     <row r="231" spans="1:7">
       <c r="A231" s="283">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="B231" s="283" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C231" s="283" t="s">
         <v>219</v>
@@ -26022,44 +26022,44 @@
         <v>45748</v>
       </c>
       <c r="F231" s="285">
-        <v>175000</v>
+        <v>22000</v>
       </c>
       <c r="G231" s="285">
-        <v>339470.45999999996</v>
+        <v>30283.15</v>
       </c>
     </row>
     <row r="232" spans="1:7">
       <c r="A232" s="283">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B232" s="283" t="s">
-        <v>262</v>
+        <v>283</v>
       </c>
       <c r="C232" s="283" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D232" s="283" t="s">
-        <v>306</v>
+        <v>231</v>
       </c>
       <c r="E232" s="286">
         <v>45748</v>
       </c>
       <c r="F232" s="285">
-        <v>22000</v>
+        <v>374000</v>
       </c>
       <c r="G232" s="285">
-        <v>30283.15</v>
+        <v>373407.7182</v>
       </c>
     </row>
     <row r="233" spans="1:7">
       <c r="A233" s="283">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="B233" s="283" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="C233" s="283" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D233" s="283" t="s">
         <v>231</v>
@@ -26068,76 +26068,76 @@
         <v>45748</v>
       </c>
       <c r="F233" s="285">
-        <v>374000</v>
+        <v>300000</v>
       </c>
       <c r="G233" s="285">
-        <v>373407.7182</v>
+        <v>273622.57</v>
       </c>
     </row>
     <row r="234" spans="1:7">
       <c r="A234" s="283">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B234" s="283" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="C234" s="283" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D234" s="283" t="s">
-        <v>231</v>
+        <v>299</v>
       </c>
       <c r="E234" s="286">
         <v>45748</v>
       </c>
       <c r="F234" s="285">
-        <v>300000</v>
+        <v>200000</v>
       </c>
       <c r="G234" s="285">
-        <v>273622.57</v>
+        <v>198060.33</v>
       </c>
     </row>
     <row r="235" spans="1:7">
       <c r="A235" s="283">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B235" s="283" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C235" s="283" t="s">
-        <v>216</v>
+        <v>298</v>
       </c>
       <c r="D235" s="283" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E235" s="286">
         <v>45748</v>
       </c>
       <c r="F235" s="285">
-        <v>200000</v>
+        <v>250000</v>
       </c>
       <c r="G235" s="285">
-        <v>198060.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:7">
       <c r="A236" s="283">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B236" s="283" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C236" s="283" t="s">
-        <v>298</v>
+        <v>222</v>
       </c>
       <c r="D236" s="283" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="E236" s="286">
         <v>45748</v>
       </c>
       <c r="F236" s="285">
-        <v>250000</v>
+        <v>0</v>
       </c>
       <c r="G236" s="285">
         <v>0</v>
@@ -26145,13 +26145,13 @@
     </row>
     <row r="237" spans="1:7">
       <c r="A237" s="283">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="B237" s="283" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="C237" s="283" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D237" s="283" t="s">
         <v>306</v>
@@ -26168,16 +26168,16 @@
     </row>
     <row r="238" spans="1:7">
       <c r="A238" s="283">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B238" s="283" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="C238" s="283" t="s">
         <v>219</v>
       </c>
       <c r="D238" s="283" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E238" s="286">
         <v>45748</v>
@@ -26190,126 +26190,126 @@
       </c>
     </row>
     <row r="239" spans="1:7">
-      <c r="A239" s="283">
-        <v>227</v>
-      </c>
-      <c r="B239" s="283" t="s">
-        <v>303</v>
-      </c>
-      <c r="C239" s="283" t="s">
+      <c r="A239" s="292">
+        <v>106</v>
+      </c>
+      <c r="B239" s="292" t="s">
+        <v>210</v>
+      </c>
+      <c r="C239" s="292" t="s">
+        <v>214</v>
+      </c>
+      <c r="D239" s="292" t="s">
+        <v>202</v>
+      </c>
+      <c r="E239" s="293">
+        <v>45778</v>
+      </c>
+      <c r="F239" s="294">
+        <v>260000</v>
+      </c>
+      <c r="G239" s="294">
+        <v>104492.97</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7">
+      <c r="A240" s="283">
+        <v>154</v>
+      </c>
+      <c r="B240" s="283" t="s">
+        <v>206</v>
+      </c>
+      <c r="C240" s="283" t="s">
         <v>219</v>
       </c>
-      <c r="D239" s="283" t="s">
-        <v>304</v>
-      </c>
-      <c r="E239" s="286">
-        <v>45748</v>
-      </c>
-      <c r="F239" s="285">
-        <v>0</v>
-      </c>
-      <c r="G239" s="285">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="240" spans="1:7">
-      <c r="A240" s="292">
-        <v>106</v>
-      </c>
-      <c r="B240" s="292" t="s">
-        <v>210</v>
-      </c>
-      <c r="C240" s="292" t="s">
-        <v>214</v>
-      </c>
-      <c r="D240" s="292" t="s">
-        <v>202</v>
-      </c>
-      <c r="E240" s="293">
+      <c r="D240" s="283" t="s">
+        <v>306</v>
+      </c>
+      <c r="E240" s="286">
         <v>45778</v>
       </c>
-      <c r="F240" s="294">
-        <v>260000</v>
-      </c>
-      <c r="G240" s="294">
-        <v>104492.97</v>
+      <c r="F240" s="285">
+        <v>44000</v>
+      </c>
+      <c r="G240" s="285">
+        <v>54238.35</v>
       </c>
     </row>
     <row r="241" spans="1:7">
       <c r="A241" s="283">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B241" s="283" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C241" s="283" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D241" s="283" t="s">
-        <v>306</v>
+        <v>204</v>
       </c>
       <c r="E241" s="286">
         <v>45778</v>
       </c>
       <c r="F241" s="285">
-        <v>44000</v>
+        <v>90000</v>
       </c>
       <c r="G241" s="285">
-        <v>54238.35</v>
+        <v>204514.16</v>
       </c>
     </row>
     <row r="242" spans="1:7">
       <c r="A242" s="283">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="B242" s="283" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="C242" s="283" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="D242" s="283" t="s">
-        <v>204</v>
+        <v>306</v>
       </c>
       <c r="E242" s="286">
         <v>45778</v>
       </c>
       <c r="F242" s="285">
-        <v>90000</v>
+        <v>175000</v>
       </c>
       <c r="G242" s="285">
-        <v>204514.16</v>
+        <v>211010.78999999998</v>
       </c>
     </row>
     <row r="243" spans="1:7">
       <c r="A243" s="283">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B243" s="283" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C243" s="283" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D243" s="283" t="s">
-        <v>306</v>
+        <v>225</v>
       </c>
       <c r="E243" s="286">
         <v>45778</v>
       </c>
       <c r="F243" s="285">
-        <v>175000</v>
+        <v>450000</v>
       </c>
       <c r="G243" s="285">
-        <v>211010.78999999998</v>
+        <v>1044732.9</v>
       </c>
     </row>
     <row r="244" spans="1:7">
       <c r="A244" s="283">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B244" s="283" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C244" s="283" t="s">
         <v>217</v>
@@ -26321,33 +26321,33 @@
         <v>45778</v>
       </c>
       <c r="F244" s="285">
-        <v>450000</v>
+        <v>0</v>
       </c>
       <c r="G244" s="285">
-        <v>1044732.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="245" spans="1:7">
       <c r="A245" s="283">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B245" s="283" t="s">
-        <v>232</v>
+        <v>265</v>
       </c>
       <c r="C245" s="283" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="D245" s="283" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="E245" s="286">
         <v>45778</v>
       </c>
       <c r="F245" s="285">
-        <v>0</v>
+        <v>400000</v>
       </c>
       <c r="G245" s="285">
-        <v>0</v>
+        <v>128994.73</v>
       </c>
     </row>
     <row r="246" spans="1:7">
@@ -26355,7 +26355,7 @@
         <v>184</v>
       </c>
       <c r="B246" s="283" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C246" s="283" t="s">
         <v>230</v>
@@ -26367,41 +26367,41 @@
         <v>45778</v>
       </c>
       <c r="F246" s="285">
-        <v>400000</v>
+        <v>250000</v>
       </c>
       <c r="G246" s="285">
-        <v>128994.73</v>
+        <v>292819.92</v>
       </c>
     </row>
     <row r="247" spans="1:7">
       <c r="A247" s="283">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B247" s="283" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C247" s="283" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D247" s="283" t="s">
-        <v>231</v>
+        <v>306</v>
       </c>
       <c r="E247" s="286">
         <v>45778</v>
       </c>
       <c r="F247" s="285">
-        <v>250000</v>
+        <v>150000</v>
       </c>
       <c r="G247" s="285">
-        <v>292819.92</v>
+        <v>92029.67</v>
       </c>
     </row>
     <row r="248" spans="1:7">
       <c r="A248" s="283">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="B248" s="283" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C248" s="283" t="s">
         <v>219</v>
@@ -26413,44 +26413,44 @@
         <v>45778</v>
       </c>
       <c r="F248" s="285">
-        <v>150000</v>
+        <v>0</v>
       </c>
       <c r="G248" s="285">
-        <v>92029.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="249" spans="1:7">
       <c r="A249" s="283">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B249" s="283" t="s">
-        <v>262</v>
+        <v>283</v>
       </c>
       <c r="C249" s="283" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D249" s="283" t="s">
-        <v>306</v>
+        <v>231</v>
       </c>
       <c r="E249" s="286">
         <v>45778</v>
       </c>
       <c r="F249" s="285">
-        <v>0</v>
+        <v>350000</v>
       </c>
       <c r="G249" s="285">
-        <v>0</v>
+        <v>327098.08</v>
       </c>
     </row>
     <row r="250" spans="1:7">
       <c r="A250" s="283">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="B250" s="283" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="C250" s="283" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D250" s="283" t="s">
         <v>231</v>
@@ -26459,47 +26459,47 @@
         <v>45778</v>
       </c>
       <c r="F250" s="285">
-        <v>350000</v>
+        <v>5000</v>
       </c>
       <c r="G250" s="285">
-        <v>327098.08</v>
+        <v>7295.8399999999992</v>
       </c>
     </row>
     <row r="251" spans="1:7">
       <c r="A251" s="283">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B251" s="283" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="C251" s="283" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D251" s="283" t="s">
-        <v>231</v>
+        <v>299</v>
       </c>
       <c r="E251" s="286">
         <v>45778</v>
       </c>
       <c r="F251" s="285">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="G251" s="285">
-        <v>7295.8399999999992</v>
+        <v>221356.49</v>
       </c>
     </row>
     <row r="252" spans="1:7">
       <c r="A252" s="283">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B252" s="283" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C252" s="283" t="s">
-        <v>216</v>
+        <v>298</v>
       </c>
       <c r="D252" s="283" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E252" s="286">
         <v>45778</v>
@@ -26508,21 +26508,21 @@
         <v>0</v>
       </c>
       <c r="G252" s="285">
-        <v>221356.49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253" spans="1:7">
       <c r="A253" s="283">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B253" s="283" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C253" s="283" t="s">
-        <v>298</v>
+        <v>222</v>
       </c>
       <c r="D253" s="283" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="E253" s="286">
         <v>45778</v>
@@ -26536,13 +26536,13 @@
     </row>
     <row r="254" spans="1:7">
       <c r="A254" s="283">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="B254" s="283" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="C254" s="283" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D254" s="283" t="s">
         <v>306</v>
@@ -26551,156 +26551,156 @@
         <v>45778</v>
       </c>
       <c r="F254" s="285">
-        <v>0</v>
+        <v>106731.25</v>
       </c>
       <c r="G254" s="285">
-        <v>0</v>
+        <v>106731.25</v>
       </c>
     </row>
     <row r="255" spans="1:7">
       <c r="A255" s="283">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B255" s="283" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="C255" s="283" t="s">
         <v>219</v>
       </c>
       <c r="D255" s="283" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E255" s="286">
         <v>45778</v>
       </c>
       <c r="F255" s="285">
-        <v>106731.25</v>
+        <v>0</v>
       </c>
       <c r="G255" s="285">
-        <v>106731.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="256" spans="1:7">
-      <c r="A256" s="283">
-        <v>227</v>
-      </c>
-      <c r="B256" s="283" t="s">
-        <v>303</v>
-      </c>
-      <c r="C256" s="283" t="s">
+      <c r="A256" s="292">
+        <v>106</v>
+      </c>
+      <c r="B256" s="292" t="s">
+        <v>210</v>
+      </c>
+      <c r="C256" s="292" t="s">
+        <v>214</v>
+      </c>
+      <c r="D256" s="292" t="s">
+        <v>202</v>
+      </c>
+      <c r="E256" s="293">
+        <v>45809</v>
+      </c>
+      <c r="F256" s="294">
+        <v>440000</v>
+      </c>
+      <c r="G256" s="294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7">
+      <c r="A257" s="283">
+        <v>154</v>
+      </c>
+      <c r="B257" s="283" t="s">
+        <v>206</v>
+      </c>
+      <c r="C257" s="283" t="s">
         <v>219</v>
       </c>
-      <c r="D256" s="283" t="s">
-        <v>304</v>
-      </c>
-      <c r="E256" s="286">
-        <v>45778</v>
-      </c>
-      <c r="F256" s="285">
-        <v>0</v>
-      </c>
-      <c r="G256" s="285">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="257" spans="1:7">
-      <c r="A257" s="292">
-        <v>106</v>
-      </c>
-      <c r="B257" s="292" t="s">
-        <v>210</v>
-      </c>
-      <c r="C257" s="292" t="s">
-        <v>214</v>
-      </c>
-      <c r="D257" s="292" t="s">
-        <v>202</v>
-      </c>
-      <c r="E257" s="293">
+      <c r="D257" s="283" t="s">
+        <v>306</v>
+      </c>
+      <c r="E257" s="286">
         <v>45809</v>
       </c>
-      <c r="F257" s="294">
-        <v>440000</v>
-      </c>
-      <c r="G257" s="294">
-        <v>0</v>
+      <c r="F257" s="291">
+        <v>130000</v>
+      </c>
+      <c r="G257" s="291">
+        <v>109690.26</v>
       </c>
     </row>
     <row r="258" spans="1:7">
       <c r="A258" s="283">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B258" s="283" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C258" s="283" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D258" s="283" t="s">
-        <v>306</v>
+        <v>204</v>
       </c>
       <c r="E258" s="286">
         <v>45809</v>
       </c>
       <c r="F258" s="291">
-        <v>130000</v>
+        <v>12000</v>
       </c>
       <c r="G258" s="291">
-        <v>109690.26</v>
+        <v>51483.81</v>
       </c>
     </row>
     <row r="259" spans="1:7">
       <c r="A259" s="283">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="B259" s="283" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="C259" s="283" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="D259" s="283" t="s">
-        <v>204</v>
+        <v>306</v>
       </c>
       <c r="E259" s="286">
         <v>45809</v>
       </c>
       <c r="F259" s="291">
-        <v>12000</v>
+        <v>200000</v>
       </c>
       <c r="G259" s="291">
-        <v>51483.81</v>
+        <v>128317.21</v>
       </c>
     </row>
     <row r="260" spans="1:7">
       <c r="A260" s="283">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B260" s="283" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C260" s="283" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D260" s="283" t="s">
-        <v>306</v>
+        <v>225</v>
       </c>
       <c r="E260" s="286">
         <v>45809</v>
       </c>
       <c r="F260" s="291">
-        <v>200000</v>
+        <v>175000</v>
       </c>
       <c r="G260" s="291">
-        <v>128317.21</v>
+        <v>423306.62</v>
       </c>
     </row>
     <row r="261" spans="1:7">
       <c r="A261" s="283">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B261" s="283" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C261" s="283" t="s">
         <v>217</v>
@@ -26712,33 +26712,33 @@
         <v>45809</v>
       </c>
       <c r="F261" s="291">
-        <v>175000</v>
+        <v>120000</v>
       </c>
       <c r="G261" s="291">
-        <v>423306.62</v>
+        <v>142089.04</v>
       </c>
     </row>
     <row r="262" spans="1:7">
       <c r="A262" s="283">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B262" s="283" t="s">
-        <v>232</v>
+        <v>265</v>
       </c>
       <c r="C262" s="283" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="D262" s="283" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="E262" s="286">
         <v>45809</v>
       </c>
       <c r="F262" s="291">
-        <v>120000</v>
+        <v>250000</v>
       </c>
       <c r="G262" s="291">
-        <v>142089.04</v>
+        <v>285642.42</v>
       </c>
     </row>
     <row r="263" spans="1:7">
@@ -26746,7 +26746,7 @@
         <v>184</v>
       </c>
       <c r="B263" s="283" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C263" s="283" t="s">
         <v>230</v>
@@ -26758,41 +26758,41 @@
         <v>45809</v>
       </c>
       <c r="F263" s="291">
-        <v>250000</v>
+        <v>150000</v>
       </c>
       <c r="G263" s="291">
-        <v>285642.42</v>
+        <v>124599.02</v>
       </c>
     </row>
     <row r="264" spans="1:7">
       <c r="A264" s="283">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B264" s="283" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C264" s="283" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D264" s="283" t="s">
-        <v>231</v>
+        <v>306</v>
       </c>
       <c r="E264" s="286">
         <v>45809</v>
       </c>
       <c r="F264" s="291">
-        <v>150000</v>
+        <v>50000</v>
       </c>
       <c r="G264" s="291">
-        <v>124599.02</v>
+        <v>24437.65</v>
       </c>
     </row>
     <row r="265" spans="1:7">
       <c r="A265" s="283">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="B265" s="283" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C265" s="283" t="s">
         <v>219</v>
@@ -26804,44 +26804,44 @@
         <v>45809</v>
       </c>
       <c r="F265" s="291">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="G265" s="291">
-        <v>24437.65</v>
+        <v>30495.67</v>
       </c>
     </row>
     <row r="266" spans="1:7">
       <c r="A266" s="283">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B266" s="283" t="s">
-        <v>262</v>
+        <v>283</v>
       </c>
       <c r="C266" s="283" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D266" s="283" t="s">
-        <v>306</v>
+        <v>231</v>
       </c>
       <c r="E266" s="286">
         <v>45809</v>
       </c>
       <c r="F266" s="291">
-        <v>25000</v>
+        <v>577754</v>
       </c>
       <c r="G266" s="291">
-        <v>30495.67</v>
+        <v>759750.85</v>
       </c>
     </row>
     <row r="267" spans="1:7">
       <c r="A267" s="283">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="B267" s="283" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="C267" s="283" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D267" s="283" t="s">
         <v>231</v>
@@ -26850,90 +26850,90 @@
         <v>45809</v>
       </c>
       <c r="F267" s="291">
-        <v>577754</v>
+        <v>5000</v>
       </c>
       <c r="G267" s="291">
-        <v>759750.85</v>
+        <v>6316.66</v>
       </c>
     </row>
     <row r="268" spans="1:7">
       <c r="A268" s="283">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B268" s="283" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="C268" s="283" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D268" s="283" t="s">
-        <v>231</v>
+        <v>299</v>
       </c>
       <c r="E268" s="286">
         <v>45809</v>
       </c>
       <c r="F268" s="291">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="G268" s="291">
-        <v>6316.66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="269" spans="1:7">
       <c r="A269" s="283">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B269" s="283" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C269" s="283" t="s">
-        <v>216</v>
+        <v>298</v>
       </c>
       <c r="D269" s="283" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E269" s="286">
         <v>45809</v>
       </c>
       <c r="F269" s="291">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="G269" s="291">
-        <v>0</v>
+        <v>549344.87</v>
       </c>
     </row>
     <row r="270" spans="1:7">
       <c r="A270" s="283">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B270" s="283" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C270" s="283" t="s">
-        <v>298</v>
+        <v>222</v>
       </c>
       <c r="D270" s="283" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="E270" s="286">
         <v>45809</v>
       </c>
       <c r="F270" s="291">
-        <v>450000</v>
+        <v>150000</v>
       </c>
       <c r="G270" s="291">
-        <v>549344.87</v>
+        <v>147743.85</v>
       </c>
     </row>
     <row r="271" spans="1:7">
       <c r="A271" s="283">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="B271" s="283" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="C271" s="283" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D271" s="283" t="s">
         <v>306</v>
@@ -26942,171 +26942,171 @@
         <v>45809</v>
       </c>
       <c r="F271" s="291">
-        <v>150000</v>
+        <v>279614</v>
       </c>
       <c r="G271" s="291">
-        <v>147743.85</v>
+        <v>223790.63</v>
       </c>
     </row>
     <row r="272" spans="1:7">
       <c r="A272" s="283">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B272" s="283" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="C272" s="283" t="s">
         <v>219</v>
       </c>
       <c r="D272" s="283" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E272" s="286">
         <v>45809</v>
       </c>
       <c r="F272" s="291">
-        <v>279614</v>
+        <v>80000</v>
       </c>
       <c r="G272" s="291">
-        <v>223790.63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="273" spans="1:7">
-      <c r="A273" s="283">
-        <v>227</v>
-      </c>
-      <c r="B273" s="283" t="s">
-        <v>303</v>
-      </c>
-      <c r="C273" s="283" t="s">
+      <c r="A273" s="292">
+        <v>106</v>
+      </c>
+      <c r="B273" s="292" t="s">
+        <v>210</v>
+      </c>
+      <c r="C273" s="292" t="s">
+        <v>214</v>
+      </c>
+      <c r="D273" s="292" t="s">
+        <v>202</v>
+      </c>
+      <c r="E273" s="293">
+        <v>45839</v>
+      </c>
+      <c r="F273" s="294">
+        <v>0</v>
+      </c>
+      <c r="G273" s="294">
+        <v>187500</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7">
+      <c r="A274" s="283">
+        <v>154</v>
+      </c>
+      <c r="B274" s="283" t="s">
+        <v>206</v>
+      </c>
+      <c r="C274" s="283" t="s">
         <v>219</v>
       </c>
-      <c r="D273" s="283" t="s">
-        <v>304</v>
-      </c>
-      <c r="E273" s="286">
-        <v>45809</v>
-      </c>
-      <c r="F273" s="291">
-        <v>80000</v>
-      </c>
-      <c r="G273" s="291">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="274" spans="1:7">
-      <c r="A274" s="292">
-        <v>106</v>
-      </c>
-      <c r="B274" s="292" t="s">
-        <v>210</v>
-      </c>
-      <c r="C274" s="292" t="s">
-        <v>214</v>
-      </c>
-      <c r="D274" s="292" t="s">
-        <v>202</v>
-      </c>
-      <c r="E274" s="293">
+      <c r="D274" s="283" t="s">
+        <v>306</v>
+      </c>
+      <c r="E274" s="286">
         <v>45839</v>
       </c>
-      <c r="F274" s="294">
-        <v>0</v>
-      </c>
-      <c r="G274" s="294">
-        <v>187500</v>
+      <c r="F274" s="285">
+        <v>0</v>
+      </c>
+      <c r="G274" s="285">
+        <v>0</v>
       </c>
     </row>
     <row r="275" spans="1:7">
       <c r="A275" s="283">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B275" s="283" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C275" s="283" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D275" s="283" t="s">
-        <v>306</v>
+        <v>204</v>
       </c>
       <c r="E275" s="286">
         <v>45839</v>
       </c>
       <c r="F275" s="285">
-        <v>0</v>
+        <v>620000</v>
       </c>
       <c r="G275" s="285">
-        <v>0</v>
+        <v>181750.65</v>
       </c>
     </row>
     <row r="276" spans="1:7">
       <c r="A276" s="283">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="B276" s="283" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="C276" s="283" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="D276" s="283" t="s">
-        <v>204</v>
+        <v>306</v>
       </c>
       <c r="E276" s="286">
         <v>45839</v>
       </c>
       <c r="F276" s="285">
-        <v>620000</v>
-      </c>
-      <c r="G276" s="285">
-        <v>181750.65</v>
+        <v>226000</v>
+      </c>
+      <c r="G276" s="294">
+        <v>100000</v>
       </c>
     </row>
     <row r="277" spans="1:7">
       <c r="A277" s="283">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="B277" s="283" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C277" s="283" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D277" s="283" t="s">
-        <v>306</v>
+        <v>225</v>
       </c>
       <c r="E277" s="286">
         <v>45839</v>
       </c>
       <c r="F277" s="285">
-        <v>226000</v>
-      </c>
-      <c r="G277" s="294">
-        <v>100000</v>
+        <v>60000</v>
+      </c>
+      <c r="G277" s="285">
+        <v>0</v>
       </c>
     </row>
     <row r="278" spans="1:7">
       <c r="A278" s="283">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B278" s="283" t="s">
-        <v>232</v>
+        <v>265</v>
       </c>
       <c r="C278" s="283" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="D278" s="283" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="E278" s="286">
         <v>45839</v>
       </c>
       <c r="F278" s="285">
-        <v>60000</v>
+        <v>850000</v>
       </c>
       <c r="G278" s="285">
-        <v>0</v>
+        <v>476000.15</v>
       </c>
     </row>
     <row r="279" spans="1:7">
@@ -27114,7 +27114,7 @@
         <v>184</v>
       </c>
       <c r="B279" s="283" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C279" s="283" t="s">
         <v>230</v>
@@ -27126,41 +27126,41 @@
         <v>45839</v>
       </c>
       <c r="F279" s="285">
-        <v>850000</v>
+        <v>540000</v>
       </c>
       <c r="G279" s="285">
-        <v>476000.15</v>
+        <v>187298.03</v>
       </c>
     </row>
     <row r="280" spans="1:7">
       <c r="A280" s="283">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B280" s="283" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C280" s="283" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D280" s="283" t="s">
-        <v>231</v>
+        <v>306</v>
       </c>
       <c r="E280" s="286">
         <v>45839</v>
       </c>
       <c r="F280" s="285">
-        <v>540000</v>
+        <v>35000</v>
       </c>
       <c r="G280" s="285">
-        <v>187298.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="281" spans="1:7">
       <c r="A281" s="283">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="B281" s="283" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C281" s="283" t="s">
         <v>219</v>
@@ -27172,7 +27172,7 @@
         <v>45839</v>
       </c>
       <c r="F281" s="285">
-        <v>35000</v>
+        <v>135000</v>
       </c>
       <c r="G281" s="285">
         <v>0</v>
@@ -27180,36 +27180,36 @@
     </row>
     <row r="282" spans="1:7">
       <c r="A282" s="283">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B282" s="283" t="s">
-        <v>262</v>
+        <v>283</v>
       </c>
       <c r="C282" s="283" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D282" s="283" t="s">
-        <v>306</v>
+        <v>231</v>
       </c>
       <c r="E282" s="286">
         <v>45839</v>
       </c>
       <c r="F282" s="285">
-        <v>135000</v>
+        <v>650000</v>
       </c>
       <c r="G282" s="285">
-        <v>0</v>
+        <v>481341.82</v>
       </c>
     </row>
     <row r="283" spans="1:7">
       <c r="A283" s="283">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="B283" s="283" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="C283" s="283" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D283" s="283" t="s">
         <v>231</v>
@@ -27218,76 +27218,76 @@
         <v>45839</v>
       </c>
       <c r="F283" s="285">
-        <v>650000</v>
+        <v>6000</v>
       </c>
       <c r="G283" s="285">
-        <v>481341.82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="284" spans="1:7">
       <c r="A284" s="283">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B284" s="283" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="C284" s="283" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D284" s="283" t="s">
-        <v>231</v>
+        <v>299</v>
       </c>
       <c r="E284" s="286">
         <v>45839</v>
       </c>
       <c r="F284" s="285">
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="G284" s="285">
-        <v>0</v>
+        <v>11623.23</v>
       </c>
     </row>
     <row r="285" spans="1:7">
       <c r="A285" s="283">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B285" s="283" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C285" s="283" t="s">
-        <v>216</v>
+        <v>298</v>
       </c>
       <c r="D285" s="283" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E285" s="286">
         <v>45839</v>
       </c>
       <c r="F285" s="285">
-        <v>0</v>
+        <v>350000</v>
       </c>
       <c r="G285" s="285">
-        <v>11623.23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="286" spans="1:7">
       <c r="A286" s="283">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B286" s="283" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C286" s="283" t="s">
-        <v>298</v>
+        <v>222</v>
       </c>
       <c r="D286" s="283" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="E286" s="286">
         <v>45839</v>
       </c>
       <c r="F286" s="285">
-        <v>350000</v>
+        <v>150000</v>
       </c>
       <c r="G286" s="285">
         <v>0</v>
@@ -27295,13 +27295,13 @@
     </row>
     <row r="287" spans="1:7">
       <c r="A287" s="283">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="B287" s="283" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="C287" s="283" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D287" s="283" t="s">
         <v>306</v>
@@ -27310,7 +27310,7 @@
         <v>45839</v>
       </c>
       <c r="F287" s="285">
-        <v>150000</v>
+        <v>0</v>
       </c>
       <c r="G287" s="285">
         <v>0</v>
@@ -27318,47 +27318,24 @@
     </row>
     <row r="288" spans="1:7">
       <c r="A288" s="283">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B288" s="283" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="C288" s="283" t="s">
         <v>219</v>
       </c>
       <c r="D288" s="283" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E288" s="286">
         <v>45839</v>
       </c>
       <c r="F288" s="285">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="G288" s="285">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="289" spans="1:7">
-      <c r="A289" s="283">
-        <v>227</v>
-      </c>
-      <c r="B289" s="283" t="s">
-        <v>303</v>
-      </c>
-      <c r="C289" s="283" t="s">
-        <v>219</v>
-      </c>
-      <c r="D289" s="283" t="s">
-        <v>304</v>
-      </c>
-      <c r="E289" s="286">
-        <v>45839</v>
-      </c>
-      <c r="F289" s="285">
-        <v>80000</v>
-      </c>
-      <c r="G289" s="285">
         <v>0</v>
       </c>
     </row>
@@ -27374,7 +27351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF7C2BA-F766-47EF-8569-EB2756BF213B}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Atualização 07/08/25 - 3
</commit_message>
<xml_diff>
--- a/1 - Acompanhamento Medições.xlsx
+++ b/1 - Acompanhamento Medições.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://brpucrs-my.sharepoint.com/personal/raphael_leitao_edu_pucrs_br/Documents/Python/Aplicativo de Acompanhamento de Medições/Acomp-de-Medicoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="642" documentId="13_ncr:1_{A1421A19-0108-4133-B863-EAC0C5A9202F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{395A55F1-A280-4CEF-979A-59ED2FE107D0}"/>
+  <xr:revisionPtr revIDLastSave="650" documentId="13_ncr:1_{A1421A19-0108-4133-B863-EAC0C5A9202F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{834DA8D0-B10C-4FA8-B978-01E4BB813E24}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="604" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="604" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RESUMO-2024" sheetId="11" r:id="rId1"/>
@@ -6342,24 +6342,54 @@
     <xf numFmtId="44" fontId="127" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="118" fillId="85" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="72" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="73" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="118" fillId="85" borderId="75" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="80" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="118" fillId="85" borderId="83" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="118" fillId="85" borderId="84" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="83" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="118" fillId="85" borderId="85" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6369,49 +6399,19 @@
     <xf numFmtId="44" fontId="113" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="73" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="111" fillId="86" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="111" fillId="86" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="72" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="111" fillId="86" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="118" fillId="85" borderId="80" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="111" fillId="86" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="113" fillId="5" borderId="84" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -9630,55 +9630,55 @@
       </c>
       <c r="C1" s="157"/>
       <c r="D1" s="157"/>
-      <c r="E1" s="310"/>
-      <c r="F1" s="310"/>
-      <c r="G1" s="310"/>
-      <c r="H1" s="310"/>
-      <c r="I1" s="310"/>
-      <c r="J1" s="310"/>
-      <c r="K1" s="310"/>
-      <c r="L1" s="310"/>
-      <c r="M1" s="310"/>
-      <c r="N1" s="310"/>
-      <c r="O1" s="311"/>
-      <c r="P1" s="310"/>
-      <c r="Q1" s="310"/>
-      <c r="R1" s="310"/>
-      <c r="S1" s="310"/>
-      <c r="T1" s="310"/>
-      <c r="U1" s="310"/>
-      <c r="V1" s="310"/>
-      <c r="W1" s="310"/>
-      <c r="X1" s="310"/>
-      <c r="Y1" s="310"/>
-      <c r="Z1" s="310"/>
-      <c r="AA1" s="310"/>
-      <c r="AB1" s="310"/>
-      <c r="AC1" s="310"/>
-      <c r="AD1" s="310"/>
-      <c r="AE1" s="310"/>
-      <c r="AF1" s="310"/>
-      <c r="AG1" s="310"/>
-      <c r="AH1" s="310"/>
-      <c r="AI1" s="310"/>
-      <c r="AJ1" s="310"/>
-      <c r="AK1" s="310"/>
-      <c r="AL1" s="310"/>
-      <c r="AM1" s="310"/>
-      <c r="AN1" s="310"/>
-      <c r="AO1" s="310"/>
-      <c r="AP1" s="310"/>
-      <c r="AQ1" s="310"/>
-      <c r="AR1" s="310"/>
-      <c r="AS1" s="310"/>
-      <c r="AT1" s="310"/>
-      <c r="AU1" s="310"/>
-      <c r="AV1" s="310"/>
-      <c r="AW1" s="310"/>
-      <c r="AX1" s="310"/>
-      <c r="AY1" s="310"/>
-      <c r="AZ1" s="310"/>
-      <c r="BA1" s="310"/>
+      <c r="E1" s="314"/>
+      <c r="F1" s="314"/>
+      <c r="G1" s="314"/>
+      <c r="H1" s="314"/>
+      <c r="I1" s="314"/>
+      <c r="J1" s="314"/>
+      <c r="K1" s="314"/>
+      <c r="L1" s="314"/>
+      <c r="M1" s="314"/>
+      <c r="N1" s="314"/>
+      <c r="O1" s="315"/>
+      <c r="P1" s="314"/>
+      <c r="Q1" s="314"/>
+      <c r="R1" s="314"/>
+      <c r="S1" s="314"/>
+      <c r="T1" s="314"/>
+      <c r="U1" s="314"/>
+      <c r="V1" s="314"/>
+      <c r="W1" s="314"/>
+      <c r="X1" s="314"/>
+      <c r="Y1" s="314"/>
+      <c r="Z1" s="314"/>
+      <c r="AA1" s="314"/>
+      <c r="AB1" s="314"/>
+      <c r="AC1" s="314"/>
+      <c r="AD1" s="314"/>
+      <c r="AE1" s="314"/>
+      <c r="AF1" s="314"/>
+      <c r="AG1" s="314"/>
+      <c r="AH1" s="314"/>
+      <c r="AI1" s="314"/>
+      <c r="AJ1" s="314"/>
+      <c r="AK1" s="314"/>
+      <c r="AL1" s="314"/>
+      <c r="AM1" s="314"/>
+      <c r="AN1" s="314"/>
+      <c r="AO1" s="314"/>
+      <c r="AP1" s="314"/>
+      <c r="AQ1" s="314"/>
+      <c r="AR1" s="314"/>
+      <c r="AS1" s="314"/>
+      <c r="AT1" s="314"/>
+      <c r="AU1" s="314"/>
+      <c r="AV1" s="314"/>
+      <c r="AW1" s="314"/>
+      <c r="AX1" s="314"/>
+      <c r="AY1" s="314"/>
+      <c r="AZ1" s="314"/>
+      <c r="BA1" s="314"/>
     </row>
     <row r="2" spans="1:53" ht="18.600000000000001">
       <c r="A2" s="151"/>
@@ -9717,99 +9717,99 @@
       <c r="AC3" s="201"/>
     </row>
     <row r="4" spans="1:53" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A4" s="313" t="s">
+      <c r="A4" s="303" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="315" t="s">
+      <c r="B4" s="305" t="s">
         <v>234</v>
       </c>
-      <c r="C4" s="315" t="s">
+      <c r="C4" s="305" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="317" t="s">
+      <c r="D4" s="307" t="s">
         <v>236</v>
       </c>
-      <c r="E4" s="309" t="s">
+      <c r="E4" s="317" t="s">
         <v>250</v>
       </c>
-      <c r="F4" s="306"/>
-      <c r="G4" s="306"/>
-      <c r="H4" s="307"/>
-      <c r="I4" s="306" t="s">
+      <c r="F4" s="316"/>
+      <c r="G4" s="316"/>
+      <c r="H4" s="318"/>
+      <c r="I4" s="316" t="s">
         <v>249</v>
       </c>
-      <c r="J4" s="306"/>
-      <c r="K4" s="306"/>
-      <c r="L4" s="306"/>
-      <c r="M4" s="309" t="s">
+      <c r="J4" s="316"/>
+      <c r="K4" s="316"/>
+      <c r="L4" s="316"/>
+      <c r="M4" s="317" t="s">
         <v>251</v>
       </c>
-      <c r="N4" s="306"/>
-      <c r="O4" s="306"/>
-      <c r="P4" s="307"/>
-      <c r="Q4" s="309" t="s">
+      <c r="N4" s="316"/>
+      <c r="O4" s="316"/>
+      <c r="P4" s="318"/>
+      <c r="Q4" s="317" t="s">
         <v>256</v>
       </c>
-      <c r="R4" s="306"/>
-      <c r="S4" s="306"/>
-      <c r="T4" s="307"/>
-      <c r="U4" s="306" t="s">
+      <c r="R4" s="316"/>
+      <c r="S4" s="316"/>
+      <c r="T4" s="318"/>
+      <c r="U4" s="316" t="s">
         <v>257</v>
       </c>
-      <c r="V4" s="306"/>
-      <c r="W4" s="306"/>
-      <c r="X4" s="306"/>
-      <c r="Y4" s="309" t="s">
+      <c r="V4" s="316"/>
+      <c r="W4" s="316"/>
+      <c r="X4" s="316"/>
+      <c r="Y4" s="317" t="s">
         <v>258</v>
       </c>
-      <c r="Z4" s="306"/>
-      <c r="AA4" s="306"/>
-      <c r="AB4" s="307"/>
-      <c r="AC4" s="309" t="s">
+      <c r="Z4" s="316"/>
+      <c r="AA4" s="316"/>
+      <c r="AB4" s="318"/>
+      <c r="AC4" s="317" t="s">
         <v>260</v>
       </c>
-      <c r="AD4" s="306"/>
-      <c r="AE4" s="306"/>
-      <c r="AF4" s="307"/>
-      <c r="AG4" s="309" t="s">
+      <c r="AD4" s="316"/>
+      <c r="AE4" s="316"/>
+      <c r="AF4" s="318"/>
+      <c r="AG4" s="317" t="s">
         <v>261</v>
       </c>
-      <c r="AH4" s="306"/>
-      <c r="AI4" s="306"/>
-      <c r="AJ4" s="307"/>
-      <c r="AK4" s="309" t="s">
+      <c r="AH4" s="316"/>
+      <c r="AI4" s="316"/>
+      <c r="AJ4" s="318"/>
+      <c r="AK4" s="317" t="s">
         <v>237</v>
       </c>
-      <c r="AL4" s="306"/>
-      <c r="AM4" s="306"/>
-      <c r="AN4" s="307"/>
-      <c r="AO4" s="306" t="s">
+      <c r="AL4" s="316"/>
+      <c r="AM4" s="316"/>
+      <c r="AN4" s="318"/>
+      <c r="AO4" s="316" t="s">
         <v>238</v>
       </c>
-      <c r="AP4" s="306"/>
-      <c r="AQ4" s="306"/>
-      <c r="AR4" s="307"/>
-      <c r="AS4" s="309" t="s">
+      <c r="AP4" s="316"/>
+      <c r="AQ4" s="316"/>
+      <c r="AR4" s="318"/>
+      <c r="AS4" s="317" t="s">
         <v>239</v>
       </c>
-      <c r="AT4" s="306"/>
-      <c r="AU4" s="306"/>
-      <c r="AV4" s="307"/>
-      <c r="AW4" s="309" t="s">
+      <c r="AT4" s="316"/>
+      <c r="AU4" s="316"/>
+      <c r="AV4" s="318"/>
+      <c r="AW4" s="317" t="s">
         <v>240</v>
       </c>
-      <c r="AX4" s="306"/>
-      <c r="AY4" s="306"/>
-      <c r="AZ4" s="307"/>
+      <c r="AX4" s="316"/>
+      <c r="AY4" s="316"/>
+      <c r="AZ4" s="318"/>
       <c r="BA4" s="220" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:53" s="145" customFormat="1" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A5" s="314"/>
-      <c r="B5" s="316"/>
-      <c r="C5" s="316"/>
-      <c r="D5" s="318"/>
+      <c r="A5" s="304"/>
+      <c r="B5" s="306"/>
+      <c r="C5" s="306"/>
+      <c r="D5" s="308"/>
       <c r="E5" s="172" t="s">
         <v>246</v>
       </c>
@@ -10046,54 +10046,54 @@
       <c r="AB6" s="217">
         <v>0</v>
       </c>
-      <c r="AC6" s="308" t="s">
+      <c r="AC6" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AD6" s="304"/>
-      <c r="AE6" s="304" t="s">
+      <c r="AD6" s="298"/>
+      <c r="AE6" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="AF6" s="305"/>
-      <c r="AG6" s="308" t="s">
+      <c r="AF6" s="300"/>
+      <c r="AG6" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AH6" s="304"/>
-      <c r="AI6" s="304" t="s">
+      <c r="AH6" s="298"/>
+      <c r="AI6" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="AJ6" s="305"/>
-      <c r="AK6" s="308" t="s">
+      <c r="AJ6" s="300"/>
+      <c r="AK6" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AL6" s="304"/>
-      <c r="AM6" s="304" t="s">
+      <c r="AL6" s="298"/>
+      <c r="AM6" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="AN6" s="305"/>
-      <c r="AO6" s="308" t="s">
+      <c r="AN6" s="300"/>
+      <c r="AO6" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AP6" s="304"/>
-      <c r="AQ6" s="304" t="s">
+      <c r="AP6" s="298"/>
+      <c r="AQ6" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="AR6" s="305"/>
-      <c r="AS6" s="308" t="s">
+      <c r="AR6" s="300"/>
+      <c r="AS6" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AT6" s="304"/>
-      <c r="AU6" s="304" t="s">
+      <c r="AT6" s="298"/>
+      <c r="AU6" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="AV6" s="305"/>
-      <c r="AW6" s="308" t="s">
+      <c r="AV6" s="300"/>
+      <c r="AW6" s="297" t="s">
         <v>233</v>
       </c>
-      <c r="AX6" s="304"/>
-      <c r="AY6" s="304" t="s">
+      <c r="AX6" s="298"/>
+      <c r="AY6" s="298" t="s">
         <v>233</v>
       </c>
-      <c r="AZ6" s="305"/>
+      <c r="AZ6" s="300"/>
       <c r="BA6" s="256">
         <f>AX6+AT6+AP6+AL6+AH6+AD6+Z6+V6+R6+N6+J6+F6</f>
         <v>1928583.53</v>
@@ -10186,54 +10186,54 @@
       <c r="AB7" s="209">
         <v>0</v>
       </c>
-      <c r="AC7" s="297" t="s">
+      <c r="AC7" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AD7" s="295"/>
-      <c r="AE7" s="295" t="s">
+      <c r="AD7" s="296"/>
+      <c r="AE7" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AF7" s="296"/>
-      <c r="AG7" s="297" t="s">
+      <c r="AF7" s="299"/>
+      <c r="AG7" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AH7" s="295"/>
-      <c r="AI7" s="295" t="s">
+      <c r="AH7" s="296"/>
+      <c r="AI7" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AJ7" s="296"/>
-      <c r="AK7" s="297" t="s">
+      <c r="AJ7" s="299"/>
+      <c r="AK7" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AL7" s="295"/>
-      <c r="AM7" s="295" t="s">
+      <c r="AL7" s="296"/>
+      <c r="AM7" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AN7" s="296"/>
-      <c r="AO7" s="297" t="s">
+      <c r="AN7" s="299"/>
+      <c r="AO7" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AP7" s="295"/>
-      <c r="AQ7" s="295" t="s">
+      <c r="AP7" s="296"/>
+      <c r="AQ7" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AR7" s="296"/>
-      <c r="AS7" s="297" t="s">
+      <c r="AR7" s="299"/>
+      <c r="AS7" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AT7" s="295"/>
-      <c r="AU7" s="295" t="s">
+      <c r="AT7" s="296"/>
+      <c r="AU7" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AV7" s="296"/>
-      <c r="AW7" s="297" t="s">
+      <c r="AV7" s="299"/>
+      <c r="AW7" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AX7" s="295"/>
-      <c r="AY7" s="295" t="s">
+      <c r="AX7" s="296"/>
+      <c r="AY7" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AZ7" s="296"/>
+      <c r="AZ7" s="299"/>
       <c r="BA7" s="257">
         <f t="shared" ref="BA7:BA31" si="0">AX7+AT7+AP7+AL7+AH7+AD7+Z7+V7+R7+N7+J7+F7</f>
         <v>1513239.29</v>
@@ -10514,38 +10514,38 @@
       <c r="AJ9" s="209">
         <v>0</v>
       </c>
-      <c r="AK9" s="297" t="s">
+      <c r="AK9" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AL9" s="295"/>
-      <c r="AM9" s="295" t="s">
+      <c r="AL9" s="296"/>
+      <c r="AM9" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AN9" s="296"/>
-      <c r="AO9" s="297" t="s">
+      <c r="AN9" s="299"/>
+      <c r="AO9" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AP9" s="295"/>
-      <c r="AQ9" s="295" t="s">
+      <c r="AP9" s="296"/>
+      <c r="AQ9" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AR9" s="296"/>
-      <c r="AS9" s="297" t="s">
+      <c r="AR9" s="299"/>
+      <c r="AS9" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AT9" s="295"/>
-      <c r="AU9" s="295" t="s">
+      <c r="AT9" s="296"/>
+      <c r="AU9" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AV9" s="296"/>
-      <c r="AW9" s="297" t="s">
+      <c r="AV9" s="299"/>
+      <c r="AW9" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AX9" s="295"/>
-      <c r="AY9" s="295" t="s">
+      <c r="AX9" s="296"/>
+      <c r="AY9" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AZ9" s="296"/>
+      <c r="AZ9" s="299"/>
       <c r="BA9" s="257">
         <f t="shared" si="0"/>
         <v>137879.14000000001</v>
@@ -10659,36 +10659,36 @@
       <c r="AJ10" s="209">
         <v>0</v>
       </c>
-      <c r="AK10" s="302" t="s">
+      <c r="AK10" s="312" t="s">
         <v>266</v>
       </c>
-      <c r="AL10" s="303"/>
+      <c r="AL10" s="313"/>
       <c r="AM10" s="184"/>
       <c r="AN10" s="208"/>
-      <c r="AO10" s="302" t="s">
+      <c r="AO10" s="312" t="s">
         <v>266</v>
       </c>
-      <c r="AP10" s="303"/>
+      <c r="AP10" s="313"/>
       <c r="AQ10" s="180">
         <v>0</v>
       </c>
       <c r="AR10" s="211">
         <v>0</v>
       </c>
-      <c r="AS10" s="302" t="s">
+      <c r="AS10" s="312" t="s">
         <v>266</v>
       </c>
-      <c r="AT10" s="303"/>
+      <c r="AT10" s="313"/>
       <c r="AU10" s="180">
         <v>0</v>
       </c>
       <c r="AV10" s="209">
         <v>0</v>
       </c>
-      <c r="AW10" s="302" t="s">
+      <c r="AW10" s="312" t="s">
         <v>266</v>
       </c>
-      <c r="AX10" s="303"/>
+      <c r="AX10" s="313"/>
       <c r="AY10" s="180">
         <v>0</v>
       </c>
@@ -11095,62 +11095,62 @@
       <c r="X13" s="209">
         <v>0</v>
       </c>
-      <c r="Y13" s="297" t="s">
+      <c r="Y13" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="Z13" s="295"/>
-      <c r="AA13" s="295" t="s">
+      <c r="Z13" s="296"/>
+      <c r="AA13" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AB13" s="296"/>
-      <c r="AC13" s="297" t="s">
+      <c r="AB13" s="299"/>
+      <c r="AC13" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AD13" s="295"/>
-      <c r="AE13" s="295" t="s">
+      <c r="AD13" s="296"/>
+      <c r="AE13" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AF13" s="296"/>
-      <c r="AG13" s="297" t="s">
+      <c r="AF13" s="299"/>
+      <c r="AG13" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AH13" s="295"/>
-      <c r="AI13" s="295" t="s">
+      <c r="AH13" s="296"/>
+      <c r="AI13" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AJ13" s="296"/>
-      <c r="AK13" s="297" t="s">
+      <c r="AJ13" s="299"/>
+      <c r="AK13" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AL13" s="295"/>
-      <c r="AM13" s="295" t="s">
+      <c r="AL13" s="296"/>
+      <c r="AM13" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AN13" s="296"/>
-      <c r="AO13" s="297" t="s">
+      <c r="AN13" s="299"/>
+      <c r="AO13" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AP13" s="295"/>
-      <c r="AQ13" s="295" t="s">
+      <c r="AP13" s="296"/>
+      <c r="AQ13" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AR13" s="296"/>
-      <c r="AS13" s="297" t="s">
+      <c r="AR13" s="299"/>
+      <c r="AS13" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AT13" s="295"/>
-      <c r="AU13" s="295" t="s">
+      <c r="AT13" s="296"/>
+      <c r="AU13" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AV13" s="296"/>
-      <c r="AW13" s="297" t="s">
+      <c r="AV13" s="299"/>
+      <c r="AW13" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AX13" s="295"/>
-      <c r="AY13" s="295" t="s">
+      <c r="AX13" s="296"/>
+      <c r="AY13" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AZ13" s="296"/>
+      <c r="AZ13" s="299"/>
       <c r="BA13" s="257">
         <f t="shared" si="0"/>
         <v>3541.48</v>
@@ -11227,62 +11227,62 @@
       <c r="X14" s="209">
         <v>0</v>
       </c>
-      <c r="Y14" s="297" t="s">
+      <c r="Y14" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="Z14" s="295"/>
-      <c r="AA14" s="295" t="s">
+      <c r="Z14" s="296"/>
+      <c r="AA14" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AB14" s="296"/>
-      <c r="AC14" s="297" t="s">
+      <c r="AB14" s="299"/>
+      <c r="AC14" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AD14" s="295"/>
-      <c r="AE14" s="295" t="s">
+      <c r="AD14" s="296"/>
+      <c r="AE14" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AF14" s="296"/>
-      <c r="AG14" s="297" t="s">
+      <c r="AF14" s="299"/>
+      <c r="AG14" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AH14" s="295"/>
-      <c r="AI14" s="295" t="s">
+      <c r="AH14" s="296"/>
+      <c r="AI14" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AJ14" s="296"/>
-      <c r="AK14" s="297" t="s">
+      <c r="AJ14" s="299"/>
+      <c r="AK14" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AL14" s="295"/>
-      <c r="AM14" s="295" t="s">
+      <c r="AL14" s="296"/>
+      <c r="AM14" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AN14" s="296"/>
-      <c r="AO14" s="297" t="s">
+      <c r="AN14" s="299"/>
+      <c r="AO14" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AP14" s="295"/>
-      <c r="AQ14" s="295" t="s">
+      <c r="AP14" s="296"/>
+      <c r="AQ14" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AR14" s="296"/>
-      <c r="AS14" s="297" t="s">
+      <c r="AR14" s="299"/>
+      <c r="AS14" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AT14" s="295"/>
-      <c r="AU14" s="295" t="s">
+      <c r="AT14" s="296"/>
+      <c r="AU14" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AV14" s="296"/>
-      <c r="AW14" s="297" t="s">
+      <c r="AV14" s="299"/>
+      <c r="AW14" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AX14" s="295"/>
-      <c r="AY14" s="295" t="s">
+      <c r="AX14" s="296"/>
+      <c r="AY14" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AZ14" s="296"/>
+      <c r="AZ14" s="299"/>
       <c r="BA14" s="257">
         <f t="shared" si="0"/>
         <v>58229.89</v>
@@ -11361,62 +11361,62 @@
       <c r="X15" s="209">
         <v>0</v>
       </c>
-      <c r="Y15" s="297" t="s">
+      <c r="Y15" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="Z15" s="295"/>
-      <c r="AA15" s="295" t="s">
+      <c r="Z15" s="296"/>
+      <c r="AA15" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AB15" s="296"/>
-      <c r="AC15" s="297" t="s">
+      <c r="AB15" s="299"/>
+      <c r="AC15" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AD15" s="295"/>
-      <c r="AE15" s="295" t="s">
+      <c r="AD15" s="296"/>
+      <c r="AE15" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AF15" s="296"/>
-      <c r="AG15" s="297" t="s">
+      <c r="AF15" s="299"/>
+      <c r="AG15" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AH15" s="295"/>
-      <c r="AI15" s="295" t="s">
+      <c r="AH15" s="296"/>
+      <c r="AI15" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AJ15" s="296"/>
-      <c r="AK15" s="297" t="s">
+      <c r="AJ15" s="299"/>
+      <c r="AK15" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AL15" s="295"/>
-      <c r="AM15" s="295" t="s">
+      <c r="AL15" s="296"/>
+      <c r="AM15" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AN15" s="296"/>
-      <c r="AO15" s="297" t="s">
+      <c r="AN15" s="299"/>
+      <c r="AO15" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AP15" s="295"/>
-      <c r="AQ15" s="295" t="s">
+      <c r="AP15" s="296"/>
+      <c r="AQ15" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AR15" s="296"/>
-      <c r="AS15" s="297" t="s">
+      <c r="AR15" s="299"/>
+      <c r="AS15" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AT15" s="295"/>
-      <c r="AU15" s="295" t="s">
+      <c r="AT15" s="296"/>
+      <c r="AU15" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AV15" s="296"/>
-      <c r="AW15" s="297" t="s">
+      <c r="AV15" s="299"/>
+      <c r="AW15" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AX15" s="295"/>
-      <c r="AY15" s="295" t="s">
+      <c r="AX15" s="296"/>
+      <c r="AY15" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AZ15" s="296"/>
+      <c r="AZ15" s="299"/>
       <c r="BA15" s="257">
         <f t="shared" si="0"/>
         <v>130564.39</v>
@@ -11780,86 +11780,86 @@
       <c r="L18" s="204">
         <v>0</v>
       </c>
-      <c r="M18" s="300" t="s">
+      <c r="M18" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="N18" s="299"/>
-      <c r="O18" s="300" t="s">
+      <c r="N18" s="309"/>
+      <c r="O18" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="P18" s="299"/>
-      <c r="Q18" s="300" t="s">
+      <c r="P18" s="309"/>
+      <c r="Q18" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="R18" s="299"/>
-      <c r="S18" s="300" t="s">
+      <c r="R18" s="309"/>
+      <c r="S18" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="T18" s="312"/>
-      <c r="U18" s="297" t="s">
+      <c r="T18" s="302"/>
+      <c r="U18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="V18" s="295"/>
-      <c r="W18" s="295" t="s">
+      <c r="V18" s="296"/>
+      <c r="W18" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="X18" s="296"/>
-      <c r="Y18" s="297" t="s">
+      <c r="X18" s="299"/>
+      <c r="Y18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="Z18" s="295"/>
-      <c r="AA18" s="295" t="s">
+      <c r="Z18" s="296"/>
+      <c r="AA18" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AB18" s="296"/>
-      <c r="AC18" s="297" t="s">
+      <c r="AB18" s="299"/>
+      <c r="AC18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AD18" s="295"/>
-      <c r="AE18" s="295" t="s">
+      <c r="AD18" s="296"/>
+      <c r="AE18" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AF18" s="296"/>
-      <c r="AG18" s="297" t="s">
+      <c r="AF18" s="299"/>
+      <c r="AG18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AH18" s="295"/>
-      <c r="AI18" s="295" t="s">
+      <c r="AH18" s="296"/>
+      <c r="AI18" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AJ18" s="296"/>
-      <c r="AK18" s="297" t="s">
+      <c r="AJ18" s="299"/>
+      <c r="AK18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AL18" s="295"/>
-      <c r="AM18" s="295" t="s">
+      <c r="AL18" s="296"/>
+      <c r="AM18" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AN18" s="296"/>
-      <c r="AO18" s="297" t="s">
+      <c r="AN18" s="299"/>
+      <c r="AO18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AP18" s="295"/>
-      <c r="AQ18" s="295" t="s">
+      <c r="AP18" s="296"/>
+      <c r="AQ18" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AR18" s="296"/>
-      <c r="AS18" s="297" t="s">
+      <c r="AR18" s="299"/>
+      <c r="AS18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AT18" s="295"/>
-      <c r="AU18" s="295" t="s">
+      <c r="AT18" s="296"/>
+      <c r="AU18" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AV18" s="296"/>
-      <c r="AW18" s="297" t="s">
+      <c r="AV18" s="299"/>
+      <c r="AW18" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AX18" s="295"/>
-      <c r="AY18" s="295" t="s">
+      <c r="AX18" s="296"/>
+      <c r="AY18" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AZ18" s="296"/>
+      <c r="AZ18" s="299"/>
       <c r="BA18" s="257">
         <f t="shared" si="0"/>
         <v>141707.61000000002</v>
@@ -11890,94 +11890,94 @@
       <c r="H19" s="214">
         <v>0</v>
       </c>
-      <c r="I19" s="297" t="s">
+      <c r="I19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="J19" s="295"/>
-      <c r="K19" s="295" t="s">
+      <c r="J19" s="296"/>
+      <c r="K19" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="L19" s="295"/>
-      <c r="M19" s="300" t="s">
+      <c r="L19" s="296"/>
+      <c r="M19" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="N19" s="299"/>
-      <c r="O19" s="300" t="s">
+      <c r="N19" s="309"/>
+      <c r="O19" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="P19" s="299"/>
-      <c r="Q19" s="300" t="s">
+      <c r="P19" s="309"/>
+      <c r="Q19" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="R19" s="299"/>
-      <c r="S19" s="300" t="s">
+      <c r="R19" s="309"/>
+      <c r="S19" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="T19" s="312"/>
-      <c r="U19" s="297" t="s">
+      <c r="T19" s="302"/>
+      <c r="U19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="V19" s="295"/>
-      <c r="W19" s="295" t="s">
+      <c r="V19" s="296"/>
+      <c r="W19" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="X19" s="296"/>
-      <c r="Y19" s="297" t="s">
+      <c r="X19" s="299"/>
+      <c r="Y19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="Z19" s="295"/>
-      <c r="AA19" s="295" t="s">
+      <c r="Z19" s="296"/>
+      <c r="AA19" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AB19" s="296"/>
-      <c r="AC19" s="297" t="s">
+      <c r="AB19" s="299"/>
+      <c r="AC19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AD19" s="295"/>
-      <c r="AE19" s="295" t="s">
+      <c r="AD19" s="296"/>
+      <c r="AE19" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AF19" s="296"/>
-      <c r="AG19" s="297" t="s">
+      <c r="AF19" s="299"/>
+      <c r="AG19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AH19" s="295"/>
-      <c r="AI19" s="295" t="s">
+      <c r="AH19" s="296"/>
+      <c r="AI19" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AJ19" s="296"/>
-      <c r="AK19" s="297" t="s">
+      <c r="AJ19" s="299"/>
+      <c r="AK19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AL19" s="295"/>
-      <c r="AM19" s="295" t="s">
+      <c r="AL19" s="296"/>
+      <c r="AM19" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AN19" s="296"/>
-      <c r="AO19" s="297" t="s">
+      <c r="AN19" s="299"/>
+      <c r="AO19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AP19" s="295"/>
-      <c r="AQ19" s="295" t="s">
+      <c r="AP19" s="296"/>
+      <c r="AQ19" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AR19" s="296"/>
-      <c r="AS19" s="297" t="s">
+      <c r="AR19" s="299"/>
+      <c r="AS19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AT19" s="295"/>
-      <c r="AU19" s="295" t="s">
+      <c r="AT19" s="296"/>
+      <c r="AU19" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AV19" s="296"/>
-      <c r="AW19" s="297" t="s">
+      <c r="AV19" s="299"/>
+      <c r="AW19" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AX19" s="295"/>
-      <c r="AY19" s="295" t="s">
+      <c r="AX19" s="296"/>
+      <c r="AY19" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AZ19" s="296"/>
+      <c r="AZ19" s="299"/>
       <c r="BA19" s="257">
         <f t="shared" si="0"/>
         <v>99385</v>
@@ -12497,94 +12497,94 @@
       <c r="H23" s="214">
         <v>0</v>
       </c>
-      <c r="I23" s="298" t="s">
+      <c r="I23" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="J23" s="299"/>
-      <c r="K23" s="300" t="s">
+      <c r="J23" s="309"/>
+      <c r="K23" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="L23" s="301"/>
-      <c r="M23" s="298" t="s">
+      <c r="L23" s="311"/>
+      <c r="M23" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="N23" s="299"/>
-      <c r="O23" s="300" t="s">
+      <c r="N23" s="309"/>
+      <c r="O23" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="P23" s="301"/>
-      <c r="Q23" s="298" t="s">
+      <c r="P23" s="311"/>
+      <c r="Q23" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="R23" s="299"/>
-      <c r="S23" s="300" t="s">
+      <c r="R23" s="309"/>
+      <c r="S23" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="T23" s="301"/>
-      <c r="U23" s="298" t="s">
+      <c r="T23" s="311"/>
+      <c r="U23" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="V23" s="299"/>
-      <c r="W23" s="300" t="s">
+      <c r="V23" s="309"/>
+      <c r="W23" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="X23" s="301"/>
-      <c r="Y23" s="298" t="s">
+      <c r="X23" s="311"/>
+      <c r="Y23" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="Z23" s="299"/>
-      <c r="AA23" s="300" t="s">
+      <c r="Z23" s="309"/>
+      <c r="AA23" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="AB23" s="301"/>
-      <c r="AC23" s="298" t="s">
+      <c r="AB23" s="311"/>
+      <c r="AC23" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="AD23" s="299"/>
-      <c r="AE23" s="300" t="s">
+      <c r="AD23" s="309"/>
+      <c r="AE23" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="AF23" s="301"/>
-      <c r="AG23" s="298" t="s">
+      <c r="AF23" s="311"/>
+      <c r="AG23" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="AH23" s="299"/>
-      <c r="AI23" s="300" t="s">
+      <c r="AH23" s="309"/>
+      <c r="AI23" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="AJ23" s="301"/>
-      <c r="AK23" s="298" t="s">
+      <c r="AJ23" s="311"/>
+      <c r="AK23" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="AL23" s="299"/>
-      <c r="AM23" s="300" t="s">
+      <c r="AL23" s="309"/>
+      <c r="AM23" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="AN23" s="301"/>
-      <c r="AO23" s="298" t="s">
+      <c r="AN23" s="311"/>
+      <c r="AO23" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="AP23" s="299"/>
-      <c r="AQ23" s="300" t="s">
+      <c r="AP23" s="309"/>
+      <c r="AQ23" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="AR23" s="301"/>
-      <c r="AS23" s="298" t="s">
+      <c r="AR23" s="311"/>
+      <c r="AS23" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="AT23" s="299"/>
-      <c r="AU23" s="300" t="s">
+      <c r="AT23" s="309"/>
+      <c r="AU23" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="AV23" s="301"/>
-      <c r="AW23" s="298" t="s">
+      <c r="AV23" s="311"/>
+      <c r="AW23" s="310" t="s">
         <v>233</v>
       </c>
-      <c r="AX23" s="299"/>
-      <c r="AY23" s="300" t="s">
+      <c r="AX23" s="309"/>
+      <c r="AY23" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="AZ23" s="301"/>
+      <c r="AZ23" s="311"/>
       <c r="BA23" s="257">
         <f t="shared" si="0"/>
         <v>163670.23000000001</v>
@@ -12841,54 +12841,54 @@
       <c r="AB25" s="209">
         <v>0</v>
       </c>
-      <c r="AC25" s="297" t="s">
+      <c r="AC25" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AD25" s="295"/>
-      <c r="AE25" s="295" t="s">
+      <c r="AD25" s="296"/>
+      <c r="AE25" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AF25" s="296"/>
-      <c r="AG25" s="297" t="s">
+      <c r="AF25" s="299"/>
+      <c r="AG25" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AH25" s="295"/>
-      <c r="AI25" s="295" t="s">
+      <c r="AH25" s="296"/>
+      <c r="AI25" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AJ25" s="296"/>
-      <c r="AK25" s="297" t="s">
+      <c r="AJ25" s="299"/>
+      <c r="AK25" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AL25" s="295"/>
-      <c r="AM25" s="295" t="s">
+      <c r="AL25" s="296"/>
+      <c r="AM25" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AN25" s="296"/>
-      <c r="AO25" s="297" t="s">
+      <c r="AN25" s="299"/>
+      <c r="AO25" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AP25" s="295"/>
-      <c r="AQ25" s="295" t="s">
+      <c r="AP25" s="296"/>
+      <c r="AQ25" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AR25" s="296"/>
-      <c r="AS25" s="297" t="s">
+      <c r="AR25" s="299"/>
+      <c r="AS25" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AT25" s="295"/>
-      <c r="AU25" s="295" t="s">
+      <c r="AT25" s="296"/>
+      <c r="AU25" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AV25" s="296"/>
-      <c r="AW25" s="297" t="s">
+      <c r="AV25" s="299"/>
+      <c r="AW25" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AX25" s="295"/>
-      <c r="AY25" s="295" t="s">
+      <c r="AX25" s="296"/>
+      <c r="AY25" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AZ25" s="296"/>
+      <c r="AZ25" s="299"/>
       <c r="BA25" s="257">
         <f t="shared" si="0"/>
         <v>90477.23</v>
@@ -12992,46 +12992,46 @@
       <c r="AF26" s="211">
         <v>0</v>
       </c>
-      <c r="AG26" s="297" t="s">
+      <c r="AG26" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AH26" s="295"/>
-      <c r="AI26" s="295" t="s">
+      <c r="AH26" s="296"/>
+      <c r="AI26" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AJ26" s="296"/>
-      <c r="AK26" s="297" t="s">
+      <c r="AJ26" s="299"/>
+      <c r="AK26" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AL26" s="295"/>
-      <c r="AM26" s="295" t="s">
+      <c r="AL26" s="296"/>
+      <c r="AM26" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AN26" s="296"/>
-      <c r="AO26" s="297" t="s">
+      <c r="AN26" s="299"/>
+      <c r="AO26" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AP26" s="295"/>
-      <c r="AQ26" s="295" t="s">
+      <c r="AP26" s="296"/>
+      <c r="AQ26" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AR26" s="296"/>
-      <c r="AS26" s="297" t="s">
+      <c r="AR26" s="299"/>
+      <c r="AS26" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AT26" s="295"/>
-      <c r="AU26" s="295" t="s">
+      <c r="AT26" s="296"/>
+      <c r="AU26" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AV26" s="296"/>
-      <c r="AW26" s="297" t="s">
+      <c r="AV26" s="299"/>
+      <c r="AW26" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AX26" s="295"/>
-      <c r="AY26" s="295" t="s">
+      <c r="AX26" s="296"/>
+      <c r="AY26" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AZ26" s="296"/>
+      <c r="AZ26" s="299"/>
       <c r="BA26" s="257">
         <f t="shared" si="0"/>
         <v>65199.1</v>
@@ -13500,22 +13500,22 @@
       <c r="AR29" s="209">
         <v>0</v>
       </c>
-      <c r="AS29" s="297" t="s">
+      <c r="AS29" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AT29" s="295"/>
-      <c r="AU29" s="295" t="s">
+      <c r="AT29" s="296"/>
+      <c r="AU29" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AV29" s="296"/>
-      <c r="AW29" s="297" t="s">
+      <c r="AV29" s="299"/>
+      <c r="AW29" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AX29" s="295"/>
-      <c r="AY29" s="295" t="s">
+      <c r="AX29" s="296"/>
+      <c r="AY29" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AZ29" s="296"/>
+      <c r="AZ29" s="299"/>
       <c r="BA29" s="257">
         <f t="shared" si="0"/>
         <v>518414.18</v>
@@ -13641,30 +13641,30 @@
         <v>44788.195919999998</v>
       </c>
       <c r="AN30" s="209"/>
-      <c r="AO30" s="297" t="s">
+      <c r="AO30" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AP30" s="295"/>
-      <c r="AQ30" s="295" t="s">
+      <c r="AP30" s="296"/>
+      <c r="AQ30" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AR30" s="296"/>
-      <c r="AS30" s="297" t="s">
+      <c r="AR30" s="299"/>
+      <c r="AS30" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AT30" s="295"/>
-      <c r="AU30" s="295" t="s">
+      <c r="AT30" s="296"/>
+      <c r="AU30" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AV30" s="296"/>
-      <c r="AW30" s="297" t="s">
+      <c r="AV30" s="299"/>
+      <c r="AW30" s="295" t="s">
         <v>233</v>
       </c>
-      <c r="AX30" s="295"/>
-      <c r="AY30" s="295" t="s">
+      <c r="AX30" s="296"/>
+      <c r="AY30" s="296" t="s">
         <v>233</v>
       </c>
-      <c r="AZ30" s="296"/>
+      <c r="AZ30" s="299"/>
       <c r="BA30" s="257">
         <f t="shared" si="0"/>
         <v>48341.279999999999</v>
@@ -14204,22 +14204,157 @@
     <sortCondition ref="A6:A16"/>
   </sortState>
   <mergeCells count="191">
-    <mergeCell ref="AC18:AD18"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="AG15:AH15"/>
-    <mergeCell ref="AI13:AJ13"/>
-    <mergeCell ref="AI14:AJ14"/>
-    <mergeCell ref="AI15:AJ15"/>
-    <mergeCell ref="AI19:AJ19"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="AG7:AH7"/>
-    <mergeCell ref="AG14:AH14"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="AG13:AH13"/>
-    <mergeCell ref="AG18:AH18"/>
+    <mergeCell ref="AM15:AN15"/>
+    <mergeCell ref="AO13:AP13"/>
+    <mergeCell ref="AQ13:AR13"/>
+    <mergeCell ref="AO14:AP14"/>
+    <mergeCell ref="AQ14:AR14"/>
+    <mergeCell ref="AO15:AP15"/>
+    <mergeCell ref="AQ15:AR15"/>
+    <mergeCell ref="AU14:AV14"/>
+    <mergeCell ref="AS15:AT15"/>
+    <mergeCell ref="AU15:AV15"/>
+    <mergeCell ref="AW13:AX13"/>
+    <mergeCell ref="AY13:AZ13"/>
+    <mergeCell ref="AW14:AX14"/>
+    <mergeCell ref="AY14:AZ14"/>
+    <mergeCell ref="AS18:AT18"/>
+    <mergeCell ref="AS19:AT19"/>
+    <mergeCell ref="AU18:AV18"/>
+    <mergeCell ref="AU19:AV19"/>
+    <mergeCell ref="AW18:AX18"/>
+    <mergeCell ref="AW19:AX19"/>
+    <mergeCell ref="AY18:AZ18"/>
+    <mergeCell ref="AY19:AZ19"/>
+    <mergeCell ref="AW15:AX15"/>
+    <mergeCell ref="AY15:AZ15"/>
+    <mergeCell ref="AS13:AT13"/>
+    <mergeCell ref="AU13:AV13"/>
+    <mergeCell ref="AS14:AT14"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="Y23:Z23"/>
+    <mergeCell ref="AS23:AT23"/>
+    <mergeCell ref="AU23:AV23"/>
+    <mergeCell ref="AY30:AZ30"/>
+    <mergeCell ref="AS25:AT25"/>
+    <mergeCell ref="AU25:AV25"/>
+    <mergeCell ref="AS26:AT26"/>
+    <mergeCell ref="AU26:AV26"/>
+    <mergeCell ref="AW25:AX25"/>
+    <mergeCell ref="AY25:AZ25"/>
+    <mergeCell ref="AW26:AX26"/>
+    <mergeCell ref="AY26:AZ26"/>
+    <mergeCell ref="AS29:AT29"/>
+    <mergeCell ref="AU29:AV29"/>
+    <mergeCell ref="AW29:AX29"/>
+    <mergeCell ref="AY29:AZ29"/>
+    <mergeCell ref="AW23:AX23"/>
+    <mergeCell ref="AY23:AZ23"/>
+    <mergeCell ref="AS10:AT10"/>
+    <mergeCell ref="AW10:AX10"/>
+    <mergeCell ref="AO7:AP7"/>
+    <mergeCell ref="AQ6:AR6"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="AO4:AR4"/>
+    <mergeCell ref="AO6:AP6"/>
+    <mergeCell ref="AS30:AT30"/>
+    <mergeCell ref="AU30:AV30"/>
+    <mergeCell ref="AW30:AX30"/>
+    <mergeCell ref="AS4:AV4"/>
+    <mergeCell ref="AS6:AT6"/>
+    <mergeCell ref="AU6:AV6"/>
+    <mergeCell ref="AS7:AT7"/>
+    <mergeCell ref="AU7:AV7"/>
+    <mergeCell ref="AS9:AT9"/>
+    <mergeCell ref="AU9:AV9"/>
+    <mergeCell ref="AW4:AZ4"/>
+    <mergeCell ref="AW6:AX6"/>
+    <mergeCell ref="AY6:AZ6"/>
+    <mergeCell ref="AW7:AX7"/>
+    <mergeCell ref="AY7:AZ7"/>
+    <mergeCell ref="AW9:AX9"/>
+    <mergeCell ref="AY9:AZ9"/>
+    <mergeCell ref="AO10:AP10"/>
+    <mergeCell ref="AO9:AP9"/>
+    <mergeCell ref="AQ9:AR9"/>
+    <mergeCell ref="AQ25:AR25"/>
+    <mergeCell ref="AM25:AN25"/>
+    <mergeCell ref="AO30:AP30"/>
+    <mergeCell ref="AQ30:AR30"/>
+    <mergeCell ref="AQ26:AR26"/>
+    <mergeCell ref="AK9:AL9"/>
+    <mergeCell ref="AM9:AN9"/>
+    <mergeCell ref="AM26:AN26"/>
+    <mergeCell ref="AK18:AL18"/>
+    <mergeCell ref="AK19:AL19"/>
+    <mergeCell ref="AM18:AN18"/>
+    <mergeCell ref="AM19:AN19"/>
+    <mergeCell ref="AO18:AP18"/>
+    <mergeCell ref="AO19:AP19"/>
+    <mergeCell ref="AQ18:AR18"/>
+    <mergeCell ref="AQ19:AR19"/>
+    <mergeCell ref="AK23:AL23"/>
+    <mergeCell ref="AM23:AN23"/>
+    <mergeCell ref="AO23:AP23"/>
+    <mergeCell ref="AQ23:AR23"/>
+    <mergeCell ref="AK13:AL13"/>
+    <mergeCell ref="E1:BA1"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="Y4:AB4"/>
+    <mergeCell ref="U4:X4"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="AG4:AJ4"/>
+    <mergeCell ref="AK4:AN4"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="AK7:AL7"/>
+    <mergeCell ref="AM6:AN6"/>
+    <mergeCell ref="AM7:AN7"/>
+    <mergeCell ref="AE23:AF23"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="AA13:AB13"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="AI7:AJ7"/>
+    <mergeCell ref="AI18:AJ18"/>
+    <mergeCell ref="AC13:AD13"/>
+    <mergeCell ref="AC14:AD14"/>
+    <mergeCell ref="AK10:AL10"/>
+    <mergeCell ref="AA23:AB23"/>
+    <mergeCell ref="AE13:AF13"/>
+    <mergeCell ref="AE14:AF14"/>
+    <mergeCell ref="AE15:AF15"/>
+    <mergeCell ref="AE18:AF18"/>
+    <mergeCell ref="AM13:AN13"/>
+    <mergeCell ref="AK14:AL14"/>
+    <mergeCell ref="AM14:AN14"/>
+    <mergeCell ref="AK15:AL15"/>
+    <mergeCell ref="AK25:AL25"/>
+    <mergeCell ref="AK26:AL26"/>
+    <mergeCell ref="AO25:AP25"/>
+    <mergeCell ref="AO26:AP26"/>
+    <mergeCell ref="AC19:AD19"/>
+    <mergeCell ref="AG23:AH23"/>
+    <mergeCell ref="AG19:AH19"/>
+    <mergeCell ref="AI23:AJ23"/>
+    <mergeCell ref="AC25:AD25"/>
+    <mergeCell ref="AE25:AF25"/>
+    <mergeCell ref="AG25:AH25"/>
+    <mergeCell ref="AG26:AH26"/>
+    <mergeCell ref="AI25:AJ25"/>
+    <mergeCell ref="AI26:AJ26"/>
+    <mergeCell ref="AC23:AD23"/>
+    <mergeCell ref="AE19:AF19"/>
     <mergeCell ref="S19:T19"/>
     <mergeCell ref="U19:V19"/>
     <mergeCell ref="W19:X19"/>
@@ -14244,157 +14379,22 @@
     <mergeCell ref="W18:X18"/>
     <mergeCell ref="Y18:Z18"/>
     <mergeCell ref="AA18:AB18"/>
-    <mergeCell ref="AK25:AL25"/>
-    <mergeCell ref="AK26:AL26"/>
-    <mergeCell ref="AO25:AP25"/>
-    <mergeCell ref="AO26:AP26"/>
-    <mergeCell ref="AC19:AD19"/>
-    <mergeCell ref="AG23:AH23"/>
-    <mergeCell ref="AG19:AH19"/>
-    <mergeCell ref="AI23:AJ23"/>
-    <mergeCell ref="AC25:AD25"/>
-    <mergeCell ref="AE25:AF25"/>
-    <mergeCell ref="AG25:AH25"/>
-    <mergeCell ref="AG26:AH26"/>
-    <mergeCell ref="AI25:AJ25"/>
-    <mergeCell ref="AI26:AJ26"/>
-    <mergeCell ref="AC23:AD23"/>
-    <mergeCell ref="AE19:AF19"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="AK7:AL7"/>
-    <mergeCell ref="AM6:AN6"/>
-    <mergeCell ref="AM7:AN7"/>
-    <mergeCell ref="AE23:AF23"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="AA13:AB13"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="AC15:AD15"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="AI7:AJ7"/>
-    <mergeCell ref="AI18:AJ18"/>
-    <mergeCell ref="AC13:AD13"/>
-    <mergeCell ref="AC14:AD14"/>
-    <mergeCell ref="AK10:AL10"/>
-    <mergeCell ref="AA23:AB23"/>
-    <mergeCell ref="AE13:AF13"/>
-    <mergeCell ref="AE14:AF14"/>
-    <mergeCell ref="AE15:AF15"/>
-    <mergeCell ref="AE18:AF18"/>
-    <mergeCell ref="AM13:AN13"/>
-    <mergeCell ref="AK14:AL14"/>
-    <mergeCell ref="AM14:AN14"/>
-    <mergeCell ref="AK15:AL15"/>
-    <mergeCell ref="E1:BA1"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="Y4:AB4"/>
-    <mergeCell ref="U4:X4"/>
-    <mergeCell ref="AC4:AF4"/>
-    <mergeCell ref="AG4:AJ4"/>
-    <mergeCell ref="AK4:AN4"/>
-    <mergeCell ref="AO10:AP10"/>
-    <mergeCell ref="AO9:AP9"/>
-    <mergeCell ref="AQ9:AR9"/>
-    <mergeCell ref="AQ25:AR25"/>
-    <mergeCell ref="AM25:AN25"/>
-    <mergeCell ref="AO30:AP30"/>
-    <mergeCell ref="AQ30:AR30"/>
-    <mergeCell ref="AQ26:AR26"/>
-    <mergeCell ref="AK9:AL9"/>
-    <mergeCell ref="AM9:AN9"/>
-    <mergeCell ref="AM26:AN26"/>
-    <mergeCell ref="AK18:AL18"/>
-    <mergeCell ref="AK19:AL19"/>
-    <mergeCell ref="AM18:AN18"/>
-    <mergeCell ref="AM19:AN19"/>
-    <mergeCell ref="AO18:AP18"/>
-    <mergeCell ref="AO19:AP19"/>
-    <mergeCell ref="AQ18:AR18"/>
-    <mergeCell ref="AQ19:AR19"/>
-    <mergeCell ref="AK23:AL23"/>
-    <mergeCell ref="AM23:AN23"/>
-    <mergeCell ref="AO23:AP23"/>
-    <mergeCell ref="AQ23:AR23"/>
-    <mergeCell ref="AK13:AL13"/>
-    <mergeCell ref="AS10:AT10"/>
-    <mergeCell ref="AW10:AX10"/>
-    <mergeCell ref="AO7:AP7"/>
-    <mergeCell ref="AQ6:AR6"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="AO4:AR4"/>
-    <mergeCell ref="AO6:AP6"/>
-    <mergeCell ref="AS30:AT30"/>
-    <mergeCell ref="AU30:AV30"/>
-    <mergeCell ref="AW30:AX30"/>
-    <mergeCell ref="AS4:AV4"/>
-    <mergeCell ref="AS6:AT6"/>
-    <mergeCell ref="AU6:AV6"/>
-    <mergeCell ref="AS7:AT7"/>
-    <mergeCell ref="AU7:AV7"/>
-    <mergeCell ref="AS9:AT9"/>
-    <mergeCell ref="AU9:AV9"/>
-    <mergeCell ref="AW4:AZ4"/>
-    <mergeCell ref="AW6:AX6"/>
-    <mergeCell ref="AY6:AZ6"/>
-    <mergeCell ref="AW7:AX7"/>
-    <mergeCell ref="AY7:AZ7"/>
-    <mergeCell ref="AW9:AX9"/>
-    <mergeCell ref="AY9:AZ9"/>
-    <mergeCell ref="AS23:AT23"/>
-    <mergeCell ref="AU23:AV23"/>
-    <mergeCell ref="AY30:AZ30"/>
-    <mergeCell ref="AS25:AT25"/>
-    <mergeCell ref="AU25:AV25"/>
-    <mergeCell ref="AS26:AT26"/>
-    <mergeCell ref="AU26:AV26"/>
-    <mergeCell ref="AW25:AX25"/>
-    <mergeCell ref="AY25:AZ25"/>
-    <mergeCell ref="AW26:AX26"/>
-    <mergeCell ref="AY26:AZ26"/>
-    <mergeCell ref="AS29:AT29"/>
-    <mergeCell ref="AU29:AV29"/>
-    <mergeCell ref="AW29:AX29"/>
-    <mergeCell ref="AY29:AZ29"/>
-    <mergeCell ref="AW23:AX23"/>
-    <mergeCell ref="AY23:AZ23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="Y23:Z23"/>
-    <mergeCell ref="AW13:AX13"/>
-    <mergeCell ref="AY13:AZ13"/>
-    <mergeCell ref="AW14:AX14"/>
-    <mergeCell ref="AY14:AZ14"/>
-    <mergeCell ref="AS18:AT18"/>
-    <mergeCell ref="AS19:AT19"/>
-    <mergeCell ref="AU18:AV18"/>
-    <mergeCell ref="AU19:AV19"/>
-    <mergeCell ref="AW18:AX18"/>
-    <mergeCell ref="AW19:AX19"/>
-    <mergeCell ref="AY18:AZ18"/>
-    <mergeCell ref="AY19:AZ19"/>
-    <mergeCell ref="AW15:AX15"/>
-    <mergeCell ref="AY15:AZ15"/>
-    <mergeCell ref="AS13:AT13"/>
-    <mergeCell ref="AU13:AV13"/>
-    <mergeCell ref="AS14:AT14"/>
-    <mergeCell ref="AM15:AN15"/>
-    <mergeCell ref="AO13:AP13"/>
-    <mergeCell ref="AQ13:AR13"/>
-    <mergeCell ref="AO14:AP14"/>
-    <mergeCell ref="AQ14:AR14"/>
-    <mergeCell ref="AO15:AP15"/>
-    <mergeCell ref="AQ15:AR15"/>
-    <mergeCell ref="AU14:AV14"/>
-    <mergeCell ref="AS15:AT15"/>
-    <mergeCell ref="AU15:AV15"/>
+    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="AG15:AH15"/>
+    <mergeCell ref="AI13:AJ13"/>
+    <mergeCell ref="AI14:AJ14"/>
+    <mergeCell ref="AI15:AJ15"/>
+    <mergeCell ref="AI19:AJ19"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="AG7:AH7"/>
+    <mergeCell ref="AG14:AH14"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="AG13:AH13"/>
+    <mergeCell ref="AG18:AH18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -16344,17 +16344,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="C49:G49"/>
     <mergeCell ref="C50:G50"/>
     <mergeCell ref="C52:G52"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="C21:G21"/>
     <mergeCell ref="C23:G23"/>
     <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C49:G49"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -17937,93 +17937,93 @@
       <c r="AD3" s="201"/>
     </row>
     <row r="4" spans="1:56 16377:16378" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A4" s="313" t="s">
+      <c r="A4" s="303" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="315" t="s">
+      <c r="B4" s="305" t="s">
         <v>234</v>
       </c>
-      <c r="C4" s="315" t="s">
+      <c r="C4" s="305" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="317" t="s">
+      <c r="D4" s="307" t="s">
         <v>236</v>
       </c>
-      <c r="E4" s="315" t="s">
+      <c r="E4" s="305" t="s">
         <v>310</v>
       </c>
-      <c r="F4" s="309" t="s">
+      <c r="F4" s="317" t="s">
         <v>250</v>
       </c>
-      <c r="G4" s="306"/>
-      <c r="H4" s="306"/>
-      <c r="I4" s="307"/>
-      <c r="J4" s="306" t="s">
+      <c r="G4" s="316"/>
+      <c r="H4" s="316"/>
+      <c r="I4" s="318"/>
+      <c r="J4" s="316" t="s">
         <v>249</v>
       </c>
-      <c r="K4" s="306"/>
-      <c r="L4" s="306"/>
-      <c r="M4" s="306"/>
-      <c r="N4" s="309" t="s">
+      <c r="K4" s="316"/>
+      <c r="L4" s="316"/>
+      <c r="M4" s="316"/>
+      <c r="N4" s="317" t="s">
         <v>251</v>
       </c>
-      <c r="O4" s="306"/>
-      <c r="P4" s="306"/>
-      <c r="Q4" s="307"/>
-      <c r="R4" s="309" t="s">
+      <c r="O4" s="316"/>
+      <c r="P4" s="316"/>
+      <c r="Q4" s="318"/>
+      <c r="R4" s="317" t="s">
         <v>256</v>
       </c>
-      <c r="S4" s="306"/>
-      <c r="T4" s="306"/>
-      <c r="U4" s="307"/>
-      <c r="V4" s="306" t="s">
+      <c r="S4" s="316"/>
+      <c r="T4" s="316"/>
+      <c r="U4" s="318"/>
+      <c r="V4" s="316" t="s">
         <v>257</v>
       </c>
-      <c r="W4" s="306"/>
-      <c r="X4" s="306"/>
-      <c r="Y4" s="306"/>
-      <c r="Z4" s="309" t="s">
+      <c r="W4" s="316"/>
+      <c r="X4" s="316"/>
+      <c r="Y4" s="316"/>
+      <c r="Z4" s="317" t="s">
         <v>258</v>
       </c>
-      <c r="AA4" s="306"/>
-      <c r="AB4" s="306"/>
-      <c r="AC4" s="307"/>
-      <c r="AD4" s="309" t="s">
+      <c r="AA4" s="316"/>
+      <c r="AB4" s="316"/>
+      <c r="AC4" s="318"/>
+      <c r="AD4" s="317" t="s">
         <v>260</v>
       </c>
-      <c r="AE4" s="306"/>
-      <c r="AF4" s="306"/>
-      <c r="AG4" s="307"/>
-      <c r="AH4" s="309" t="s">
+      <c r="AE4" s="316"/>
+      <c r="AF4" s="316"/>
+      <c r="AG4" s="318"/>
+      <c r="AH4" s="317" t="s">
         <v>261</v>
       </c>
-      <c r="AI4" s="306"/>
-      <c r="AJ4" s="306"/>
-      <c r="AK4" s="307"/>
-      <c r="AL4" s="309" t="s">
+      <c r="AI4" s="316"/>
+      <c r="AJ4" s="316"/>
+      <c r="AK4" s="318"/>
+      <c r="AL4" s="317" t="s">
         <v>237</v>
       </c>
-      <c r="AM4" s="306"/>
-      <c r="AN4" s="306"/>
-      <c r="AO4" s="307"/>
-      <c r="AP4" s="306" t="s">
+      <c r="AM4" s="316"/>
+      <c r="AN4" s="316"/>
+      <c r="AO4" s="318"/>
+      <c r="AP4" s="316" t="s">
         <v>238</v>
       </c>
-      <c r="AQ4" s="306"/>
-      <c r="AR4" s="306"/>
-      <c r="AS4" s="307"/>
-      <c r="AT4" s="309" t="s">
+      <c r="AQ4" s="316"/>
+      <c r="AR4" s="316"/>
+      <c r="AS4" s="318"/>
+      <c r="AT4" s="317" t="s">
         <v>239</v>
       </c>
-      <c r="AU4" s="306"/>
-      <c r="AV4" s="306"/>
-      <c r="AW4" s="307"/>
-      <c r="AX4" s="309" t="s">
+      <c r="AU4" s="316"/>
+      <c r="AV4" s="316"/>
+      <c r="AW4" s="318"/>
+      <c r="AX4" s="317" t="s">
         <v>240</v>
       </c>
-      <c r="AY4" s="306"/>
-      <c r="AZ4" s="306"/>
-      <c r="BA4" s="307"/>
+      <c r="AY4" s="316"/>
+      <c r="AZ4" s="316"/>
+      <c r="BA4" s="318"/>
       <c r="BB4" s="220" t="s">
         <v>307</v>
       </c>
@@ -18035,11 +18035,11 @@
       </c>
     </row>
     <row r="5" spans="1:56 16377:16378" s="145" customFormat="1" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A5" s="314"/>
-      <c r="B5" s="316"/>
-      <c r="C5" s="316"/>
-      <c r="D5" s="318"/>
-      <c r="E5" s="316"/>
+      <c r="A5" s="304"/>
+      <c r="B5" s="306"/>
+      <c r="C5" s="306"/>
+      <c r="D5" s="308"/>
+      <c r="E5" s="306"/>
       <c r="F5" s="172" t="s">
         <v>246</v>
       </c>
@@ -20661,11 +20661,15 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="AX9:BA9"/>
-    <mergeCell ref="AH9:AK9"/>
-    <mergeCell ref="AL9:AO9"/>
-    <mergeCell ref="AP9:AS9"/>
-    <mergeCell ref="AT9:AW9"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="AT4:AW4"/>
+    <mergeCell ref="AX4:BA4"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="Z4:AC4"/>
+    <mergeCell ref="AL4:AO4"/>
+    <mergeCell ref="AP4:AS4"/>
+    <mergeCell ref="AH4:AK4"/>
     <mergeCell ref="J9:M9"/>
     <mergeCell ref="N9:Q9"/>
     <mergeCell ref="A4:A5"/>
@@ -20676,15 +20680,11 @@
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="AD4:AG4"/>
-    <mergeCell ref="AT4:AW4"/>
-    <mergeCell ref="AX4:BA4"/>
-    <mergeCell ref="V4:Y4"/>
-    <mergeCell ref="Z4:AC4"/>
-    <mergeCell ref="AL4:AO4"/>
-    <mergeCell ref="AP4:AS4"/>
-    <mergeCell ref="AH4:AK4"/>
+    <mergeCell ref="AX9:BA9"/>
+    <mergeCell ref="AH9:AK9"/>
+    <mergeCell ref="AL9:AO9"/>
+    <mergeCell ref="AP9:AS9"/>
+    <mergeCell ref="AT9:AW9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -20702,8 +20702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C60C3C0C-3E40-486A-9B59-1C5056167637}">
   <dimension ref="A1:G288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="I220" sqref="I220"/>
+    <sheetView topLeftCell="A170" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -27351,8 +27351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF7C2BA-F766-47EF-8569-EB2756BF213B}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -27394,7 +27394,9 @@
       <c r="D2" s="283" t="s">
         <v>202</v>
       </c>
-      <c r="E2" s="290"/>
+      <c r="E2" s="290">
+        <v>20474999.59</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="283">
@@ -27409,7 +27411,9 @@
       <c r="D3" s="283" t="s">
         <v>306</v>
       </c>
-      <c r="E3" s="290"/>
+      <c r="E3" s="290">
+        <v>2245350.35</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="283">
@@ -27424,7 +27428,9 @@
       <c r="D4" s="283" t="s">
         <v>204</v>
       </c>
-      <c r="E4" s="290"/>
+      <c r="E4" s="290">
+        <v>15800000</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="283">
@@ -27471,7 +27477,9 @@
       <c r="D7" s="283" t="s">
         <v>225</v>
       </c>
-      <c r="E7" s="290"/>
+      <c r="E7" s="290">
+        <v>4530000</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="283">
@@ -27503,7 +27511,9 @@
       <c r="D9" s="283" t="s">
         <v>231</v>
       </c>
-      <c r="E9" s="290"/>
+      <c r="E9" s="290">
+        <v>15049967.470000001</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="283">
@@ -27518,7 +27528,9 @@
       <c r="D10" s="283" t="s">
         <v>231</v>
       </c>
-      <c r="E10" s="290"/>
+      <c r="E10" s="290">
+        <v>15049967.470000001</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="283">
@@ -27652,7 +27664,9 @@
       <c r="D18" s="283" t="s">
         <v>306</v>
       </c>
-      <c r="E18" s="290"/>
+      <c r="E18" s="290">
+        <v>279614</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="283">
@@ -27667,7 +27681,9 @@
       <c r="D19" s="283" t="s">
         <v>304</v>
       </c>
-      <c r="E19" s="290"/>
+      <c r="E19" s="290">
+        <v>492915.39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Atualização 07/08/25 - 43
</commit_message>
<xml_diff>
--- a/1 - Acompanhamento Medições.xlsx
+++ b/1 - Acompanhamento Medições.xlsx
@@ -20702,8 +20702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C60C3C0C-3E40-486A-9B59-1C5056167637}">
   <dimension ref="A1:G288"/>
   <sheetViews>
-    <sheetView topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="B187" sqref="B187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -27352,7 +27352,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>